<commit_message>
fix: end of day backup
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BAFE6D-C591-46E3-906A-BC363D2C5E72}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF3ED65-CB4E-426C-B362-227FEB539EB9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="91">
   <si>
     <t>Page</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Train</t>
   </si>
   <si>
-    <t>After branch is saved the original branch should retain all of its original training</t>
-  </si>
-  <si>
     <t>Attempts to branch above training errors should succeed</t>
   </si>
   <si>
@@ -295,6 +292,18 @@
   </si>
   <si>
     <t>Not selecting a turn and no special buttons show up</t>
+  </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>"Close" and "Delete" buttons should change to "Save Branch" and "Abandon Branch" after branching</t>
+  </si>
+  <si>
+    <t>After branch is saved the original training should remain unchanged</t>
+  </si>
+  <si>
+    <t>After branch is abandonded the original training should remain unchanged</t>
   </si>
 </sst>
 </file>
@@ -379,8 +388,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F57" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F57" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F59" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F59" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -690,11 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24:C36"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +734,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1086,7 +1095,7 @@
         <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1100,7 +1109,7 @@
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1114,7 +1123,7 @@
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1128,7 +1137,7 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1142,7 +1151,7 @@
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1156,7 +1165,10 @@
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>89</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1170,7 +1182,10 @@
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1184,10 +1199,7 @@
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1201,7 +1213,7 @@
         <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1215,7 +1227,10 @@
         <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="F35" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1229,35 +1244,35 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" t="s">
-        <v>39</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1268,10 +1283,10 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1282,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
         <v>39</v>
@@ -1296,10 +1311,10 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1310,9 +1325,23 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1321,27 +1350,13 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1352,10 +1367,10 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1366,7 +1381,7 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
         <v>39</v>
@@ -1380,10 +1395,10 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1394,21 +1409,39 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>3</v>
       </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
@@ -1427,6 +1460,16 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: test case log.whatsyourname
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BAFE6D-C591-46E3-906A-BC363D2C5E72}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAA18B5-0905-4B30-A17E-C657C51C3536}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="91">
   <si>
     <t>Page</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Train</t>
   </si>
   <si>
-    <t>After branch is saved the original branch should retain all of its original training</t>
-  </si>
-  <si>
     <t>Attempts to branch above training errors should succeed</t>
   </si>
   <si>
@@ -295,6 +292,18 @@
   </si>
   <si>
     <t>Not selecting a turn and no special buttons show up</t>
+  </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>"Close" and "Delete" buttons should change to "Save Branch" and "Abandon Branch" after branching</t>
+  </si>
+  <si>
+    <t>After branch is saved the original training should remain unchanged</t>
+  </si>
+  <si>
+    <t>After branch is abandonded the original training should remain unchanged</t>
   </si>
 </sst>
 </file>
@@ -379,8 +388,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F57" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F57" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F59" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F59" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -690,11 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24:C36"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +734,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1086,7 +1095,7 @@
         <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1100,7 +1109,7 @@
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1114,7 +1123,7 @@
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1128,7 +1137,7 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1142,7 +1151,7 @@
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1156,7 +1165,10 @@
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>89</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1170,7 +1182,10 @@
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1184,10 +1199,7 @@
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1201,7 +1213,7 @@
         <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1215,7 +1227,10 @@
         <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="F35" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1229,35 +1244,35 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" t="s">
-        <v>39</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1268,10 +1283,10 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1282,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
         <v>39</v>
@@ -1296,10 +1311,10 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1310,9 +1325,23 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1321,27 +1350,13 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1352,10 +1367,10 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1366,7 +1381,7 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
         <v>39</v>
@@ -1380,10 +1395,10 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1394,21 +1409,39 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>3</v>
       </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
@@ -1427,6 +1460,16 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: test case log.whatsyourname (#784)
Test case Log What's Your Name was broken. This fixes it.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BAFE6D-C591-46E3-906A-BC363D2C5E72}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAA18B5-0905-4B30-A17E-C657C51C3536}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="91">
   <si>
     <t>Page</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Train</t>
   </si>
   <si>
-    <t>After branch is saved the original branch should retain all of its original training</t>
-  </si>
-  <si>
     <t>Attempts to branch above training errors should succeed</t>
   </si>
   <si>
@@ -295,6 +292,18 @@
   </si>
   <si>
     <t>Not selecting a turn and no special buttons show up</t>
+  </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>"Close" and "Delete" buttons should change to "Save Branch" and "Abandon Branch" after branching</t>
+  </si>
+  <si>
+    <t>After branch is saved the original training should remain unchanged</t>
+  </si>
+  <si>
+    <t>After branch is abandonded the original training should remain unchanged</t>
   </si>
 </sst>
 </file>
@@ -379,8 +388,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F57" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F57" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F59" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F59" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -690,11 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24:C36"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +734,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1086,7 +1095,7 @@
         <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1100,7 +1109,7 @@
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1114,7 +1123,7 @@
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1128,7 +1137,7 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1142,7 +1151,7 @@
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1156,7 +1165,10 @@
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>89</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1170,7 +1182,10 @@
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1184,10 +1199,7 @@
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1201,7 +1213,7 @@
         <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1215,7 +1227,10 @@
         <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="F35" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1229,35 +1244,35 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" t="s">
-        <v>39</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1268,10 +1283,10 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1282,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
         <v>39</v>
@@ -1296,10 +1311,10 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1310,9 +1325,23 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1321,27 +1350,13 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1352,10 +1367,10 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1366,7 +1381,7 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
         <v>39</v>
@@ -1380,10 +1395,10 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1394,21 +1409,39 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>3</v>
       </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
@@ -1427,6 +1460,16 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: first test case complete
VerifyEditTrainingControlsAndLabels test case is complete and working
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBC6093-8116-463B-8EEA-54CBF45EC93E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F163E0AC-0261-4CB6-ABF6-839E9BE807F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="95">
   <si>
     <t>Page</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Branching</t>
   </si>
   <si>
-    <t>User turn should show branch icon, Bot turn should not.</t>
-  </si>
-  <si>
     <t>Buttons should remain "Close" and "Delete" as long as nothing changes</t>
   </si>
   <si>
@@ -318,7 +315,7 @@
     <t>Add score and add input buttons show for all turns</t>
   </si>
   <si>
-    <t>no test yet, but SelectAndValidateEachChatTurn is working via zTemp</t>
+    <t>VerifyChatEditControls</t>
   </si>
 </sst>
 </file>
@@ -403,8 +400,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F64" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F64" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F63" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F63" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -714,11 +711,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1073,77 +1070,75 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>84</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>91</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>93</v>
+      </c>
+      <c r="E26" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" t="s">
-        <v>74</v>
+        <v>92</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
         <v>71</v>
@@ -1152,12 +1147,12 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
         <v>71</v>
@@ -1166,12 +1161,12 @@
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
         <v>71</v>
@@ -1180,15 +1175,12 @@
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
-      </c>
-      <c r="E31" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>71</v>
@@ -1197,15 +1189,12 @@
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
-      </c>
-      <c r="E32" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
         <v>71</v>
@@ -1214,12 +1203,12 @@
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" t="s">
         <v>71</v>
@@ -1228,12 +1217,12 @@
         <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
         <v>71</v>
@@ -1242,15 +1231,15 @@
         <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
-      </c>
-      <c r="F35" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="E35" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
         <v>71</v>
@@ -1259,12 +1248,15 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>89</v>
+      </c>
+      <c r="E36" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
         <v>71</v>
@@ -1273,12 +1265,12 @@
         <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
         <v>71</v>
@@ -1287,75 +1279,80 @@
         <v>20</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
         <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>85</v>
-      </c>
-      <c r="E40" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
         <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
         <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
-      </c>
-      <c r="E42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" t="s">
-        <v>94</v>
-      </c>
-      <c r="E43" t="s">
-        <v>95</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1366,10 +1363,10 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1380,10 +1377,10 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1397,7 +1394,7 @@
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1408,10 +1405,10 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1422,24 +1419,24 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D50" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" t="s">
-        <v>42</v>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1450,10 +1447,10 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1464,10 +1461,10 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1481,7 +1478,7 @@
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1492,10 +1489,10 @@
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1506,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D57" t="s">
         <v>43</v>
@@ -1516,15 +1513,6 @@
       <c r="A58" t="s">
         <v>3</v>
       </c>
-      <c r="B58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -1548,11 +1536,6 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: added one more verification to new branching test
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F163E0AC-0261-4CB6-ABF6-839E9BE807F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638F5502-0542-4819-845E-F65B12C41A2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="95">
   <si>
     <t>Page</t>
   </si>
@@ -315,7 +315,7 @@
     <t>Add score and add input buttons show for all turns</t>
   </si>
   <si>
-    <t>VerifyChatEditControls</t>
+    <t>VerifyEditTrainingControlsAndLabels</t>
   </si>
 </sst>
 </file>
@@ -369,16 +369,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thick">
@@ -400,13 +409,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F63" totalsRowShown="0" headerRowBorderDxfId="0" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F63" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F64" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F64" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
     <tableColumn id="2" xr3:uid="{B0123158-48C7-47B5-8788-3102666127B5}" name="Page"/>
-    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations"/>
+    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name"/>
     <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes"/>
   </tableColumns>
@@ -711,18 +720,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="112.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="60.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.77734375" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" customWidth="1"/>
@@ -739,7 +748,7 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -759,7 +768,7 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -773,7 +782,7 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -787,7 +796,7 @@
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
@@ -804,7 +813,7 @@
       <c r="C5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E5" t="s">
@@ -821,7 +830,7 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
@@ -838,7 +847,7 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -852,7 +861,7 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -866,7 +875,7 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -880,7 +889,7 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E10" t="s">
@@ -897,7 +906,7 @@
       <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E11" t="s">
@@ -914,7 +923,7 @@
       <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E12" t="s">
@@ -931,7 +940,7 @@
       <c r="C14" t="s">
         <v>53</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E14" t="s">
@@ -948,14 +957,14 @@
       <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -965,14 +974,14 @@
       <c r="C16" t="s">
         <v>53</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -982,7 +991,7 @@
       <c r="C17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E17" t="s">
@@ -999,7 +1008,7 @@
       <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="4" t="s">
         <v>61</v>
       </c>
       <c r="E18" t="s">
@@ -1016,14 +1025,14 @@
       <c r="C19" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1033,7 +1042,7 @@
       <c r="C20" t="s">
         <v>53</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E20" t="s">
@@ -1050,7 +1059,7 @@
       <c r="C21" t="s">
         <v>53</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E21" t="s">
@@ -1064,7 +1073,7 @@
       <c r="C22" t="s">
         <v>20</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1078,7 +1087,7 @@
       <c r="C24" t="s">
         <v>20</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
         <v>84</v>
       </c>
       <c r="E24" t="s">
@@ -1095,7 +1104,7 @@
       <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E25" t="s">
@@ -1112,7 +1121,7 @@
       <c r="C26" t="s">
         <v>20</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E26" t="s">
@@ -1129,25 +1138,28 @@
       <c r="C27" t="s">
         <v>20</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E27" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" t="s">
-        <v>72</v>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1160,11 +1172,14 @@
       <c r="C30" t="s">
         <v>20</v>
       </c>
-      <c r="D30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -1174,11 +1189,14 @@
       <c r="C31" t="s">
         <v>20</v>
       </c>
-      <c r="D31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -1188,11 +1206,11 @@
       <c r="C32" t="s">
         <v>20</v>
       </c>
-      <c r="D32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D32" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -1202,11 +1220,11 @@
       <c r="C33" t="s">
         <v>20</v>
       </c>
-      <c r="D33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D33" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -1216,8 +1234,8 @@
       <c r="C34" t="s">
         <v>20</v>
       </c>
-      <c r="D34" t="s">
-        <v>77</v>
+      <c r="D34" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1230,11 +1248,8 @@
       <c r="C35" t="s">
         <v>20</v>
       </c>
-      <c r="D35" t="s">
-        <v>88</v>
-      </c>
-      <c r="E35" t="s">
-        <v>86</v>
+      <c r="D35" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1247,8 +1262,8 @@
       <c r="C36" t="s">
         <v>20</v>
       </c>
-      <c r="D36" t="s">
-        <v>89</v>
+      <c r="D36" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="E36" t="s">
         <v>86</v>
@@ -1264,8 +1279,11 @@
       <c r="C37" t="s">
         <v>20</v>
       </c>
-      <c r="D37" t="s">
-        <v>74</v>
+      <c r="D37" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1278,11 +1296,11 @@
       <c r="C38" t="s">
         <v>20</v>
       </c>
-      <c r="D38" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D38" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -1292,11 +1310,8 @@
       <c r="C39" t="s">
         <v>20</v>
       </c>
-      <c r="D39" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" t="s">
-        <v>83</v>
+      <c r="D39" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1309,8 +1324,11 @@
       <c r="C40" t="s">
         <v>20</v>
       </c>
-      <c r="D40" t="s">
-        <v>81</v>
+      <c r="D40" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1323,36 +1341,8 @@
       <c r="C41" t="s">
         <v>20</v>
       </c>
-      <c r="D41" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" t="s">
-        <v>38</v>
+      <c r="D41" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1363,10 +1353,10 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" t="s">
-        <v>39</v>
+        <v>46</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1377,10 +1367,10 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>40</v>
+        <v>12</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1393,8 +1383,8 @@
       <c r="C48" t="s">
         <v>8</v>
       </c>
-      <c r="D48" t="s">
-        <v>39</v>
+      <c r="D48" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1405,10 +1395,10 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1419,24 +1409,24 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
         <v>11</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" s="4" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1447,10 +1437,10 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" t="s">
-        <v>39</v>
+        <v>46</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1461,10 +1451,10 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" t="s">
-        <v>41</v>
+        <v>12</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1477,8 +1467,8 @@
       <c r="C55" t="s">
         <v>8</v>
       </c>
-      <c r="D55" t="s">
-        <v>39</v>
+      <c r="D55" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1489,10 +1479,10 @@
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" t="s">
-        <v>43</v>
+        <v>8</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1503,9 +1493,9 @@
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1513,6 +1503,15 @@
       <c r="A58" t="s">
         <v>3</v>
       </c>
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -1536,6 +1535,11 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: new verification added
After branch is saved the original training should remain unchanged
         ...and...
After branch is abandonded the original training should remain unchanged
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638F5502-0542-4819-845E-F65B12C41A2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA50F113-5ED4-415E-B0C2-94326BD768C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="95">
   <si>
     <t>Page</t>
   </si>
@@ -724,7 +724,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1299,6 +1299,9 @@
       <c r="D38" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="E38" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">

</xml_diff>

<commit_message>
fix: replaced some cy.commands with cy.enquque
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA50F113-5ED4-415E-B0C2-94326BD768C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0510A268-2AB5-4481-ACC4-0ED2F9A0FA5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -724,7 +724,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,7 +1283,7 @@
         <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: first branching test is nearly ready to try
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9321925-A82E-40EC-B1C8-75F98D214791}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3602747-D140-4328-B834-846E8D9E3F1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="97">
   <si>
     <t>Page</t>
   </si>
@@ -319,13 +319,16 @@
   </si>
   <si>
     <t>After new branch has been created, all edit controls in the chat pane should disappear</t>
+  </si>
+  <si>
+    <t>TODO: Branching + Edit how do they mix? Edit first does not allow branching.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,13 +344,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -372,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
@@ -380,6 +396,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -726,8 +745,8 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,6 +1384,20 @@
         <v>81</v>
       </c>
     </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
feat: updated grid with newly working test
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316B360D-A824-4A6D-A4C4-8BC5E3E4EB04}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388BAC73-7966-4E4A-91FC-E8DF61957832}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="96">
   <si>
     <t>Page</t>
   </si>
@@ -289,9 +289,6 @@
   </si>
   <si>
     <t>Not selecting a turn and no special buttons show up</t>
-  </si>
-  <si>
-    <t>manual</t>
   </si>
   <si>
     <t>"Close" and "Delete" buttons should change to "Save Branch" and "Abandon Branch" after branching</t>
@@ -744,9 +741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,7 +1101,7 @@
         <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
@@ -1113,7 +1110,7 @@
         <v>84</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1121,16 +1118,16 @@
         <v>79</v>
       </c>
       <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1138,16 +1135,16 @@
         <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
         <v>93</v>
-      </c>
-      <c r="E26" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1155,16 +1152,16 @@
         <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1172,7 +1169,7 @@
         <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
@@ -1181,7 +1178,7 @@
         <v>85</v>
       </c>
       <c r="E28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1198,7 +1195,7 @@
         <v>72</v>
       </c>
       <c r="E30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1212,10 +1209,10 @@
         <v>20</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1231,6 +1228,9 @@
       <c r="D32" s="4" t="s">
         <v>76</v>
       </c>
+      <c r="E32" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -1245,6 +1245,9 @@
       <c r="D33" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="E33" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -1257,7 +1260,10 @@
         <v>20</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="E34" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1287,6 +1293,9 @@
       <c r="D36" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="E36" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -1299,10 +1308,10 @@
         <v>20</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E37" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1316,10 +1325,10 @@
         <v>20</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1336,7 +1345,7 @@
         <v>74</v>
       </c>
       <c r="E39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1395,7 +1404,7 @@
         <v>20</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Tag and Frog and Fixes to Broken Tests (#856)
This is a start to the Tag and Frog scenario by creating the preliminary model necessary for the main test.
Also fixed a couple of bugs in test code:
The new time values in the grid broke tests that validated the dates that had been there.
There were two Refresh "Training Status" buttons on the page when Train Dialog modal is up. Cypress threw an error when trying to click on two buttons. Fixed it so it clicks on the last button.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388BAC73-7966-4E4A-91FC-E8DF61957832}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9A082E-45C9-48E4-80C7-BF2C977E7D25}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="99">
   <si>
     <t>Page</t>
   </si>
@@ -319,6 +319,15 @@
   </si>
   <si>
     <t>TODO: Branching + Edit how do they mix? Edit first does not allow branching.</t>
+  </si>
+  <si>
+    <t>Label Entities</t>
+  </si>
+  <si>
+    <t>Selecting a user turn causes "Entity Detection" UI Elements to show up</t>
+  </si>
+  <si>
+    <t>Selecting a Bot turn causes Action Selection UI Elements to show up</t>
   </si>
 </sst>
 </file>
@@ -428,8 +437,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F65" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F65" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F68" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F68" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -739,11 +748,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1181,89 +1190,66 @@
         <v>93</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="4" t="s">
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E34" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1277,10 +1263,13 @@
         <v>20</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="E35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -1291,7 +1280,7 @@
         <v>20</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E36" t="s">
         <v>71</v>
@@ -1308,13 +1297,13 @@
         <v>20</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -1325,10 +1314,7 @@
         <v>20</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E38" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1342,13 +1328,13 @@
         <v>20</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1359,7 +1345,10 @@
         <v>20</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>75</v>
+        <v>87</v>
+      </c>
+      <c r="E40" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1373,10 +1362,10 @@
         <v>20</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F41" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="E41" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1390,63 +1379,80 @@
         <v>20</v>
       </c>
       <c r="D42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="5" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" t="s">
-        <v>46</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1457,10 +1463,10 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1471,10 +1477,10 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1485,10 +1491,24 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1496,13 +1516,13 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1510,27 +1530,13 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>3</v>
-      </c>
-      <c r="B56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1541,10 +1547,10 @@
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1555,10 +1561,10 @@
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1569,26 +1575,53 @@
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>3</v>
       </c>
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>3</v>
       </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>3</v>
       </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -1602,6 +1635,21 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tag and frog (#872)
Test cases for entity tagging conflicts between trainings.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9A082E-45C9-48E4-80C7-BF2C977E7D25}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4751989-C385-4C21-9AD7-0BD159037626}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10884" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="103">
   <si>
     <t>Page</t>
   </si>
@@ -328,6 +328,18 @@
   </si>
   <si>
     <t>Selecting a Bot turn causes Action Selection UI Elements to show up</t>
+  </si>
+  <si>
+    <t>CreateModels.TagAndFrog</t>
+  </si>
+  <si>
+    <t>User can label one word of a user utterance as a single value for a single entity</t>
+  </si>
+  <si>
+    <t>User can label two words of a user utterance as two values for a single entity</t>
+  </si>
+  <si>
+    <t>User can label two words of a user utterance as a single value for a single entity</t>
   </si>
 </sst>
 </file>
@@ -437,8 +449,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F68" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F68" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F70" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F70" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -748,11 +760,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1454,36 +1466,45 @@
       <c r="C48" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D48" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1491,13 +1512,13 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1505,13 +1526,13 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1519,13 +1540,13 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1533,41 +1554,41 @@
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D55" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" t="s">
-        <v>12</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1575,13 +1596,13 @@
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1589,13 +1610,13 @@
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -1603,13 +1624,13 @@
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1617,20 +1638,38 @@
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
@@ -1650,6 +1689,16 @@
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: regression test list and updated test grid
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1973B851-47DC-4D26-88E7-1A23ED1B2A32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCBC503-ADB8-4AAA-A46E-02FA2CFBCFC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="146">
   <si>
     <t>Page</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Michael manually does this on a regular basis</t>
   </si>
   <si>
-    <t>Entity shows up as selected when single word utterance is made by user</t>
-  </si>
-  <si>
     <t>DisqualifyingEntities</t>
   </si>
   <si>
@@ -219,15 +216,6 @@
     <t>Disqualifying Entity</t>
   </si>
   <si>
-    <t>Entities are detected based on past training</t>
-  </si>
-  <si>
-    <t>Entity Selection</t>
-  </si>
-  <si>
-    <t>User can select entity to be stored in memory</t>
-  </si>
-  <si>
     <t>All WhatsYourName tests</t>
   </si>
   <si>
@@ -406,6 +394,81 @@
   </si>
   <si>
     <t>The generic error message will persist after each error is fixed in a multiple error condition training until the last error is fixed.</t>
+  </si>
+  <si>
+    <t>EndSession</t>
+  </si>
+  <si>
+    <t>EndSession.EndSession</t>
+  </si>
+  <si>
+    <t>An EndSession chat turn should only contain a delete button when selected.</t>
+  </si>
+  <si>
+    <t>Score Action for any Bot turn other than the last turn should disable all EndSession Actions.</t>
+  </si>
+  <si>
+    <t>Inserting a Bot turn so that it is NOT the last turn should not automatically select an EndSession action based on past trainings.</t>
+  </si>
+  <si>
+    <t>Bug 1913 - TODO</t>
+  </si>
+  <si>
+    <t>Score Action for the last Bot turn that is already an EndSession should NOT disable all other EndSession Actions.</t>
+  </si>
+  <si>
+    <t>EndSession.AddEndSessionAction</t>
+  </si>
+  <si>
+    <t>Chat input control for "Type your message" should not be visible when an EndSession Action has been used.</t>
+  </si>
+  <si>
+    <t>Entity shows up as labeled when single word utterance is made by user</t>
+  </si>
+  <si>
+    <t>Entities are detected and labeled based on past training</t>
+  </si>
+  <si>
+    <t>User can label entity to be stored in memory</t>
+  </si>
+  <si>
+    <t>Entity Labeling</t>
+  </si>
+  <si>
+    <t>Abandon button should discard Log Dialog session and not persist it.</t>
+  </si>
+  <si>
+    <t>Bot should respond to user utterance with expected response due to existing Train Dialogs</t>
+  </si>
+  <si>
+    <t>EndSession Action should show the Data defined in the Action as the final response to user utterance.</t>
+  </si>
+  <si>
+    <t>CreateModels.EndSession</t>
+  </si>
+  <si>
+    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn and saving it should not result in two Train Dialogs. (Bug 2026)</t>
+  </si>
+  <si>
+    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn should not delete the description field. (Bug 2026)</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>LODO</t>
+  </si>
+  <si>
+    <t>Editing a Bot turn that is the last turn, and the user creates a new EndSession Action, it should automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 2014)</t>
+  </si>
+  <si>
+    <t>Editing a Bot turn that is NOT the last turn, and the user creates a new EndSession Action, it should not automaticaly replace the existing Bot turn with that newly created EndSession Action. If the user follows on and creates another NON-EndSession Action, it should automatically replace the existing Bot turn. (Bug 1913)</t>
+  </si>
+  <si>
+    <t>Editing a Bot turn that is NOT the last turn, and the user creates a new EndSession Action, it should not automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 1913)</t>
+  </si>
+  <si>
+    <t>Inserting a Bot turn so that it IS the last turn should automatically select an EndSession action if past trainings would indicate that is the best Action. (Bug 1914)</t>
   </si>
 </sst>
 </file>
@@ -501,8 +564,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F90" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F90" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F112" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F112" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -812,15 +875,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81.28515625" style="3" customWidth="1"/>
@@ -847,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -915,7 +979,7 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -977,7 +1041,7 @@
         <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -996,101 +1060,101 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" t="s">
         <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
         <v>49</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
         <v>50</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
@@ -1098,16 +1162,16 @@
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
         <v>43</v>
@@ -1115,632 +1179,632 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" t="s">
         <v>84</v>
-      </c>
-      <c r="C22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" t="s">
         <v>84</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
         <v>84</v>
-      </c>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
         <v>84</v>
-      </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
         <v>84</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
         <v>16</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E31" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
         <v>16</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E37" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E38" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" t="s">
         <v>74</v>
-      </c>
-      <c r="B42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F42" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
         <v>16</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E46" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C49" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E49" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E50" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" t="s">
         <v>109</v>
-      </c>
-      <c r="E51" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="E52" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C53" t="s">
         <v>16</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E53" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
         <v>16</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E54" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C55" t="s">
         <v>16</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E55" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C56" t="s">
         <v>16</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E56" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
         <v>16</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E57" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C58" t="s">
         <v>16</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E58" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C59" t="s">
         <v>16</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E59" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C60" t="s">
         <v>16</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E60" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
         <v>16</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E61" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C62" t="s">
         <v>16</v>
@@ -1748,10 +1812,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s">
         <v>16</v>
@@ -1759,294 +1823,584 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C66" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C67" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C68" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E71" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" t="s">
+        <v>121</v>
+      </c>
+      <c r="C73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E74" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>70</v>
+      </c>
+      <c r="B77" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E78" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" t="s">
+        <v>121</v>
+      </c>
+      <c r="C79" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E79" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" t="s">
+        <v>121</v>
+      </c>
+      <c r="C80" t="s">
+        <v>16</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E80" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>70</v>
+      </c>
+      <c r="B81" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>70</v>
+      </c>
+      <c r="B82" t="s">
+        <v>121</v>
+      </c>
+      <c r="C82" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E82" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>17</v>
+      </c>
+      <c r="B86" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>17</v>
+      </c>
+      <c r="B87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>17</v>
+      </c>
+      <c r="B89" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>3</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B92" t="s">
         <v>4</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C92" t="s">
         <v>42</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D92" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E92" t="s">
+        <v>94</v>
+      </c>
+      <c r="F92" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E94" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" t="s">
+        <v>4</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s">
+        <v>96</v>
+      </c>
+      <c r="C96" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F70" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>3</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B98" t="s">
         <v>4</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C98" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" t="s">
+        <v>4</v>
+      </c>
+      <c r="C99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>42</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
         <v>12</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="D102" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>3</v>
       </c>
-      <c r="B72" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" t="s">
         <v>8</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E72" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="D103" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>3</v>
       </c>
-      <c r="B73" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B104" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D104" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>3</v>
+      </c>
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>3</v>
+      </c>
+      <c r="B108" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>3</v>
       </c>
-      <c r="B74" t="s">
-        <v>100</v>
-      </c>
-      <c r="C74" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>3</v>
       </c>
-      <c r="B75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>3</v>
       </c>
-      <c r="B76" t="s">
-        <v>4</v>
-      </c>
-      <c r="C76" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77" t="s">
-        <v>11</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" t="s">
-        <v>42</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>3</v>
-      </c>
-      <c r="B80" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" t="s">
-        <v>12</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" t="s">
-        <v>8</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" t="s">
-        <v>8</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" t="s">
-        <v>10</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" t="s">
-        <v>11</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: xlsx files are a pain in GIT
Not sure if this is the same or different so saving once again.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCBC503-ADB8-4AAA-A46E-02FA2CFBCFC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF83D70-84CF-47FE-B5FE-2F26DFF99F15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="144">
   <si>
     <t>Page</t>
   </si>
@@ -411,9 +411,6 @@
     <t>Inserting a Bot turn so that it is NOT the last turn should not automatically select an EndSession action based on past trainings.</t>
   </si>
   <si>
-    <t>Bug 1913 - TODO</t>
-  </si>
-  <si>
     <t>Score Action for the last Bot turn that is already an EndSession should NOT disable all other EndSession Actions.</t>
   </si>
   <si>
@@ -456,19 +453,16 @@
     <t>TODO</t>
   </si>
   <si>
-    <t>LODO</t>
-  </si>
-  <si>
     <t>Editing a Bot turn that is the last turn, and the user creates a new EndSession Action, it should automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 2014)</t>
   </si>
   <si>
-    <t>Editing a Bot turn that is NOT the last turn, and the user creates a new EndSession Action, it should not automaticaly replace the existing Bot turn with that newly created EndSession Action. If the user follows on and creates another NON-EndSession Action, it should automatically replace the existing Bot turn. (Bug 1913)</t>
-  </si>
-  <si>
     <t>Editing a Bot turn that is NOT the last turn, and the user creates a new EndSession Action, it should not automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 1913)</t>
   </si>
   <si>
-    <t>Inserting a Bot turn so that it IS the last turn should automatically select an EndSession action if past trainings would indicate that is the best Action. (Bug 1914)</t>
+    <t>Editing a Bot turn that is NOT the last turn, and the user creates a new EndSession Action, it should not automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 1913) If the user imediately follows on and creates another NON-EndSession Action, it should automatically replace the existing Bot turn. (to confirm fix did not break this)</t>
+  </si>
+  <si>
+    <t>Inserting a Bot turn so that it IS the last turn should automatically select an EndSession action if past trainings would indicate that is the best Action. (Bug 2027)</t>
   </si>
 </sst>
 </file>
@@ -877,9 +871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
   <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,7 +1063,7 @@
         <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E12" t="s">
         <v>46</v>
@@ -1188,7 +1182,7 @@
         <v>47</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
         <v>61</v>
@@ -1196,13 +1190,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1904,7 +1898,7 @@
         <v>16</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E71" t="s">
         <v>122</v>
@@ -1969,10 +1963,10 @@
         <v>16</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E75" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2000,13 +1994,13 @@
         <v>16</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E77" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>70</v>
       </c>
@@ -2017,10 +2011,10 @@
         <v>16</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2034,10 +2028,10 @@
         <v>16</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E79" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2051,10 +2045,10 @@
         <v>16</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E80" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2068,10 +2062,10 @@
         <v>16</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E81" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2085,10 +2079,10 @@
         <v>16</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E82" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2102,7 +2096,7 @@
         <v>17</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2116,7 +2110,7 @@
         <v>17</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2130,7 +2124,7 @@
         <v>17</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create End Session Model (#1103)
When I created the EndSession test case I manually created the model that I imported for that test thinking that I did not need to use automation to build it. However, I hit 2 significant bugs (1968 & 1969) at the time which reproduced for me in that short time frame I was working on it (over the course of 30 minutes or so). I filed the bugs and in the morning nobody, not even me, could reproduce the bugs.

So I am adding in this test case thinking if it is some confluence of timing issues with services that those bugs will eventually occur again and we can catch it.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD2D532-B347-4996-8DDE-99C2D116BB0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF83D70-84CF-47FE-B5FE-2F26DFF99F15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="144">
   <si>
     <t>Page</t>
   </si>
@@ -411,27 +411,9 @@
     <t>Inserting a Bot turn so that it is NOT the last turn should not automatically select an EndSession action based on past trainings.</t>
   </si>
   <si>
-    <t>Bug 1913 - TODO</t>
-  </si>
-  <si>
-    <t>Inserting a Bot turn so that it IS the last turn should automatically select an EndSession action if past trainings would indicate that is the best Action.</t>
-  </si>
-  <si>
-    <t>Editing a Bot turn that is NOT the last turn, and the user creates a new EndSession Action, it should not automaticaly replace the existing Bot turn with that newly created EndSession Action.</t>
-  </si>
-  <si>
-    <t>Editing a Bot turn that is the last turn, and the user creates a new EndSession Action, it should automaticaly replace the existing Bot turn with that newly created EndSession Action.</t>
-  </si>
-  <si>
-    <t>Editing a Bot turn that is NOT the last turn, and the user creates a new EndSession Action, it should not automaticaly replace the existing Bot turn with that newly created EndSession Action. If the user follows on and creates another NON-EndSession Action, it should automatically replace the existing Bot turn.</t>
-  </si>
-  <si>
     <t>Score Action for the last Bot turn that is already an EndSession should NOT disable all other EndSession Actions.</t>
   </si>
   <si>
-    <t>Bug 2014 - TODO</t>
-  </si>
-  <si>
     <t>EndSession.AddEndSessionAction</t>
   </si>
   <si>
@@ -457,6 +439,30 @@
   </si>
   <si>
     <t>EndSession Action should show the Data defined in the Action as the final response to user utterance.</t>
+  </si>
+  <si>
+    <t>CreateModels.EndSession</t>
+  </si>
+  <si>
+    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn and saving it should not result in two Train Dialogs. (Bug 2026)</t>
+  </si>
+  <si>
+    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn should not delete the description field. (Bug 2026)</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Editing a Bot turn that is the last turn, and the user creates a new EndSession Action, it should automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 2014)</t>
+  </si>
+  <si>
+    <t>Editing a Bot turn that is NOT the last turn, and the user creates a new EndSession Action, it should not automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 1913)</t>
+  </si>
+  <si>
+    <t>Editing a Bot turn that is NOT the last turn, and the user creates a new EndSession Action, it should not automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 1913) If the user imediately follows on and creates another NON-EndSession Action, it should automatically replace the existing Bot turn. (to confirm fix did not break this)</t>
+  </si>
+  <si>
+    <t>Inserting a Bot turn so that it IS the last turn should automatically select an EndSession action if past trainings would indicate that is the best Action. (Bug 2027)</t>
   </si>
 </sst>
 </file>
@@ -552,8 +558,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F110" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F110" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F112" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F112" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -863,11 +869,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1063,7 @@
         <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E12" t="s">
         <v>46</v>
@@ -1176,7 +1182,7 @@
         <v>47</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
         <v>61</v>
@@ -1184,13 +1190,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1892,7 +1898,7 @@
         <v>16</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E71" t="s">
         <v>122</v>
@@ -1957,10 +1963,10 @@
         <v>16</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="E75" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1988,13 +1994,13 @@
         <v>16</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="E77" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>70</v>
       </c>
@@ -2005,10 +2011,10 @@
         <v>16</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="E78" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2022,10 +2028,10 @@
         <v>16</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="E79" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2039,41 +2045,47 @@
         <v>16</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E80" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>70</v>
+      </c>
+      <c r="B81" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E81" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="C82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>17</v>
-      </c>
-      <c r="B83" t="s">
-        <v>17</v>
-      </c>
-      <c r="C83" t="s">
-        <v>17</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="E82" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -2084,7 +2096,7 @@
         <v>17</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2097,8 +2109,11 @@
       <c r="C85" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D85" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -2107,6 +2122,9 @@
       </c>
       <c r="C86" t="s">
         <v>17</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2120,38 +2138,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>3</v>
-      </c>
-      <c r="B90" t="s">
-        <v>4</v>
-      </c>
-      <c r="C90" t="s">
-        <v>42</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E90" t="s">
-        <v>94</v>
-      </c>
-      <c r="F90" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B91" t="s">
-        <v>4</v>
-      </c>
-      <c r="C91" t="s">
-        <v>12</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>97</v>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>17</v>
+      </c>
+      <c r="B89" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2162,13 +2168,16 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E92" t="s">
-        <v>89</v>
+        <v>94</v>
+      </c>
+      <c r="F92" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2179,10 +2188,10 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2190,13 +2199,16 @@
         <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="C94" t="s">
         <v>8</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>95</v>
+        <v>36</v>
+      </c>
+      <c r="E94" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2210,7 +2222,7 @@
         <v>8</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2218,13 +2230,13 @@
         <v>3</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C96" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2235,9 +2247,23 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D97" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2246,27 +2272,13 @@
         <v>3</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>3</v>
-      </c>
-      <c r="B100" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" t="s">
-        <v>12</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2277,10 +2289,10 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2291,7 +2303,7 @@
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>35</v>
@@ -2305,10 +2317,10 @@
         <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2319,23 +2331,38 @@
         <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>3</v>
       </c>
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
       <c r="B106" t="s">
-        <v>99</v>
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2347,6 +2374,9 @@
       <c r="A108" t="s">
         <v>3</v>
       </c>
+      <c r="B108" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
@@ -2355,6 +2385,16 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: refactor plus test grid update
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AE0D30-5F4B-40CE-B990-7E2BEB24B24D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E4949E-8DC8-44F2-95A6-4BB99F37407D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="152">
   <si>
     <t>Page</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Saved to a file in JSON format</t>
   </si>
   <si>
-    <t>Disapears from home page, cannot manually create a link to it.</t>
-  </si>
-  <si>
     <t>Setting is persisted, shows checked after save then edit</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>Michael manually does this on a regular basis</t>
   </si>
   <si>
-    <t>DisqualifyingEntities</t>
-  </si>
-  <si>
     <t>Action Dialog, Train Dialog</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>No Wait</t>
   </si>
   <si>
-    <t>WaitVsNoWaitActions</t>
-  </si>
-  <si>
     <t>Action is disabled in Train Dialog Scorer component when disqualifying Entities exist in memory</t>
   </si>
   <si>
@@ -309,9 +300,6 @@
     <t>User can label two words of a user utterance as two values for a single entity</t>
   </si>
   <si>
-    <t>User can label two words of a user utterance as a single value for a single entity</t>
-  </si>
-  <si>
     <t>Only verifies name</t>
   </si>
   <si>
@@ -426,12 +414,6 @@
     <t>Entities are detected and labeled based on past training</t>
   </si>
   <si>
-    <t>User can label entity to be stored in memory</t>
-  </si>
-  <si>
-    <t>Entity Labeling</t>
-  </si>
-  <si>
     <t>Abandon button should discard Log Dialog session and not persist it.</t>
   </si>
   <si>
@@ -444,9 +426,6 @@
     <t>CreateModels.EndSession</t>
   </si>
   <si>
-    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn and saving it should not result in two Train Dialogs. (Bug 2026)</t>
-  </si>
-  <si>
     <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn should not delete the description field. (Bug 2026)</t>
   </si>
   <si>
@@ -463,6 +442,51 @@
   </si>
   <si>
     <t>Inserting a Bot turn so that it IS the last turn should automatically select an EndSession action if past trainings would indicate that is the best Action. (Bug 2027)</t>
+  </si>
+  <si>
+    <t>EditAndBranching.TagAndFrog</t>
+  </si>
+  <si>
+    <t>Disapears from home page.</t>
+  </si>
+  <si>
+    <t>The Description field should be empty on a new Train Dialog after adding a Description to a Train Dialog then Scoring an EndSession Bot response. (Bug 2031)</t>
+  </si>
+  <si>
+    <t>Exporting a model after saving and EndSession Train Dialog should not result in a duplicate Train Dialog in the model. (Bug 2032)</t>
+  </si>
+  <si>
+    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn and saving it should not result in two Train Dialogs. (Bug 1969)</t>
+  </si>
+  <si>
+    <t>Train.BookMeAFlight</t>
+  </si>
+  <si>
+    <t>User can label two or more words of a user utterance as a single value for a single entity</t>
+  </si>
+  <si>
+    <t>Actions containing entites with "datetimeV2" resolver types resolve common expressions of dates, like "tomorrow" and "Sunday next week", to the correct calander dates.</t>
+  </si>
+  <si>
+    <t>Train.DisqualifyingEntities</t>
+  </si>
+  <si>
+    <t>Train.WaitVsNoWaitActions</t>
+  </si>
+  <si>
+    <t>Required Entity</t>
+  </si>
+  <si>
+    <t>Action is disabled in Train Dialog Scorer component when it requires 1 Entity and it does not exist in memory</t>
+  </si>
+  <si>
+    <t>Action is disabled in Train Dialog Scorer component when it requires 2 or more Entities and any one of them does not exist in memory</t>
+  </si>
+  <si>
+    <t>Train.WhatsYourName</t>
+  </si>
+  <si>
+    <t>Partially covered by multiple tests - TODO for full coverage</t>
   </si>
 </sst>
 </file>
@@ -558,8 +582,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F112" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F112" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F117" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F117" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -869,11 +893,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -916,13 +940,13 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -933,13 +957,13 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -956,7 +980,7 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -973,7 +997,7 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,7 +1042,7 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1035,7 +1059,7 @@
         <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1049,778 +1073,805 @@
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>130</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>131</v>
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="E29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
         <v>77</v>
       </c>
-      <c r="E32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>66</v>
+        <v>76</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C42" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" t="s">
         <v>71</v>
-      </c>
-      <c r="F42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
         <v>16</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" t="s">
         <v>86</v>
       </c>
-      <c r="C47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E50" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C51" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" t="s">
         <v>105</v>
       </c>
-      <c r="E51" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C52" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C53" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C54" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="E54" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C55" t="s">
         <v>16</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>111</v>
+      <c r="D55" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="E55" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C56" t="s">
         <v>16</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E56" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C57" t="s">
         <v>16</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E57" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C58" t="s">
         <v>16</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E58" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
         <v>16</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E59" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>119</v>
+      <c r="D60" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="E60" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>120</v>
+      <c r="D61" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="E61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>70</v>
-      </c>
-      <c r="B62" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>70</v>
-      </c>
-      <c r="B63" t="s">
-        <v>102</v>
-      </c>
-      <c r="C63" t="s">
-        <v>16</v>
+      <c r="E63" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C64" t="s">
         <v>16</v>
@@ -1828,10 +1879,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C65" t="s">
         <v>16</v>
@@ -1839,10 +1890,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C66" t="s">
         <v>16</v>
@@ -1850,10 +1901,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C67" t="s">
         <v>16</v>
@@ -1861,295 +1912,298 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C68" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
+        <v>98</v>
+      </c>
+      <c r="C70" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72" t="s">
+        <v>117</v>
+      </c>
+      <c r="C72" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E73" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" t="s">
+        <v>117</v>
+      </c>
+      <c r="C74" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E74" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" t="s">
+        <v>117</v>
+      </c>
+      <c r="C75" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" t="s">
+        <v>117</v>
+      </c>
+      <c r="C76" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C70" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70" s="3" t="s">
+      <c r="E76" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>67</v>
+      </c>
+      <c r="B77" t="s">
+        <v>117</v>
+      </c>
+      <c r="C77" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E77" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
+        <v>117</v>
+      </c>
+      <c r="C79" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E79" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" t="s">
+        <v>16</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E80" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>67</v>
+      </c>
+      <c r="B81" t="s">
+        <v>117</v>
+      </c>
+      <c r="C81" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E81" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E70" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>121</v>
-      </c>
-      <c r="C71" t="s">
-        <v>16</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E71" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" t="s">
-        <v>121</v>
-      </c>
-      <c r="C72" t="s">
-        <v>16</v>
-      </c>
-      <c r="D72" s="3" t="s">
+      <c r="E82" t="s">
         <v>123</v>
       </c>
-      <c r="E72" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>70</v>
-      </c>
-      <c r="B73" t="s">
-        <v>121</v>
-      </c>
-      <c r="C73" t="s">
-        <v>16</v>
-      </c>
-      <c r="E73" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74" t="s">
-        <v>16</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E74" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>70</v>
-      </c>
-      <c r="B75" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E75" t="s">
+    </row>
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" t="s">
+        <v>117</v>
+      </c>
+      <c r="C83" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E83" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>67</v>
+      </c>
+      <c r="B84" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E84" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E85" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>67</v>
+      </c>
+      <c r="B86" t="s">
+        <v>117</v>
+      </c>
+      <c r="C86" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>70</v>
-      </c>
-      <c r="B76" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" t="s">
-        <v>16</v>
-      </c>
-      <c r="E76" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>70</v>
-      </c>
-      <c r="B77" t="s">
-        <v>121</v>
-      </c>
-      <c r="C77" t="s">
-        <v>16</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E77" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>70</v>
-      </c>
-      <c r="B78" t="s">
-        <v>121</v>
-      </c>
-      <c r="C78" t="s">
-        <v>16</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E78" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" t="s">
-        <v>121</v>
-      </c>
-      <c r="C79" t="s">
-        <v>16</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E79" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>70</v>
-      </c>
-      <c r="B80" t="s">
-        <v>121</v>
-      </c>
-      <c r="C80" t="s">
-        <v>16</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E80" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>70</v>
-      </c>
-      <c r="B81" t="s">
-        <v>121</v>
-      </c>
-      <c r="C81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E81" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>70</v>
-      </c>
-      <c r="B82" t="s">
-        <v>121</v>
-      </c>
-      <c r="C82" t="s">
-        <v>16</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E82" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>17</v>
-      </c>
-      <c r="B84" t="s">
-        <v>17</v>
-      </c>
-      <c r="C84" t="s">
-        <v>17</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>17</v>
-      </c>
-      <c r="B85" t="s">
-        <v>17</v>
-      </c>
-      <c r="C85" t="s">
-        <v>17</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>17</v>
-      </c>
-      <c r="B86" t="s">
-        <v>17</v>
-      </c>
-      <c r="C86" t="s">
-        <v>17</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B87" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="C87" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>17</v>
-      </c>
-      <c r="B88" t="s">
-        <v>17</v>
-      </c>
-      <c r="C88" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -2159,87 +2213,72 @@
       <c r="C89" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D89" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>17</v>
+      </c>
+      <c r="B90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" t="s">
+        <v>17</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C91" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C92" t="s">
-        <v>42</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E92" t="s">
-        <v>94</v>
-      </c>
-      <c r="F92" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C93" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C94" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E94" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>3</v>
-      </c>
-      <c r="B95" t="s">
-        <v>4</v>
-      </c>
-      <c r="C95" t="s">
-        <v>8</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>3</v>
-      </c>
-      <c r="B96" t="s">
-        <v>96</v>
-      </c>
-      <c r="C96" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -2247,13 +2286,19 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E97" t="s">
+        <v>90</v>
+      </c>
+      <c r="F97" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -2261,13 +2306,13 @@
         <v>4</v>
       </c>
       <c r="C98" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>3</v>
       </c>
@@ -2275,83 +2320,86 @@
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E99" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>3</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="C101" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>3</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>3</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>3</v>
-      </c>
-      <c r="B105" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" t="s">
-        <v>10</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -2359,42 +2407,112 @@
         <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>10</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor Train & Edit Dialog - Test Grid Updated (#1116)
Updated the Test Grid - Should now contain most test scenarios that are covered (unless I missed something)

Refactored Train.BookMeAFlight test case into the new pattern so as to help me understand what it covered while updating the Test Grid.

Moved the code that was in EditDialogModal.js into Train.js since it was confusing while using the two for coding up test cases.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF83D70-84CF-47FE-B5FE-2F26DFF99F15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E4949E-8DC8-44F2-95A6-4BB99F37407D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="152">
   <si>
     <t>Page</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Saved to a file in JSON format</t>
   </si>
   <si>
-    <t>Disapears from home page, cannot manually create a link to it.</t>
-  </si>
-  <si>
     <t>Setting is persisted, shows checked after save then edit</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>Michael manually does this on a regular basis</t>
   </si>
   <si>
-    <t>DisqualifyingEntities</t>
-  </si>
-  <si>
     <t>Action Dialog, Train Dialog</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>No Wait</t>
   </si>
   <si>
-    <t>WaitVsNoWaitActions</t>
-  </si>
-  <si>
     <t>Action is disabled in Train Dialog Scorer component when disqualifying Entities exist in memory</t>
   </si>
   <si>
@@ -309,9 +300,6 @@
     <t>User can label two words of a user utterance as two values for a single entity</t>
   </si>
   <si>
-    <t>User can label two words of a user utterance as a single value for a single entity</t>
-  </si>
-  <si>
     <t>Only verifies name</t>
   </si>
   <si>
@@ -426,12 +414,6 @@
     <t>Entities are detected and labeled based on past training</t>
   </si>
   <si>
-    <t>User can label entity to be stored in memory</t>
-  </si>
-  <si>
-    <t>Entity Labeling</t>
-  </si>
-  <si>
     <t>Abandon button should discard Log Dialog session and not persist it.</t>
   </si>
   <si>
@@ -444,9 +426,6 @@
     <t>CreateModels.EndSession</t>
   </si>
   <si>
-    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn and saving it should not result in two Train Dialogs. (Bug 2026)</t>
-  </si>
-  <si>
     <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn should not delete the description field. (Bug 2026)</t>
   </si>
   <si>
@@ -463,6 +442,51 @@
   </si>
   <si>
     <t>Inserting a Bot turn so that it IS the last turn should automatically select an EndSession action if past trainings would indicate that is the best Action. (Bug 2027)</t>
+  </si>
+  <si>
+    <t>EditAndBranching.TagAndFrog</t>
+  </si>
+  <si>
+    <t>Disapears from home page.</t>
+  </si>
+  <si>
+    <t>The Description field should be empty on a new Train Dialog after adding a Description to a Train Dialog then Scoring an EndSession Bot response. (Bug 2031)</t>
+  </si>
+  <si>
+    <t>Exporting a model after saving and EndSession Train Dialog should not result in a duplicate Train Dialog in the model. (Bug 2032)</t>
+  </si>
+  <si>
+    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn and saving it should not result in two Train Dialogs. (Bug 1969)</t>
+  </si>
+  <si>
+    <t>Train.BookMeAFlight</t>
+  </si>
+  <si>
+    <t>User can label two or more words of a user utterance as a single value for a single entity</t>
+  </si>
+  <si>
+    <t>Actions containing entites with "datetimeV2" resolver types resolve common expressions of dates, like "tomorrow" and "Sunday next week", to the correct calander dates.</t>
+  </si>
+  <si>
+    <t>Train.DisqualifyingEntities</t>
+  </si>
+  <si>
+    <t>Train.WaitVsNoWaitActions</t>
+  </si>
+  <si>
+    <t>Required Entity</t>
+  </si>
+  <si>
+    <t>Action is disabled in Train Dialog Scorer component when it requires 1 Entity and it does not exist in memory</t>
+  </si>
+  <si>
+    <t>Action is disabled in Train Dialog Scorer component when it requires 2 or more Entities and any one of them does not exist in memory</t>
+  </si>
+  <si>
+    <t>Train.WhatsYourName</t>
+  </si>
+  <si>
+    <t>Partially covered by multiple tests - TODO for full coverage</t>
   </si>
 </sst>
 </file>
@@ -558,8 +582,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F112" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F112" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F117" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F117" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -869,11 +893,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -916,13 +940,13 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -933,13 +957,13 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -956,7 +980,7 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -973,7 +997,7 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,7 +1042,7 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1035,7 +1059,7 @@
         <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1049,778 +1073,805 @@
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>130</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>131</v>
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="E29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
         <v>77</v>
       </c>
-      <c r="E32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>66</v>
+        <v>76</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C42" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" t="s">
         <v>71</v>
-      </c>
-      <c r="F42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
         <v>16</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" t="s">
         <v>86</v>
       </c>
-      <c r="C47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E50" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C51" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" t="s">
         <v>105</v>
       </c>
-      <c r="E51" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C52" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C53" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C54" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="E54" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C55" t="s">
         <v>16</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>111</v>
+      <c r="D55" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="E55" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C56" t="s">
         <v>16</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E56" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C57" t="s">
         <v>16</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E57" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C58" t="s">
         <v>16</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E58" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
         <v>16</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E59" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>119</v>
+      <c r="D60" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="E60" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>120</v>
+      <c r="D61" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="E61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>70</v>
-      </c>
-      <c r="B62" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>70</v>
-      </c>
-      <c r="B63" t="s">
-        <v>102</v>
-      </c>
-      <c r="C63" t="s">
-        <v>16</v>
+      <c r="E63" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C64" t="s">
         <v>16</v>
@@ -1828,10 +1879,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C65" t="s">
         <v>16</v>
@@ -1839,10 +1890,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C66" t="s">
         <v>16</v>
@@ -1850,10 +1901,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C67" t="s">
         <v>16</v>
@@ -1861,295 +1912,298 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C68" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
+        <v>98</v>
+      </c>
+      <c r="C70" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72" t="s">
+        <v>117</v>
+      </c>
+      <c r="C72" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E73" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" t="s">
+        <v>117</v>
+      </c>
+      <c r="C74" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E74" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" t="s">
+        <v>117</v>
+      </c>
+      <c r="C75" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" t="s">
+        <v>117</v>
+      </c>
+      <c r="C76" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C70" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70" s="3" t="s">
+      <c r="E76" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>67</v>
+      </c>
+      <c r="B77" t="s">
+        <v>117</v>
+      </c>
+      <c r="C77" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E77" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
+        <v>117</v>
+      </c>
+      <c r="C79" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E79" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" t="s">
+        <v>16</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E80" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>67</v>
+      </c>
+      <c r="B81" t="s">
+        <v>117</v>
+      </c>
+      <c r="C81" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E81" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E70" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>121</v>
-      </c>
-      <c r="C71" t="s">
-        <v>16</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E71" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" t="s">
-        <v>121</v>
-      </c>
-      <c r="C72" t="s">
-        <v>16</v>
-      </c>
-      <c r="D72" s="3" t="s">
+      <c r="E82" t="s">
         <v>123</v>
       </c>
-      <c r="E72" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>70</v>
-      </c>
-      <c r="B73" t="s">
-        <v>121</v>
-      </c>
-      <c r="C73" t="s">
-        <v>16</v>
-      </c>
-      <c r="E73" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74" t="s">
-        <v>16</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E74" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>70</v>
-      </c>
-      <c r="B75" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E75" t="s">
+    </row>
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" t="s">
+        <v>117</v>
+      </c>
+      <c r="C83" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E83" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>67</v>
+      </c>
+      <c r="B84" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E84" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E85" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>67</v>
+      </c>
+      <c r="B86" t="s">
+        <v>117</v>
+      </c>
+      <c r="C86" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>70</v>
-      </c>
-      <c r="B76" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" t="s">
-        <v>16</v>
-      </c>
-      <c r="E76" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>70</v>
-      </c>
-      <c r="B77" t="s">
-        <v>121</v>
-      </c>
-      <c r="C77" t="s">
-        <v>16</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E77" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>70</v>
-      </c>
-      <c r="B78" t="s">
-        <v>121</v>
-      </c>
-      <c r="C78" t="s">
-        <v>16</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E78" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" t="s">
-        <v>121</v>
-      </c>
-      <c r="C79" t="s">
-        <v>16</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E79" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>70</v>
-      </c>
-      <c r="B80" t="s">
-        <v>121</v>
-      </c>
-      <c r="C80" t="s">
-        <v>16</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E80" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>70</v>
-      </c>
-      <c r="B81" t="s">
-        <v>121</v>
-      </c>
-      <c r="C81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E81" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>70</v>
-      </c>
-      <c r="B82" t="s">
-        <v>121</v>
-      </c>
-      <c r="C82" t="s">
-        <v>16</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E82" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>17</v>
-      </c>
-      <c r="B84" t="s">
-        <v>17</v>
-      </c>
-      <c r="C84" t="s">
-        <v>17</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>17</v>
-      </c>
-      <c r="B85" t="s">
-        <v>17</v>
-      </c>
-      <c r="C85" t="s">
-        <v>17</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>17</v>
-      </c>
-      <c r="B86" t="s">
-        <v>17</v>
-      </c>
-      <c r="C86" t="s">
-        <v>17</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B87" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="C87" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>17</v>
-      </c>
-      <c r="B88" t="s">
-        <v>17</v>
-      </c>
-      <c r="C88" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -2159,87 +2213,72 @@
       <c r="C89" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D89" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>17</v>
+      </c>
+      <c r="B90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" t="s">
+        <v>17</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C91" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C92" t="s">
-        <v>42</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E92" t="s">
-        <v>94</v>
-      </c>
-      <c r="F92" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C93" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C94" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E94" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>3</v>
-      </c>
-      <c r="B95" t="s">
-        <v>4</v>
-      </c>
-      <c r="C95" t="s">
-        <v>8</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>3</v>
-      </c>
-      <c r="B96" t="s">
-        <v>96</v>
-      </c>
-      <c r="C96" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -2247,13 +2286,19 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E97" t="s">
+        <v>90</v>
+      </c>
+      <c r="F97" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -2261,13 +2306,13 @@
         <v>4</v>
       </c>
       <c r="C98" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>3</v>
       </c>
@@ -2275,83 +2320,86 @@
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E99" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>3</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="C101" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>3</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>3</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>3</v>
-      </c>
-      <c r="B105" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" t="s">
-        <v>10</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -2359,42 +2407,112 @@
         <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>10</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: one more minor change
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5682D816-9567-463B-919C-62E258B14072}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D00A077-75D8-4580-B8B4-05897AB60BCC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="242">
   <si>
     <t>Page</t>
   </si>
@@ -789,6 +789,9 @@
   </si>
   <si>
     <t>Verifies Train Dialog starts off with No Tags nor Descriptions. Verifies that adding Tags and Descriptions to Train Dialog and saving them results in them showing up in the grid. Verifies that editing Train Dialog shows the persisted T&amp;D. Verifies that changes made to T&amp;D are discarded when the Train Dialog is abandonded. Verifies that editing a Train Dialog and adding a new tag and modifying the description is persisted whtn the dialog is saved and reloaded. There are more steps that modify the T&amp;D, delete a turn, save, edit again, add more rounds, and finally verify the T&amp;Ds again. Branching and T&amp;D modifications verified after saving.</t>
+  </si>
+  <si>
+    <t>A very simple test of Log Dialogs with 2 rounds. Basically the same thing the loop test does without the loop.</t>
   </si>
 </sst>
 </file>
@@ -3060,8 +3063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B719F-1470-4AFA-970E-2998AD817A19}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3330,7 +3333,9 @@
       <c r="B25" t="s">
         <v>182</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D26" s="3"/>

</xml_diff>

<commit_message>
fix: tag and frog
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EF505E-561B-472A-A211-B883672C5EE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FF3A32-E8F1-45BE-87E1-D6DFB5C2A224}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="274">
   <si>
     <t>Page</t>
   </si>
@@ -547,9 +547,6 @@
     <t>DisqualifyingEntities</t>
   </si>
   <si>
-    <t>EntitiesAffectActionScoring</t>
-  </si>
-  <si>
     <t>Creates a model with Actions that can be disqualified in scoring by Disqualifying, Expected and Required Entities</t>
   </si>
   <si>
@@ -559,29 +556,6 @@
     <t>TagAndFrog</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ConsistentEntityLabeling</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-EntityLabeling</t>
-    </r>
-  </si>
-  <si>
     <t>Creates a model to be used to validate that consistent Entity labeling is enforced by the UI</t>
   </si>
   <si>
@@ -603,38 +577,15 @@
     <t>WhatsYourName</t>
   </si>
   <si>
-    <t>TextEntityAndActions</t>
-  </si>
-  <si>
     <t>Creates a model with a "name" entity and two simple actions; "What's your name" and "Hello $name"</t>
   </si>
   <si>
     <t>EditAndBranching</t>
   </si>
   <si>
-    <t>BasicBranching
-SimpleBranching</t>
-  </si>
-  <si>
     <t>Test the basic Train Dialog branching feature and verifies that the original dialog does not change and that the branched dialog is persisted correctly.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">ConsistentEntityLabeling
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EntityLabeling</t>
-    </r>
-  </si>
-  <si>
     <t>Verifies that the user cannot modify training such that entity labeling would become inconsistent.</t>
   </si>
   <si>
@@ -653,9 +604,6 @@
     <t>ErrorHandling</t>
   </si>
   <si>
-    <t>(more tests planed based on bugs reports)</t>
-  </si>
-  <si>
     <t>ActionUnavailable</t>
   </si>
   <si>
@@ -879,6 +827,43 @@
   </si>
   <si>
     <t>Verify that you can delete an Action that is not used by a Train Dialog by simply confirming that you want to delete it without a warning poping up.</t>
+  </si>
+  <si>
+    <t>Add Turn</t>
+  </si>
+  <si>
+    <t>Edit a turn, verify "Submit Changes" and "Undo" button is disabled. Change entity label, verify "Submit Changes" and "Undo" buttons become enabled.
+Variations from here:
+1) Submit - verify expectation
+2) Undo - verify returns to original state
+3) Select a different User Turn - verify it asks to save changes - yes verify - no verify those buttons are disabled and returns to original state just like undo (bug 2074)
+4) Select a different Bot Turn - verify same as #3 (bug 2075)</t>
+  </si>
+  <si>
+    <t>Add a new user turn to new or exiting Train Dialog (at User turn 2 and beyond) and "Undo" button should show up.
+Variations from here:
+1) Undo - verify
+2) Score Actions - verify - this is the most common path and is verified in many places
+3) Abandon - verify 
+4) Verify cannot click on to edit any other existing turn</t>
+  </si>
+  <si>
+    <t>Entity labeling from ConsistentEntityLabeling tests</t>
+  </si>
+  <si>
+    <t>TODO new case for when something was not labeled and now it is</t>
+  </si>
+  <si>
+    <t>******</t>
+  </si>
+  <si>
+    <t>EntityLabeling</t>
+  </si>
+  <si>
+    <t>ConsistentEntityLabeling</t>
+  </si>
+  <si>
+    <t>(more tests planed based on bug reports)</t>
   </si>
 </sst>
 </file>
@@ -1010,8 +995,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F150" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F150" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F156" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F156" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -1321,11 +1306,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1520,13 +1505,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1534,13 +1519,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1548,13 +1533,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1562,13 +1547,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1576,13 +1561,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1590,13 +1575,13 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,7 +1612,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1641,7 +1626,7 @@
         <v>39</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1655,7 +1640,7 @@
         <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1669,7 +1654,7 @@
         <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1683,7 +1668,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1697,7 +1682,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1711,7 +1696,7 @@
         <v>39</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1725,7 +1710,7 @@
         <v>39</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1733,13 +1718,13 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1747,13 +1732,13 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1761,13 +1746,13 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1885,13 +1870,13 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1899,13 +1884,13 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1913,13 +1898,13 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1927,13 +1912,13 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2242,41 +2227,35 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>58</v>
+        <v>265</v>
       </c>
       <c r="C66" t="s">
         <v>15</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E66" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>58</v>
-      </c>
-      <c r="C67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2287,10 +2266,10 @@
         <v>15</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E68" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2304,13 +2283,13 @@
         <v>15</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E69" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -2321,7 +2300,7 @@
         <v>15</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E70" t="s">
         <v>58</v>
@@ -2338,7 +2317,10 @@
         <v>15</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="E71" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2352,13 +2334,13 @@
         <v>15</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E72" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>66</v>
       </c>
@@ -2369,10 +2351,7 @@
         <v>15</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E73" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2386,10 +2365,10 @@
         <v>15</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E74" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2403,13 +2382,13 @@
         <v>15</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="E75" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>66</v>
       </c>
@@ -2420,7 +2399,10 @@
         <v>15</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="E76" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2434,13 +2416,13 @@
         <v>15</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F77" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="E77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>66</v>
       </c>
@@ -2451,7 +2433,24 @@
         <v>15</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F79" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,33 +2458,13 @@
         <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C80" t="s">
         <v>15</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E80" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>66</v>
-      </c>
-      <c r="B81" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E81" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2499,112 +2478,60 @@
         <v>15</v>
       </c>
       <c r="D82" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>66</v>
+      </c>
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" t="s">
+        <v>82</v>
+      </c>
+      <c r="C84" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E84" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>66</v>
-      </c>
-      <c r="B84" t="s">
-        <v>97</v>
-      </c>
-      <c r="C84" t="s">
-        <v>13</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E84" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>66</v>
-      </c>
-      <c r="B85" t="s">
-        <v>97</v>
-      </c>
-      <c r="C85" t="s">
-        <v>13</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E85" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>66</v>
-      </c>
-      <c r="B86" t="s">
-        <v>97</v>
-      </c>
-      <c r="C86" t="s">
-        <v>13</v>
+        <v>270</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E86" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>66</v>
-      </c>
-      <c r="B87" t="s">
-        <v>97</v>
-      </c>
-      <c r="C87" t="s">
-        <v>15</v>
+        <v>270</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E87" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>66</v>
-      </c>
-      <c r="B88" t="s">
-        <v>97</v>
-      </c>
-      <c r="C88" t="s">
-        <v>15</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E88" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>66</v>
-      </c>
-      <c r="B89" t="s">
-        <v>97</v>
-      </c>
-      <c r="C89" t="s">
-        <v>15</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E89" t="s">
-        <v>105</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2615,16 +2542,16 @@
         <v>97</v>
       </c>
       <c r="C90" t="s">
-        <v>15</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>106</v>
+        <v>13</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="E90" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>66</v>
       </c>
@@ -2632,13 +2559,13 @@
         <v>97</v>
       </c>
       <c r="C91" t="s">
-        <v>15</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>107</v>
+        <v>13</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="E91" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2649,13 +2576,13 @@
         <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>15</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>109</v>
+        <v>13</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="E92" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2668,11 +2595,11 @@
       <c r="C93" t="s">
         <v>15</v>
       </c>
-      <c r="D93" s="4" t="s">
-        <v>113</v>
+      <c r="D93" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="E93" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2685,14 +2612,14 @@
       <c r="C94" t="s">
         <v>15</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>112</v>
+      <c r="D94" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="E94" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>66</v>
       </c>
@@ -2702,11 +2629,11 @@
       <c r="C95" t="s">
         <v>15</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>114</v>
+      <c r="D95" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="E95" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2719,14 +2646,14 @@
       <c r="C96" t="s">
         <v>15</v>
       </c>
-      <c r="D96" s="3" t="s">
-        <v>115</v>
+      <c r="D96" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="E96" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>66</v>
       </c>
@@ -2736,8 +2663,14 @@
       <c r="C97" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D97" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E97" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>66</v>
       </c>
@@ -2747,8 +2680,14 @@
       <c r="C98" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D98" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E98" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>66</v>
       </c>
@@ -2758,8 +2697,14 @@
       <c r="C99" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D99" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E99" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>66</v>
       </c>
@@ -2769,6 +2714,12 @@
       <c r="C100" t="s">
         <v>15</v>
       </c>
+      <c r="D100" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E100" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
@@ -2780,8 +2731,14 @@
       <c r="C101" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D101" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E101" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>66</v>
       </c>
@@ -2791,6 +2748,12 @@
       <c r="C102" t="s">
         <v>15</v>
       </c>
+      <c r="D102" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E102" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
@@ -2803,38 +2766,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>66</v>
+      </c>
+      <c r="B104" t="s">
+        <v>97</v>
+      </c>
+      <c r="C104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>66</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C105" t="s">
         <v>15</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E105" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>66</v>
       </c>
       <c r="B106" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C106" t="s">
         <v>15</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E106" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -2842,16 +2804,10 @@
         <v>66</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C107" t="s">
         <v>15</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E107" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2859,50 +2815,24 @@
         <v>66</v>
       </c>
       <c r="B108" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C108" t="s">
         <v>15</v>
       </c>
-      <c r="E108" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>66</v>
       </c>
       <c r="B109" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C109" t="s">
         <v>15</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E109" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>66</v>
-      </c>
-      <c r="B110" t="s">
-        <v>116</v>
-      </c>
-      <c r="C110" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E110" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>66</v>
       </c>
@@ -2912,11 +2842,14 @@
       <c r="C111" t="s">
         <v>15</v>
       </c>
+      <c r="D111" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E111" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>66</v>
       </c>
@@ -2927,13 +2860,13 @@
         <v>15</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E112" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>66</v>
       </c>
@@ -2944,13 +2877,13 @@
         <v>15</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="E113" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>66</v>
       </c>
@@ -2960,11 +2893,8 @@
       <c r="C114" t="s">
         <v>15</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="E114" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2978,10 +2908,10 @@
         <v>15</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E115" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2995,13 +2925,13 @@
         <v>15</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E116" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>66</v>
       </c>
@@ -3011,14 +2941,11 @@
       <c r="C117" t="s">
         <v>15</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="E117" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>66</v>
       </c>
@@ -3029,13 +2956,13 @@
         <v>15</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E118" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>66</v>
       </c>
@@ -3046,13 +2973,13 @@
         <v>15</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E119" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>66</v>
       </c>
@@ -3062,173 +2989,182 @@
       <c r="C120" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D120" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E120" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>66</v>
+      </c>
+      <c r="B121" t="s">
+        <v>116</v>
+      </c>
+      <c r="C121" t="s">
+        <v>15</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E121" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B122" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C122" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="E122" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B123" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C123" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>126</v>
+        <v>140</v>
+      </c>
+      <c r="E123" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B124" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C124" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="E124" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B125" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C125" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E125" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>66</v>
+      </c>
+      <c r="B126" t="s">
+        <v>116</v>
+      </c>
+      <c r="C126" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>16</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B128" t="s">
         <v>16</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C128" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+      <c r="D128" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>16</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B129" t="s">
         <v>16</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C129" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D129" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C130" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E130" t="s">
-        <v>89</v>
-      </c>
-      <c r="F130" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C131" t="s">
-        <v>12</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C132" t="s">
-        <v>8</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E132" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C133" t="s">
-        <v>8</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>3</v>
-      </c>
-      <c r="B134" t="s">
-        <v>91</v>
-      </c>
-      <c r="C134" t="s">
-        <v>8</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>3</v>
-      </c>
-      <c r="B135" t="s">
-        <v>4</v>
-      </c>
-      <c r="C135" t="s">
-        <v>8</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3239,10 +3175,16 @@
         <v>4</v>
       </c>
       <c r="C136" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="E136" t="s">
+        <v>89</v>
+      </c>
+      <c r="F136" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3253,10 +3195,27 @@
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>36</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>3</v>
+      </c>
+      <c r="B138" t="s">
+        <v>4</v>
+      </c>
+      <c r="C138" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E138" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3264,13 +3223,13 @@
         <v>3</v>
       </c>
       <c r="B139" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3278,13 +3237,13 @@
         <v>3</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C140" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3292,13 +3251,13 @@
         <v>3</v>
       </c>
       <c r="B141" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3306,13 +3265,13 @@
         <v>3</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3320,59 +3279,129 @@
         <v>3</v>
       </c>
       <c r="B143" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C143" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>3</v>
-      </c>
-      <c r="B144" t="s">
-        <v>5</v>
-      </c>
-      <c r="C144" t="s">
-        <v>11</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145" t="s">
+        <v>40</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>3</v>
       </c>
       <c r="B146" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="C146" t="s">
+        <v>12</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" t="s">
+        <v>8</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148" t="s">
+        <v>8</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149" t="s">
+        <v>10</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
+        <v>3</v>
+      </c>
+      <c r="B150" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150" t="s">
+        <v>11</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>3</v>
+      </c>
+      <c r="B152" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3389,8 +3418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B719F-1470-4AFA-970E-2998AD817A19}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3444,11 +3473,9 @@
       <c r="B4" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3459,21 +3486,21 @@
         <v>116</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>166</v>
       </c>
       <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3481,13 +3508,13 @@
         <v>166</v>
       </c>
       <c r="B7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3495,10 +3522,10 @@
         <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3506,13 +3533,11 @@
         <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>183</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="C9" s="9"/>
       <c r="D9" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3520,41 +3545,39 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>186</v>
-      </c>
+      <c r="C11" s="10"/>
       <c r="D11" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>188</v>
+        <v>173</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
         <v>80</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3568,7 +3591,7 @@
         <v>116</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -3576,7 +3599,7 @@
         <v>116</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>195</v>
+        <v>273</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3585,57 +3608,57 @@
     </row>
     <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B20" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" t="s">
         <v>194</v>
       </c>
-      <c r="B21" t="s">
-        <v>200</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B22" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3643,24 +3666,24 @@
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3671,13 +3694,13 @@
         <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3688,7 +3711,7 @@
         <v>170</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3696,13 +3719,13 @@
         <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C29" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -3710,13 +3733,13 @@
         <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C30" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -3724,13 +3747,13 @@
         <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>188</v>
+        <v>173</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3738,10 +3761,10 @@
         <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3749,13 +3772,13 @@
         <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C33" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3769,74 +3792,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B39" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>214</v>
+      </c>
+      <c r="B40" t="s">
         <v>220</v>
       </c>
-      <c r="B40" t="s">
-        <v>226</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B41" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B42" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B43" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3844,39 +3867,39 @@
     </row>
     <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>228</v>
+      </c>
+      <c r="B45" t="s">
+        <v>229</v>
+      </c>
+      <c r="C45" t="s">
+        <v>206</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="B45" t="s">
-        <v>235</v>
-      </c>
-      <c r="C45" t="s">
-        <v>212</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B46" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C46" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B47" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C47" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
Spec File Rename (#1140)
- Repathed the root folder that the Regression Tests are in
- Runs tests based on Glob pattern for the new Regression Test folder
- Renamed some of the Spec Files
- Fixed a bug
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EF505E-561B-472A-A211-B883672C5EE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B762853-3719-4A33-8467-D6AEA1043DC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="274">
   <si>
     <t>Page</t>
   </si>
@@ -547,9 +547,6 @@
     <t>DisqualifyingEntities</t>
   </si>
   <si>
-    <t>EntitiesAffectActionScoring</t>
-  </si>
-  <si>
     <t>Creates a model with Actions that can be disqualified in scoring by Disqualifying, Expected and Required Entities</t>
   </si>
   <si>
@@ -559,29 +556,6 @@
     <t>TagAndFrog</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ConsistentEntityLabeling</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-EntityLabeling</t>
-    </r>
-  </si>
-  <si>
     <t>Creates a model to be used to validate that consistent Entity labeling is enforced by the UI</t>
   </si>
   <si>
@@ -603,38 +577,15 @@
     <t>WhatsYourName</t>
   </si>
   <si>
-    <t>TextEntityAndActions</t>
-  </si>
-  <si>
     <t>Creates a model with a "name" entity and two simple actions; "What's your name" and "Hello $name"</t>
   </si>
   <si>
     <t>EditAndBranching</t>
   </si>
   <si>
-    <t>BasicBranching
-SimpleBranching</t>
-  </si>
-  <si>
     <t>Test the basic Train Dialog branching feature and verifies that the original dialog does not change and that the branched dialog is persisted correctly.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">ConsistentEntityLabeling
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EntityLabeling</t>
-    </r>
-  </si>
-  <si>
     <t>Verifies that the user cannot modify training such that entity labeling would become inconsistent.</t>
   </si>
   <si>
@@ -653,9 +604,6 @@
     <t>ErrorHandling</t>
   </si>
   <si>
-    <t>(more tests planed based on bugs reports)</t>
-  </si>
-  <si>
     <t>ActionUnavailable</t>
   </si>
   <si>
@@ -716,9 +664,6 @@
     <t>Verifies that Score Actions comes up again after selecting a Non-Wait Action and that the user is prompted to type in a message after a Wait Action is selected.</t>
   </si>
   <si>
-    <t>Verifies automatic Expected Entity labeling occurs.</t>
-  </si>
-  <si>
     <t>ExpectedEntityLabeling</t>
   </si>
   <si>
@@ -791,9 +736,6 @@
     <t>Verifies Train Dialog starts off with No Tags nor Descriptions. Verifies that adding Tags and Descriptions to Train Dialog and saving them results in them showing up in the grid. Verifies that editing Train Dialog shows the persisted T&amp;D. Verifies that changes made to T&amp;D are discarded when the Train Dialog is abandonded. Verifies that editing a Train Dialog and adding a new tag and modifying the description is persisted whtn the dialog is saved and reloaded. There are more steps that modify the T&amp;D, delete a turn, save, edit again, add more rounds, and finally verify the T&amp;Ds again. Branching and T&amp;D modifications verified after saving.</t>
   </si>
   <si>
-    <t>A very simple test of Log Dialogs with 2 rounds. Basically the same thing the loop test does without the loop.</t>
-  </si>
-  <si>
     <t>Rename</t>
   </si>
   <si>
@@ -879,6 +821,49 @@
   </si>
   <si>
     <t>Verify that you can delete an Action that is not used by a Train Dialog by simply confirming that you want to delete it without a warning poping up.</t>
+  </si>
+  <si>
+    <t>Add Turn</t>
+  </si>
+  <si>
+    <t>Edit a turn, verify "Submit Changes" and "Undo" button is disabled. Change entity label, verify "Submit Changes" and "Undo" buttons become enabled.
+Variations from here:
+1) Submit - verify expectation
+2) Undo - verify returns to original state
+3) Select a different User Turn - verify it asks to save changes - yes verify - no verify those buttons are disabled and returns to original state just like undo (bug 2074)
+4) Select a different Bot Turn - verify same as #3 (bug 2075)</t>
+  </si>
+  <si>
+    <t>Add a new user turn to new or exiting Train Dialog (at User turn 2 and beyond) and "Undo" button should show up.
+Variations from here:
+1) Undo - verify
+2) Score Actions - verify - this is the most common path and is verified in many places
+3) Abandon - verify 
+4) Verify cannot click on to edit any other existing turn</t>
+  </si>
+  <si>
+    <t>Entity labeling from ConsistentEntityLabeling tests</t>
+  </si>
+  <si>
+    <t>TODO new case for when something was not labeled and now it is</t>
+  </si>
+  <si>
+    <t>******</t>
+  </si>
+  <si>
+    <t>EntityLabeling</t>
+  </si>
+  <si>
+    <t>ConsistentEntityLabeling</t>
+  </si>
+  <si>
+    <t>(more tests planed based on bug reports)</t>
+  </si>
+  <si>
+    <t>Verifies that automatic Expected Entity labeling occurs.</t>
+  </si>
+  <si>
+    <t>A very simple test of Log Dialogs with 2 rounds. Basically the same test as the LoopYourName test without the loop.</t>
   </si>
 </sst>
 </file>
@@ -1010,8 +995,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F150" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F150" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F156" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F156" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
@@ -1321,11 +1306,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1520,13 +1505,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1534,13 +1519,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1548,13 +1533,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1562,13 +1547,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1576,13 +1561,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1590,13 +1575,13 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,7 +1612,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1641,7 +1626,7 @@
         <v>39</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1655,7 +1640,7 @@
         <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1669,7 +1654,7 @@
         <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1683,7 +1668,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1697,7 +1682,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1711,7 +1696,7 @@
         <v>39</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1725,7 +1710,7 @@
         <v>39</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1733,13 +1718,13 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1747,13 +1732,13 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1761,13 +1746,13 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1885,13 +1870,13 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1899,13 +1884,13 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1913,13 +1898,13 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1927,13 +1912,13 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2242,41 +2227,35 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>58</v>
+        <v>263</v>
       </c>
       <c r="C66" t="s">
         <v>15</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E66" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>58</v>
-      </c>
-      <c r="C67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2287,10 +2266,10 @@
         <v>15</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E68" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2304,13 +2283,13 @@
         <v>15</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E69" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -2321,7 +2300,7 @@
         <v>15</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E70" t="s">
         <v>58</v>
@@ -2338,7 +2317,10 @@
         <v>15</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="E71" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2352,13 +2334,13 @@
         <v>15</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E72" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>66</v>
       </c>
@@ -2369,10 +2351,7 @@
         <v>15</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E73" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2386,10 +2365,10 @@
         <v>15</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E74" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2403,13 +2382,13 @@
         <v>15</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="E75" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>66</v>
       </c>
@@ -2420,7 +2399,10 @@
         <v>15</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="E76" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2434,13 +2416,13 @@
         <v>15</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F77" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="E77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>66</v>
       </c>
@@ -2451,7 +2433,24 @@
         <v>15</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F79" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,33 +2458,13 @@
         <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C80" t="s">
         <v>15</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E80" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>66</v>
-      </c>
-      <c r="B81" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E81" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2499,112 +2478,60 @@
         <v>15</v>
       </c>
       <c r="D82" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>66</v>
+      </c>
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" t="s">
+        <v>82</v>
+      </c>
+      <c r="C84" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E84" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>66</v>
-      </c>
-      <c r="B84" t="s">
-        <v>97</v>
-      </c>
-      <c r="C84" t="s">
-        <v>13</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E84" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>66</v>
-      </c>
-      <c r="B85" t="s">
-        <v>97</v>
-      </c>
-      <c r="C85" t="s">
-        <v>13</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E85" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>66</v>
-      </c>
-      <c r="B86" t="s">
-        <v>97</v>
-      </c>
-      <c r="C86" t="s">
-        <v>13</v>
+        <v>268</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E86" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>66</v>
-      </c>
-      <c r="B87" t="s">
-        <v>97</v>
-      </c>
-      <c r="C87" t="s">
-        <v>15</v>
+        <v>268</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E87" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>66</v>
-      </c>
-      <c r="B88" t="s">
-        <v>97</v>
-      </c>
-      <c r="C88" t="s">
-        <v>15</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E88" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>66</v>
-      </c>
-      <c r="B89" t="s">
-        <v>97</v>
-      </c>
-      <c r="C89" t="s">
-        <v>15</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E89" t="s">
-        <v>105</v>
+        <v>267</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2615,16 +2542,16 @@
         <v>97</v>
       </c>
       <c r="C90" t="s">
-        <v>15</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>106</v>
+        <v>13</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="E90" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>66</v>
       </c>
@@ -2632,13 +2559,13 @@
         <v>97</v>
       </c>
       <c r="C91" t="s">
-        <v>15</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>107</v>
+        <v>13</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="E91" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2649,13 +2576,13 @@
         <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>15</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>109</v>
+        <v>13</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="E92" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2668,11 +2595,11 @@
       <c r="C93" t="s">
         <v>15</v>
       </c>
-      <c r="D93" s="4" t="s">
-        <v>113</v>
+      <c r="D93" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="E93" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2685,14 +2612,14 @@
       <c r="C94" t="s">
         <v>15</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>112</v>
+      <c r="D94" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="E94" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>66</v>
       </c>
@@ -2702,11 +2629,11 @@
       <c r="C95" t="s">
         <v>15</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>114</v>
+      <c r="D95" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="E95" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2719,14 +2646,14 @@
       <c r="C96" t="s">
         <v>15</v>
       </c>
-      <c r="D96" s="3" t="s">
-        <v>115</v>
+      <c r="D96" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="E96" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>66</v>
       </c>
@@ -2736,8 +2663,14 @@
       <c r="C97" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D97" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E97" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>66</v>
       </c>
@@ -2747,8 +2680,14 @@
       <c r="C98" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D98" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E98" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>66</v>
       </c>
@@ -2758,8 +2697,14 @@
       <c r="C99" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D99" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E99" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>66</v>
       </c>
@@ -2769,6 +2714,12 @@
       <c r="C100" t="s">
         <v>15</v>
       </c>
+      <c r="D100" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E100" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
@@ -2780,8 +2731,14 @@
       <c r="C101" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D101" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E101" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>66</v>
       </c>
@@ -2791,6 +2748,12 @@
       <c r="C102" t="s">
         <v>15</v>
       </c>
+      <c r="D102" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E102" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
@@ -2803,38 +2766,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>66</v>
+      </c>
+      <c r="B104" t="s">
+        <v>97</v>
+      </c>
+      <c r="C104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>66</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C105" t="s">
         <v>15</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E105" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>66</v>
       </c>
       <c r="B106" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C106" t="s">
         <v>15</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E106" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -2842,16 +2804,10 @@
         <v>66</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C107" t="s">
         <v>15</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E107" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2859,50 +2815,24 @@
         <v>66</v>
       </c>
       <c r="B108" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C108" t="s">
         <v>15</v>
       </c>
-      <c r="E108" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>66</v>
       </c>
       <c r="B109" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C109" t="s">
         <v>15</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E109" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>66</v>
-      </c>
-      <c r="B110" t="s">
-        <v>116</v>
-      </c>
-      <c r="C110" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E110" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>66</v>
       </c>
@@ -2912,11 +2842,14 @@
       <c r="C111" t="s">
         <v>15</v>
       </c>
+      <c r="D111" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E111" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>66</v>
       </c>
@@ -2927,13 +2860,13 @@
         <v>15</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E112" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>66</v>
       </c>
@@ -2944,13 +2877,13 @@
         <v>15</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="E113" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>66</v>
       </c>
@@ -2960,11 +2893,8 @@
       <c r="C114" t="s">
         <v>15</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="E114" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2978,10 +2908,10 @@
         <v>15</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E115" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2995,13 +2925,13 @@
         <v>15</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E116" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>66</v>
       </c>
@@ -3011,14 +2941,11 @@
       <c r="C117" t="s">
         <v>15</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="E117" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>66</v>
       </c>
@@ -3029,13 +2956,13 @@
         <v>15</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E118" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>66</v>
       </c>
@@ -3046,13 +2973,13 @@
         <v>15</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E119" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>66</v>
       </c>
@@ -3062,173 +2989,182 @@
       <c r="C120" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D120" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E120" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>66</v>
+      </c>
+      <c r="B121" t="s">
+        <v>116</v>
+      </c>
+      <c r="C121" t="s">
+        <v>15</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E121" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B122" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C122" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="E122" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B123" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C123" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>126</v>
+        <v>140</v>
+      </c>
+      <c r="E123" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B124" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C124" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="E124" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B125" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C125" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E125" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>66</v>
+      </c>
+      <c r="B126" t="s">
+        <v>116</v>
+      </c>
+      <c r="C126" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>16</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B128" t="s">
         <v>16</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C128" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+      <c r="D128" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>16</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B129" t="s">
         <v>16</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C129" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D129" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C130" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E130" t="s">
-        <v>89</v>
-      </c>
-      <c r="F130" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C131" t="s">
-        <v>12</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C132" t="s">
-        <v>8</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E132" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C133" t="s">
-        <v>8</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>3</v>
-      </c>
-      <c r="B134" t="s">
-        <v>91</v>
-      </c>
-      <c r="C134" t="s">
-        <v>8</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>3</v>
-      </c>
-      <c r="B135" t="s">
-        <v>4</v>
-      </c>
-      <c r="C135" t="s">
-        <v>8</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3239,10 +3175,16 @@
         <v>4</v>
       </c>
       <c r="C136" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="E136" t="s">
+        <v>89</v>
+      </c>
+      <c r="F136" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3253,10 +3195,27 @@
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>36</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>3</v>
+      </c>
+      <c r="B138" t="s">
+        <v>4</v>
+      </c>
+      <c r="C138" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E138" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3264,13 +3223,13 @@
         <v>3</v>
       </c>
       <c r="B139" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3278,13 +3237,13 @@
         <v>3</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C140" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3292,13 +3251,13 @@
         <v>3</v>
       </c>
       <c r="B141" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3306,13 +3265,13 @@
         <v>3</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3320,59 +3279,129 @@
         <v>3</v>
       </c>
       <c r="B143" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C143" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>3</v>
-      </c>
-      <c r="B144" t="s">
-        <v>5</v>
-      </c>
-      <c r="C144" t="s">
-        <v>11</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145" t="s">
+        <v>40</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>3</v>
       </c>
       <c r="B146" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="C146" t="s">
+        <v>12</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" t="s">
+        <v>8</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148" t="s">
+        <v>8</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149" t="s">
+        <v>10</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
+        <v>3</v>
+      </c>
+      <c r="B150" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150" t="s">
+        <v>11</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>3</v>
+      </c>
+      <c r="B152" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3389,8 +3418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B719F-1470-4AFA-970E-2998AD817A19}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3444,11 +3473,9 @@
       <c r="B4" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3459,21 +3486,21 @@
         <v>116</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>166</v>
       </c>
       <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3481,13 +3508,13 @@
         <v>166</v>
       </c>
       <c r="B7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3495,10 +3522,10 @@
         <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3506,13 +3533,11 @@
         <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>183</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="C9" s="9"/>
       <c r="D9" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3520,41 +3545,39 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>186</v>
-      </c>
+      <c r="C11" s="10"/>
       <c r="D11" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>188</v>
+        <v>173</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
         <v>80</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3568,7 +3591,7 @@
         <v>116</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -3576,7 +3599,7 @@
         <v>116</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>195</v>
+        <v>271</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3585,57 +3608,57 @@
     </row>
     <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B20" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" t="s">
         <v>194</v>
       </c>
-      <c r="B21" t="s">
-        <v>200</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B22" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3643,24 +3666,24 @@
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>241</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3671,13 +3694,13 @@
         <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3688,7 +3711,7 @@
         <v>170</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3696,13 +3719,13 @@
         <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
-      </c>
-      <c r="C29" t="s">
-        <v>211</v>
+        <v>202</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -3710,13 +3733,13 @@
         <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>209</v>
-      </c>
-      <c r="C30" t="s">
-        <v>212</v>
+        <v>203</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -3724,13 +3747,13 @@
         <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>188</v>
+        <v>173</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3738,10 +3761,10 @@
         <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3749,13 +3772,13 @@
         <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
-      </c>
-      <c r="C33" t="s">
-        <v>217</v>
+        <v>180</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>216</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3769,74 +3792,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B39" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>213</v>
+      </c>
+      <c r="B40" t="s">
+        <v>219</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="B40" t="s">
-        <v>226</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B41" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B42" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B43" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3844,39 +3867,39 @@
     </row>
     <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B45" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C45" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B46" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C46" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B47" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C47" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: update test grid to show new names and old names
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B762853-3719-4A33-8467-D6AEA1043DC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9721F1-D051-4FE7-9280-0D052B1720C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="272">
   <si>
     <t>Page</t>
   </si>
@@ -526,9 +526,6 @@
     <t>Current Test Name</t>
   </si>
   <si>
-    <t>AlternativeSuggestions</t>
-  </si>
-  <si>
     <t>Test Description</t>
   </si>
   <si>
@@ -724,13 +721,7 @@
     <t>entityConflicts</t>
   </si>
   <si>
-    <t>EntityConflicts</t>
-  </si>
-  <si>
     <t>entityPicker</t>
-  </si>
-  <si>
-    <t>EntityPicker</t>
   </si>
   <si>
     <t>Verifies Train Dialog starts off with No Tags nor Descriptions. Verifies that adding Tags and Descriptions to Train Dialog and saving them results in them showing up in the grid. Verifies that editing Train Dialog shows the persisted T&amp;D. Verifies that changes made to T&amp;D are discarded when the Train Dialog is abandonded. Verifies that editing a Train Dialog and adding a new tag and modifying the description is persisted whtn the dialog is saved and reloaded. There are more steps that modify the T&amp;D, delete a turn, save, edit again, add more rounds, and finally verify the T&amp;Ds again. Branching and T&amp;D modifications verified after saving.</t>
@@ -864,6 +855,9 @@
   </si>
   <si>
     <t>A very simple test of Log Dialogs with 2 rounds. Basically the same test as the LoopYourName test without the loop.</t>
+  </si>
+  <si>
+    <t>Old Test Name</t>
   </si>
 </sst>
 </file>
@@ -940,7 +934,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -961,9 +955,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1505,13 +1496,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1519,13 +1510,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1533,13 +1524,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1547,13 +1538,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1561,13 +1552,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1575,13 +1566,13 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1612,7 +1603,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1626,7 +1617,7 @@
         <v>39</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1640,7 +1631,7 @@
         <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1654,7 +1645,7 @@
         <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1668,7 +1659,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1682,7 +1673,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1696,7 +1687,7 @@
         <v>39</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1710,7 +1701,7 @@
         <v>39</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1718,13 +1709,13 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1732,13 +1723,13 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1746,13 +1737,13 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1870,13 +1861,13 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1884,13 +1875,13 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1898,13 +1889,13 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1912,13 +1903,13 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2238,7 +2229,7 @@
         <v>15</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2246,13 +2237,13 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C66" t="s">
         <v>15</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2520,18 +2511,18 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -3418,8 +3409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B719F-1470-4AFA-970E-2998AD817A19}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3438,106 +3429,105 @@
         <v>163</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>116</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3545,39 +3535,38 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="10"/>
       <c r="D11" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>270</v>
+        <v>181</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" t="s">
+        <v>172</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
         <v>80</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3591,15 +3580,15 @@
         <v>116</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>271</v>
+      <c r="B16" s="10" t="s">
+        <v>268</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3608,57 +3597,57 @@
     </row>
     <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" t="s">
         <v>189</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3666,24 +3655,24 @@
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" t="s">
         <v>198</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3693,92 +3682,92 @@
       <c r="A27" t="s">
         <v>66</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" t="s">
+        <v>185</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>66</v>
       </c>
-      <c r="B28" t="s">
-        <v>170</v>
+      <c r="C28" t="s">
+        <v>169</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" t="s">
-        <v>202</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>205</v>
+      <c r="B29" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C29" t="s">
+        <v>201</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>66</v>
       </c>
-      <c r="B30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="B30" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s">
-        <v>173</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>270</v>
+      <c r="B31" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C31" t="s">
+        <v>172</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>66</v>
       </c>
-      <c r="B32" t="s">
-        <v>178</v>
+      <c r="C32" t="s">
+        <v>177</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>66</v>
       </c>
-      <c r="B33" t="s">
-        <v>180</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>210</v>
+      <c r="B33" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" t="s">
+        <v>179</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3792,74 +3781,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>212</v>
+      </c>
+      <c r="B38" t="s">
         <v>213</v>
       </c>
-      <c r="B38" t="s">
-        <v>214</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B39" t="s">
+        <v>216</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B40" t="s">
+        <v>218</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B41" t="s">
+        <v>220</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B42" t="s">
+        <v>222</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B43" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3867,39 +3856,30 @@
     </row>
     <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>226</v>
+      </c>
+      <c r="B45" t="s">
         <v>227</v>
       </c>
-      <c r="B45" t="s">
-        <v>228</v>
-      </c>
-      <c r="C45" t="s">
-        <v>206</v>
-      </c>
       <c r="D45" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B46" t="s">
-        <v>229</v>
-      </c>
-      <c r="C46" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B47" t="s">
-        <v>231</v>
-      </c>
-      <c r="C47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: create entities for all resolver types multivalue and negatable
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9721F1-D051-4FE7-9280-0D052B1720C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9203FC-4AF2-48A4-A304-3B5456A43DF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="272">
   <si>
     <t>Page</t>
   </si>
@@ -503,18 +503,6 @@
   </si>
   <si>
     <t>Can create a programatic multivalued entity</t>
-  </si>
-  <si>
-    <t>Can create custom trained entity with each resolver type</t>
-  </si>
-  <si>
-    <t>Can create a pretrained entity of each type</t>
-  </si>
-  <si>
-    <t>Can create a pretrained multivalued entity of each type</t>
-  </si>
-  <si>
-    <t>CreateModels\AllEntityTypes</t>
   </si>
   <si>
     <t>New Entity</t>
@@ -858,6 +846,18 @@
   </si>
   <si>
     <t>Old Test Name</t>
+  </si>
+  <si>
+    <t>CreateModels/AllEntityTypes, CreateModels/EntityLabeling</t>
+  </si>
+  <si>
+    <t>CreateModels/AllEntityTypes</t>
+  </si>
+  <si>
+    <t>Can create custom trained entity with each resolver type, with and without multivalued and negatable</t>
+  </si>
+  <si>
+    <t>Can create a pretrained entity of each type with and without multivalued</t>
   </si>
 </sst>
 </file>
@@ -1299,9 +1299,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1341,7 +1341,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
@@ -1355,7 +1355,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -1363,13 +1363,16 @@
       <c r="D3" s="3" t="s">
         <v>154</v>
       </c>
+      <c r="E3" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
@@ -1378,7 +1381,7 @@
         <v>151</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1386,7 +1389,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -1395,7 +1398,7 @@
         <v>152</v>
       </c>
       <c r="E5" t="s">
-        <v>160</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1403,7 +1406,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -1411,19 +1414,25 @@
       <c r="D6" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>157</v>
+        <v>270</v>
+      </c>
+      <c r="E7" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1431,7 +1440,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -1440,7 +1449,7 @@
         <v>155</v>
       </c>
       <c r="E8" t="s">
-        <v>160</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1448,7 +1457,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -1457,7 +1466,7 @@
         <v>156</v>
       </c>
       <c r="E9" t="s">
-        <v>160</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1465,30 +1474,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>158</v>
+        <v>271</v>
       </c>
       <c r="E10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>159</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1496,13 +1491,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1510,13 +1505,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1524,13 +1519,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1538,13 +1533,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1552,13 +1547,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1566,13 +1561,13 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1603,7 +1598,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1617,7 +1612,7 @@
         <v>39</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1631,7 +1626,7 @@
         <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1645,7 +1640,7 @@
         <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1659,7 +1654,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1673,7 +1668,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1687,7 +1682,7 @@
         <v>39</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1701,7 +1696,7 @@
         <v>39</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1709,13 +1704,13 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1723,13 +1718,13 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1737,13 +1732,13 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1861,13 +1856,13 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1875,13 +1870,13 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1889,13 +1884,13 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1903,13 +1898,13 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2229,7 +2224,7 @@
         <v>15</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2237,13 +2232,13 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C66" t="s">
         <v>15</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2511,18 +2506,18 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -3409,8 +3404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B719F-1470-4AFA-970E-2998AD817A19}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3423,111 +3418,111 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
         <v>165</v>
-      </c>
-      <c r="B4" t="s">
-        <v>169</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
         <v>116</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3535,38 +3530,38 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B13" t="s">
         <v>80</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3580,7 +3575,7 @@
         <v>116</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -3588,7 +3583,7 @@
         <v>116</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3597,57 +3592,57 @@
     </row>
     <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" t="s">
         <v>188</v>
       </c>
-      <c r="B20" t="s">
-        <v>192</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3655,24 +3650,24 @@
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B24" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3683,13 +3678,13 @@
         <v>66</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C27" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3697,10 +3692,10 @@
         <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3708,13 +3703,13 @@
         <v>66</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C29" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -3722,13 +3717,13 @@
         <v>66</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -3736,13 +3731,13 @@
         <v>66</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C31" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3750,10 +3745,10 @@
         <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3761,13 +3756,13 @@
         <v>66</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C33" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3781,74 +3776,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B38" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>208</v>
+      </c>
+      <c r="B39" t="s">
         <v>212</v>
       </c>
-      <c r="B39" t="s">
-        <v>216</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B40" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B41" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B42" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B43" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3856,30 +3851,30 @@
     </row>
     <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>222</v>
+      </c>
+      <c r="B45" t="s">
+        <v>223</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="B45" t="s">
-        <v>227</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B46" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B47" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: added action type validation
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9203FC-4AF2-48A4-A304-3B5456A43DF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3E5B66-286D-4347-9151-B28FE8520935}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -160,9 +160,6 @@
     <t>All Train tests</t>
   </si>
   <si>
-    <t>All CreateModels tests (todo)</t>
-  </si>
-  <si>
     <t>Michael manually does this on a regular basis</t>
   </si>
   <si>
@@ -858,6 +855,9 @@
   </si>
   <si>
     <t>Can create a pretrained entity of each type with and without multivalued</t>
+  </si>
+  <si>
+    <t>CreateModels/DateTimeResolver, CreateModels/DisqualifyingEntities, CreateModels/EndSession, CreateModels/EntityLabeling, CreateModels/WaitVsNoWaitAction, CreateModels/WhatsYourName</t>
   </si>
 </sst>
 </file>
@@ -961,7 +961,10 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -986,14 +989,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F156" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F156" totalsRowShown="0" headerRowBorderDxfId="2" headerRowCellStyle="Heading 1">
   <autoFilter ref="A1:F156" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
     <tableColumn id="2" xr3:uid="{B0123158-48C7-47B5-8788-3102666127B5}" name="Page"/>
-    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name"/>
+    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1299,9 +1302,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,7 +1313,7 @@
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.6640625" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" customWidth="1"/>
     <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
@@ -1329,11 +1332,11 @@
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1341,7 +1344,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
@@ -1355,16 +1358,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E3" t="s">
-        <v>269</v>
+        <v>153</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1372,16 +1375,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" t="s">
-        <v>268</v>
+        <v>150</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1389,16 +1392,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" t="s">
-        <v>269</v>
+        <v>151</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1406,16 +1409,16 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" t="s">
-        <v>269</v>
+        <v>152</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1423,16 +1426,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="E7" t="s">
         <v>269</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1440,16 +1443,16 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E8" t="s">
-        <v>269</v>
+        <v>154</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1457,16 +1460,16 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E9" t="s">
-        <v>269</v>
+        <v>155</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1474,16 +1477,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="E10" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1491,13 +1494,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1505,13 +1508,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1519,13 +1522,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1533,13 +1536,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1547,13 +1550,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1561,16 +1564,16 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1583,8 +1586,8 @@
       <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
-        <v>42</v>
+      <c r="E19" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1598,7 +1601,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1612,7 +1615,7 @@
         <v>39</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1626,7 +1629,7 @@
         <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1640,7 +1643,7 @@
         <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1654,7 +1657,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1668,7 +1671,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1682,7 +1685,7 @@
         <v>39</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1696,7 +1699,7 @@
         <v>39</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1704,13 +1707,13 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1718,13 +1721,13 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1732,13 +1735,13 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1754,7 +1757,7 @@
       <c r="D32" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1771,8 +1774,8 @@
       <c r="D33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E33" t="s">
-        <v>95</v>
+      <c r="E33" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1817,7 +1820,7 @@
         <v>31</v>
       </c>
       <c r="F36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1833,8 +1836,8 @@
       <c r="D37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E37" t="s">
-        <v>96</v>
+      <c r="E37" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1848,7 +1851,7 @@
         <v>18</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1856,13 +1859,13 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1870,13 +1873,13 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1884,13 +1887,13 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1898,855 +1901,855 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E45" t="s">
-        <v>144</v>
+        <v>123</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E46" t="s">
-        <v>144</v>
+        <v>46</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E47" t="s">
-        <v>144</v>
+        <v>47</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E48" t="s">
-        <v>144</v>
+        <v>48</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C49" t="s">
-        <v>44</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E49" t="s">
-        <v>149</v>
+      <c r="E49" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E50" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
         <v>45</v>
       </c>
-      <c r="B51" t="s">
-        <v>46</v>
-      </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E51" t="s">
-        <v>145</v>
+        <v>50</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E52" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E54" t="s">
-        <v>141</v>
+        <v>142</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E55" t="s">
-        <v>57</v>
+        <v>124</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" t="s">
-        <v>80</v>
+        <v>70</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B58" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C58" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E58" t="s">
-        <v>80</v>
+      <c r="E58" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
       </c>
       <c r="D59" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E59" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E60" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E61" t="s">
-        <v>80</v>
+        <v>71</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E62" t="s">
-        <v>136</v>
+        <v>82</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E63" t="s">
-        <v>117</v>
+        <v>83</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
         <v>15</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C66" t="s">
         <v>15</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
+        <v>57</v>
+      </c>
+      <c r="C68" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C68" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E68" t="s">
-        <v>80</v>
+      <c r="E68" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C69" t="s">
         <v>15</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E69" t="s">
-        <v>80</v>
+        <v>72</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C70" t="s">
         <v>15</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E70" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C71" t="s">
         <v>15</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E71" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C72" t="s">
         <v>15</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E72" t="s">
-        <v>58</v>
+        <v>80</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C73" t="s">
         <v>15</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C74" t="s">
         <v>15</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E74" t="s">
-        <v>58</v>
+        <v>63</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C75" t="s">
         <v>15</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E75" t="s">
-        <v>58</v>
+        <v>73</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C76" t="s">
         <v>15</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E76" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C77" t="s">
         <v>15</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E77" t="s">
-        <v>80</v>
+        <v>60</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B78" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C78" t="s">
         <v>15</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>65</v>
+      </c>
+      <c r="B79" t="s">
+        <v>57</v>
+      </c>
+      <c r="C79" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B79" t="s">
-        <v>58</v>
-      </c>
-      <c r="C79" t="s">
-        <v>15</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B80" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C80" t="s">
         <v>15</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C82" t="s">
         <v>15</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E82" t="s">
         <v>85</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C83" t="s">
         <v>15</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E83" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C84" t="s">
         <v>15</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E84" t="s">
         <v>141</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B90" t="s">
+        <v>96</v>
+      </c>
+      <c r="C90" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C90" t="s">
-        <v>13</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E90" t="s">
-        <v>104</v>
+      <c r="E90" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C91" t="s">
         <v>13</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E91" t="s">
-        <v>104</v>
+        <v>98</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B92" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C92" t="s">
         <v>13</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E92" t="s">
-        <v>104</v>
+        <v>99</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C93" t="s">
         <v>15</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E93" t="s">
-        <v>104</v>
+        <v>100</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C94" t="s">
         <v>15</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E94" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B95" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C95" t="s">
         <v>15</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E95" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B96" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C96" t="s">
         <v>15</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E96" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C97" t="s">
         <v>15</v>
       </c>
       <c r="D97" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E97" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="E97" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C98" t="s">
         <v>15</v>
       </c>
       <c r="D98" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E98" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="E98" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C99" t="s">
         <v>15</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E99" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B100" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C100" t="s">
         <v>15</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E100" t="s">
         <v>111</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B101" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C101" t="s">
         <v>15</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E101" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B102" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C102" t="s">
         <v>15</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E102" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B103" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C103" t="s">
         <v>15</v>
@@ -2754,10 +2757,10 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B104" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C104" t="s">
         <v>15</v>
@@ -2765,10 +2768,10 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B105" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C105" t="s">
         <v>15</v>
@@ -2776,10 +2779,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B106" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C106" t="s">
         <v>15</v>
@@ -2787,10 +2790,10 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B107" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C107" t="s">
         <v>15</v>
@@ -2798,10 +2801,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B108" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C108" t="s">
         <v>15</v>
@@ -2809,10 +2812,10 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B109" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C109" t="s">
         <v>15</v>
@@ -2820,259 +2823,259 @@
     </row>
     <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B111" t="s">
+        <v>115</v>
+      </c>
+      <c r="C111" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E111" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C111" t="s">
-        <v>15</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E111" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C112" t="s">
         <v>15</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E112" t="s">
-        <v>131</v>
+        <v>120</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B113" t="s">
+        <v>115</v>
+      </c>
+      <c r="C113" t="s">
+        <v>15</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C113" t="s">
-        <v>15</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E113" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B114" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114" t="s">
+        <v>15</v>
+      </c>
+      <c r="E114" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C114" t="s">
-        <v>15</v>
-      </c>
-      <c r="E114" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B115" t="s">
+        <v>115</v>
+      </c>
+      <c r="C115" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E115" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C115" t="s">
-        <v>15</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E115" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C116" t="s">
         <v>15</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E116" t="s">
-        <v>131</v>
+        <v>134</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B117" t="s">
+        <v>115</v>
+      </c>
+      <c r="C117" t="s">
+        <v>15</v>
+      </c>
+      <c r="E117" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C117" t="s">
-        <v>15</v>
-      </c>
-      <c r="E117" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C118" t="s">
         <v>15</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E118" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B119" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C119" t="s">
         <v>15</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E119" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B120" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C120" t="s">
         <v>15</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E120" t="s">
         <v>131</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B121" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C121" t="s">
         <v>15</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E121" t="s">
         <v>122</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B122" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C122" t="s">
         <v>15</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E122" t="s">
         <v>129</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B123" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C123" t="s">
         <v>15</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E123" t="s">
-        <v>129</v>
+        <v>139</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B124" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C124" t="s">
         <v>15</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E124" t="s">
-        <v>131</v>
+        <v>138</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B125" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C125" t="s">
         <v>15</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E125" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B126" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C126" t="s">
         <v>15</v>
@@ -3089,7 +3092,7 @@
         <v>16</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3103,7 +3106,7 @@
         <v>16</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3117,7 +3120,7 @@
         <v>16</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3166,11 +3169,11 @@
       <c r="D136" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E136" t="s">
-        <v>89</v>
+      <c r="E136" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="F136" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3184,7 +3187,7 @@
         <v>12</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3200,8 +3203,8 @@
       <c r="D138" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E138" t="s">
-        <v>85</v>
+      <c r="E138" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3215,7 +3218,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3223,13 +3226,13 @@
         <v>3</v>
       </c>
       <c r="B140" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C140" t="s">
         <v>8</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3243,7 +3246,7 @@
         <v>8</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3368,7 +3371,7 @@
         <v>3</v>
       </c>
       <c r="B152" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -3418,111 +3421,111 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="C7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3530,38 +3533,38 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3569,21 +3572,21 @@
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3592,57 +3595,57 @@
     </row>
     <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" t="s">
         <v>184</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3650,24 +3653,24 @@
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" t="s">
         <v>193</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3675,94 +3678,94 @@
     </row>
     <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C27" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="C30" t="s">
-        <v>198</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3776,74 +3779,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" t="s">
         <v>208</v>
       </c>
-      <c r="B38" t="s">
-        <v>209</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B39" t="s">
+        <v>211</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B40" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B41" t="s">
+        <v>215</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B42" t="s">
+        <v>217</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B43" t="s">
+        <v>219</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3851,30 +3854,30 @@
     </row>
     <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>221</v>
+      </c>
+      <c r="B45" t="s">
         <v>222</v>
       </c>
-      <c r="B45" t="s">
-        <v>223</v>
-      </c>
       <c r="D45" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: update the test grid
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3E5B66-286D-4347-9151-B28FE8520935}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D07631-EE6B-455D-9992-80F263848CCF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="272">
   <si>
     <t>Page</t>
   </si>
@@ -100,27 +100,6 @@
     <t>Action shows up in grid with all expected values</t>
   </si>
   <si>
-    <t>Log shows up in grid with all expected values</t>
-  </si>
-  <si>
-    <t>Training shows up in grid with all expected values</t>
-  </si>
-  <si>
-    <t>Edit Log Dialog</t>
-  </si>
-  <si>
-    <t>New Log Dialog</t>
-  </si>
-  <si>
-    <t>New Train Dialog</t>
-  </si>
-  <si>
-    <t>Log shows up in train dialog grid with all expected values</t>
-  </si>
-  <si>
-    <t>Edit Train Dialog</t>
-  </si>
-  <si>
     <t>Shows up on home page grid and model page with all entities, actions, train dialogs and log dialogs</t>
   </si>
   <si>
@@ -316,9 +295,6 @@
     <t>Resolver Type</t>
   </si>
   <si>
-    <t>All Edit and Branching tests</t>
-  </si>
-  <si>
     <t>All Train and Edit and Branching tests</t>
   </si>
   <si>
@@ -739,25 +715,13 @@
     <t>Can create a TEXT Action</t>
   </si>
   <si>
-    <t>Validate all TEXT Action fields exist and user can set values</t>
-  </si>
-  <si>
     <t>Can create an API Action</t>
   </si>
   <si>
-    <t>Validate all API Action fields exist and user can set values</t>
-  </si>
-  <si>
     <t>Can create a CARD Action</t>
   </si>
   <si>
-    <t>Validate all CARD Action fields exist and user can set values</t>
-  </si>
-  <si>
     <t>Can create an END_SESSION Action</t>
-  </si>
-  <si>
-    <t>Validate all END_SESSION Action fields exist and user can set values</t>
   </si>
   <si>
     <t>Edit Action</t>
@@ -858,6 +822,42 @@
   </si>
   <si>
     <t>CreateModels/DateTimeResolver, CreateModels/DisqualifyingEntities, CreateModels/EndSession, CreateModels/EntityLabeling, CreateModels/WaitVsNoWaitAction, CreateModels/WhatsYourName</t>
+  </si>
+  <si>
+    <t>CreateModels/EndSession, CreateModels/WaitVsNoWaitAction</t>
+  </si>
+  <si>
+    <t>CreateModels/EndSession.spec.js, CreateModels/EntityLabeling.spec.js, CreateModels/WaitVsNoWaitActions.spec.js, EndSession/EndSession.spec.js, ErrorHandling/ActionUnavailable.spec.js, ErrorHandling/MissingAction.spec.js, Train/ConsistentEntityLabeling.spec.js, Train/DisqualifyingEntities.spec.js, Train/ExpectedEntityLabeling.spec.js, Train/LearnedEntityLabeling.spec.js, Train/WaitVsNoWaitActions.spec.js</t>
+  </si>
+  <si>
+    <t>Train with user and bot turns, save, training shows up in grid with all expected values</t>
+  </si>
+  <si>
+    <t>Edit Log, make changes, save, shows up in train dialog grid with all expected values</t>
+  </si>
+  <si>
+    <t>Edit training with user and bot turns, change or add turns, save, training shows up in grid with all expected values</t>
+  </si>
+  <si>
+    <t>New Train Dialog, Save</t>
+  </si>
+  <si>
+    <t>Edit Train Dialog, Save</t>
+  </si>
+  <si>
+    <t>New Log Dialog, Save</t>
+  </si>
+  <si>
+    <t>Edit Log Dialog, Save</t>
+  </si>
+  <si>
+    <t>Type user turns, wait for bot turns, save and log shows up in grid with all expected values</t>
+  </si>
+  <si>
+    <t>CreateModels/EndSession.spec.js, EditAndBranching/Branching.spec.js, EditAndBranching/VerifyEditTrainingControlsAndLabels.spec.js</t>
+  </si>
+  <si>
+    <t>Log/WhatsYourName, Tools/LoopYourName</t>
   </si>
 </sst>
 </file>
@@ -961,7 +961,10 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -989,14 +992,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F156" totalsRowShown="0" headerRowBorderDxfId="2" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F156" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F153" totalsRowShown="0" headerRowBorderDxfId="3" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F153" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
-    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature"/>
+    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{B0123158-48C7-47B5-8788-3102666127B5}" name="Page"/>
-    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1300,17 +1303,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F156"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81.33203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="60.44140625" style="3" bestFit="1" customWidth="1"/>
@@ -1323,7 +1326,7 @@
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1336,18 +1339,18 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>156</v>
+      <c r="B2" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>20</v>
@@ -1357,752 +1360,753 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>156</v>
+      <c r="B3" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>156</v>
+      <c r="B4" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>156</v>
+      <c r="B5" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>156</v>
+      <c r="B6" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>156</v>
+      <c r="B7" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>156</v>
+      <c r="B8" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
-        <v>156</v>
+      <c r="B9" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
-        <v>156</v>
+      <c r="B10" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>244</v>
+      <c r="B12" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>244</v>
+      <c r="B13" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>244</v>
+      <c r="B14" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>248</v>
+      <c r="B15" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>248</v>
+      <c r="B16" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
-        <v>248</v>
+      <c r="B17" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>234</v>
+        <v>226</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>13</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" t="s">
-        <v>14</v>
+      <c r="B24" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" t="s">
-        <v>14</v>
+      <c r="B25" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" t="s">
-        <v>14</v>
+      <c r="B26" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" t="s">
-        <v>242</v>
+      <c r="B28" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" t="s">
-        <v>251</v>
+      <c r="B29" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>252</v>
+        <v>264</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30" t="s">
-        <v>251</v>
+      <c r="B30" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>41</v>
+      <c r="B31" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B33" t="s">
-        <v>28</v>
+      <c r="B33" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="B34" t="s">
-        <v>25</v>
+      <c r="B34" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" t="s">
-        <v>24</v>
+      <c r="B35" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>27</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>13</v>
       </c>
-      <c r="B36" t="s">
-        <v>17</v>
+      <c r="B36" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>13</v>
       </c>
-      <c r="B37" t="s">
-        <v>19</v>
+      <c r="B37" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>95</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
-      <c r="B38" t="s">
-        <v>30</v>
+      <c r="B38" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B39" t="s">
-        <v>226</v>
+      <c r="B39" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" t="s">
-        <v>227</v>
-      </c>
-      <c r="C40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" t="s">
-        <v>230</v>
-      </c>
-      <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" t="s">
-        <v>231</v>
+        <v>37</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>54</v>
+        <v>37</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>55</v>
+        <v>37</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>46</v>
+        <v>138</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" t="s">
-        <v>43</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49" t="s">
-        <v>145</v>
-      </c>
-      <c r="C49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="E49" s="3" t="s">
-        <v>148</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>44</v>
-      </c>
-      <c r="B50" t="s">
-        <v>145</v>
+        <v>37</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" t="s">
-        <v>45</v>
+        <v>37</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>50</v>
+        <v>134</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C52" t="s">
-        <v>43</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B53" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" t="s">
-        <v>43</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" t="s">
-        <v>49</v>
+        <v>58</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>142</v>
+        <v>63</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>140</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>44</v>
-      </c>
-      <c r="B55" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>56</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>65</v>
-      </c>
-      <c r="B57" t="s">
-        <v>75</v>
+        <v>58</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
@@ -2111,295 +2115,292 @@
         <v>70</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>65</v>
-      </c>
-      <c r="B58" t="s">
-        <v>75</v>
+        <v>58</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>65</v>
-      </c>
-      <c r="B59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C59" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="E59" s="3" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B60" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61" t="s">
-        <v>75</v>
-      </c>
-      <c r="C61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" t="s">
-        <v>75</v>
-      </c>
-      <c r="C62" t="s">
-        <v>15</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>255</v>
-      </c>
-      <c r="C66" t="s">
-        <v>15</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E66" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>65</v>
-      </c>
-      <c r="B68" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C68" t="s">
         <v>15</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C69" t="s">
         <v>15</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C70" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B71" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C71" t="s">
         <v>15</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>65</v>
-      </c>
-      <c r="B72" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C72" t="s">
         <v>15</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C73" t="s">
         <v>15</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>65</v>
-      </c>
-      <c r="B74" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C74" t="s">
         <v>15</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>65</v>
-      </c>
-      <c r="B75" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C75" t="s">
         <v>15</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>65</v>
-      </c>
-      <c r="B76" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C76" t="s">
         <v>15</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>79</v>
+        <v>59</v>
+      </c>
+      <c r="F76" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>65</v>
-      </c>
-      <c r="B77" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C77" t="s">
         <v>15</v>
@@ -2407,349 +2408,334 @@
       <c r="D77" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E77" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>65</v>
-      </c>
-      <c r="B78" t="s">
-        <v>57</v>
-      </c>
-      <c r="C78" t="s">
-        <v>15</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>65</v>
-      </c>
-      <c r="B79" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C79" t="s">
         <v>15</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F79" t="s">
-        <v>69</v>
+        <v>78</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>65</v>
-      </c>
-      <c r="B80" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C80" t="s">
         <v>15</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>65</v>
-      </c>
-      <c r="B82" t="s">
-        <v>81</v>
-      </c>
-      <c r="C82" t="s">
-        <v>15</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>58</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C81" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>65</v>
-      </c>
-      <c r="B83" t="s">
-        <v>81</v>
-      </c>
-      <c r="C83" t="s">
-        <v>15</v>
+        <v>248</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>84</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>65</v>
-      </c>
-      <c r="B84" t="s">
-        <v>81</v>
-      </c>
-      <c r="C84" t="s">
-        <v>15</v>
+        <v>248</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>260</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>260</v>
+        <v>58</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>259</v>
+        <v>89</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>58</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C88" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>65</v>
-      </c>
-      <c r="B90" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C90" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>65</v>
-      </c>
-      <c r="B91" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C91" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>65</v>
-      </c>
-      <c r="B92" t="s">
+        <v>58</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C92" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E92" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C92" t="s">
-        <v>13</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>65</v>
-      </c>
-      <c r="B93" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C93" t="s">
         <v>15</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>100</v>
+      <c r="D93" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>65</v>
-      </c>
-      <c r="B94" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C94" t="s">
         <v>15</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>101</v>
+      <c r="D94" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>65</v>
-      </c>
-      <c r="B95" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C95" t="s">
         <v>15</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>65</v>
-      </c>
-      <c r="B96" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C96" t="s">
         <v>15</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>65</v>
-      </c>
-      <c r="B97" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C97" t="s">
         <v>15</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>65</v>
-      </c>
-      <c r="B98" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C98" t="s">
         <v>15</v>
       </c>
-      <c r="D98" s="4" t="s">
-        <v>108</v>
+      <c r="D98" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>65</v>
-      </c>
-      <c r="B99" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C99" t="s">
         <v>15</v>
       </c>
-      <c r="D99" s="4" t="s">
-        <v>112</v>
+      <c r="D99" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>65</v>
-      </c>
-      <c r="B100" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C100" t="s">
         <v>15</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>65</v>
-      </c>
-      <c r="B101" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C101" t="s">
         <v>15</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>65</v>
-      </c>
-      <c r="B102" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C102" t="s">
         <v>15</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>65</v>
-      </c>
-      <c r="B103" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C103" t="s">
         <v>15</v>
@@ -2757,10 +2743,10 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>65</v>
-      </c>
-      <c r="B104" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C104" t="s">
         <v>15</v>
@@ -2768,10 +2754,10 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>65</v>
-      </c>
-      <c r="B105" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C105" t="s">
         <v>15</v>
@@ -2779,201 +2765,219 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>65</v>
-      </c>
-      <c r="B106" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C106" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>65</v>
-      </c>
-      <c r="B107" t="s">
-        <v>96</v>
-      </c>
-      <c r="C107" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>65</v>
-      </c>
-      <c r="B108" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C108" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D108" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>65</v>
-      </c>
-      <c r="B109" t="s">
-        <v>96</v>
+        <v>58</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C109" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D109" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>58</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C110" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>65</v>
-      </c>
-      <c r="B111" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C111" t="s">
         <v>15</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="E111" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>65</v>
-      </c>
-      <c r="B112" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C112" t="s">
         <v>15</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>65</v>
-      </c>
-      <c r="B113" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C113" t="s">
         <v>15</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>65</v>
-      </c>
-      <c r="B114" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C114" t="s">
         <v>15</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>65</v>
-      </c>
-      <c r="B115" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C115" t="s">
         <v>15</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>65</v>
-      </c>
-      <c r="B116" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C116" t="s">
         <v>15</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>65</v>
-      </c>
-      <c r="B117" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C117" t="s">
         <v>15</v>
       </c>
+      <c r="D117" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="E117" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>65</v>
-      </c>
-      <c r="B118" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C118" t="s">
         <v>15</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>65</v>
-      </c>
-      <c r="B119" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C119" t="s">
         <v>15</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>65</v>
-      </c>
-      <c r="B120" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C120" t="s">
         <v>15</v>
@@ -2982,32 +2986,32 @@
         <v>131</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>65</v>
-      </c>
-      <c r="B121" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C121" t="s">
         <v>15</v>
       </c>
       <c r="D121" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>65</v>
-      </c>
-      <c r="B122" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C122" t="s">
         <v>15</v>
@@ -3016,350 +3020,320 @@
         <v>129</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>65</v>
-      </c>
-      <c r="B123" t="s">
-        <v>115</v>
+        <v>58</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C123" t="s">
         <v>15</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>65</v>
-      </c>
-      <c r="B124" t="s">
-        <v>115</v>
-      </c>
-      <c r="C124" t="s">
-        <v>15</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>65</v>
-      </c>
-      <c r="B125" t="s">
-        <v>115</v>
+        <v>16</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C125" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>130</v>
+        <v>271</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>65</v>
-      </c>
-      <c r="B126" t="s">
-        <v>115</v>
+        <v>16</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C126" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>16</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C127" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>16</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C128" t="s">
         <v>16</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>16</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C129" t="s">
         <v>16</v>
       </c>
-      <c r="D129" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>16</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C130" t="s">
         <v>16</v>
       </c>
-      <c r="D130" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>16</v>
-      </c>
-      <c r="B131" t="s">
-        <v>16</v>
-      </c>
-      <c r="C131" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>16</v>
-      </c>
-      <c r="B132" t="s">
-        <v>16</v>
-      </c>
-      <c r="C132" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>16</v>
-      </c>
-      <c r="B133" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>16</v>
+        <v>33</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F133" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>3</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134" t="s">
+        <v>12</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>3</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135" t="s">
+        <v>8</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>3</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C136" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E136" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F136" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>3</v>
       </c>
-      <c r="B137" t="s">
-        <v>4</v>
+      <c r="B137" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C137" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>3</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C138" t="s">
         <v>8</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>3</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>3</v>
       </c>
-      <c r="B140" t="s">
-        <v>90</v>
+      <c r="B140" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C140" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>3</v>
-      </c>
-      <c r="B141" t="s">
-        <v>4</v>
-      </c>
-      <c r="C141" t="s">
-        <v>8</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>3</v>
       </c>
-      <c r="B142" t="s">
-        <v>4</v>
+      <c r="B142" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C142" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>3</v>
       </c>
-      <c r="B143" t="s">
-        <v>4</v>
+      <c r="B143" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C143" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>3</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C144" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>3</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C145" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>3</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C146" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>3</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C147" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>3</v>
       </c>
-      <c r="B148" t="s">
-        <v>5</v>
-      </c>
-      <c r="C148" t="s">
-        <v>8</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>3</v>
       </c>
-      <c r="B149" t="s">
-        <v>5</v>
-      </c>
-      <c r="C149" t="s">
-        <v>10</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>37</v>
+      <c r="B149" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>3</v>
       </c>
-      <c r="B150" t="s">
-        <v>5</v>
-      </c>
-      <c r="C150" t="s">
-        <v>11</v>
-      </c>
-      <c r="D150" s="3" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
@@ -3370,27 +3344,9 @@
       <c r="A152" t="s">
         <v>3</v>
       </c>
-      <c r="B152" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3421,111 +3377,111 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3533,38 +3489,38 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3572,21 +3528,21 @@
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3595,57 +3551,57 @@
     </row>
     <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="B21" t="s">
-        <v>188</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3653,24 +3609,24 @@
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3678,94 +3634,94 @@
     </row>
     <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C27" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C29" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C31" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C33" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3779,74 +3735,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B38" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B39" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B40" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>199</v>
+      </c>
+      <c r="B41" t="s">
         <v>207</v>
       </c>
-      <c r="B41" t="s">
-        <v>215</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B42" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B43" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3854,30 +3810,30 @@
     </row>
     <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B45" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B46" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B47" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: update test grid
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BF6C35-95FE-41C1-954B-09D987A5DFC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E824D44-1D5C-42E5-AE2A-E31EB89DC1E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
-    <sheet name="Areas Features Validations" sheetId="1" r:id="rId1"/>
-    <sheet name="List of Test Specs" sheetId="2" r:id="rId2"/>
+    <sheet name="Read Me" sheetId="3" r:id="rId1"/>
+    <sheet name="Areas Features Validations" sheetId="1" r:id="rId2"/>
+    <sheet name="List of Test Specs" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="287">
   <si>
     <t>Page</t>
   </si>
@@ -879,6 +880,30 @@
   </si>
   <si>
     <t>EditAndBranching/Branching</t>
+  </si>
+  <si>
+    <t>* how you are using it</t>
+  </si>
+  <si>
+    <t>* if it gave you the information you wanted</t>
+  </si>
+  <si>
+    <t>* if you use it</t>
+  </si>
+  <si>
+    <t>* how often you use it</t>
+  </si>
+  <si>
+    <t>This spreadsheet was expensive to produce and to maintain…</t>
+  </si>
+  <si>
+    <t>therefore we should track its usefulness.</t>
+  </si>
+  <si>
+    <t>Please send an email to Michael Skowronski (v-miskow) to let me know…</t>
+  </si>
+  <si>
+    <t>How to use it…</t>
   </si>
 </sst>
 </file>
@@ -1326,12 +1351,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BC12DD-D15D-4ACB-8324-39485D2A6A83}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
   <dimension ref="A1:F154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,6 +2426,9 @@
       <c r="D71" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="E71" s="3" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -2391,7 +2478,7 @@
         <v>62</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>67</v>
+        <v>275</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2408,7 +2495,7 @@
         <v>48</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>67</v>
+        <v>275</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2423,6 +2510,9 @@
       </c>
       <c r="D76" s="3" t="s">
         <v>49</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3406,7 +3496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B719F-1470-4AFA-970E-2998AD817A19}">
   <dimension ref="A1:D47"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix: all scenarios have test spec names
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC5AA39-3A09-4618-8BB9-7A234E00974B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DB6659-4C5F-418C-AFF0-BBA6451BFD14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="295">
   <si>
     <t>Page</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>Action is unavailable' error message appears on a Bot turn after a training is edited and the prior user turn is modified in a way that invalidates the Bot's response.</t>
-  </si>
-  <si>
-    <t>ErrorHandling.ActionUnavailable</t>
   </si>
   <si>
     <t>Action does not exist' error message appears on a Bot turn after an Action used by a training has been deleted.</t>
@@ -840,9 +837,6 @@
     <t>Entity labeling scenarios from ConsistentEntityLabeling tests</t>
   </si>
   <si>
-    <t>ErrorHandling\ActionUnavailable, ErrorHandling\MissingAction, ErrorHandling\TwoConsecutiveUserInputs, ErrorHandling\WaitNonWait</t>
-  </si>
-  <si>
     <t>EditAndBranching/Branching, EditAndBranching/ConsistentEntityLabeling, EditAndBranching/VerifyEditTrainingControlsAndLabels, EndSession/EndSession, ErrorHandling/ActionUnavailable, ErrorHandling/BotModelMismatch, ErrorHandling/MissingAction, ErrorHandling/TwoConsecutiveUserInputs, ErrorHandling/WaitNonWait, Log/WhatsYourName, Train/ConsistentEntityLabeling, Train/DisqualifyingEntities, Train/ExpectedEntityLabeling, Train/LearnedEntityLabeling, Train/WaitVsNoWaitActions</t>
   </si>
   <si>
@@ -901,6 +895,39 @@
   </si>
   <si>
     <t>Single-Value, Negatable, Memory Panel</t>
+  </si>
+  <si>
+    <t>CreateModels/DateTimeResolver</t>
+  </si>
+  <si>
+    <t>CreateModels/DisqualifyingEntities</t>
+  </si>
+  <si>
+    <t>CreateModels/WaitVsNoWaitAction</t>
+  </si>
+  <si>
+    <t>CreateModels/WhatsYourName</t>
+  </si>
+  <si>
+    <t>ErrorHandling/ActionUnavailable</t>
+  </si>
+  <si>
+    <t>Train/ConsistentEntityLabeling</t>
+  </si>
+  <si>
+    <t>Train/ExpectedEntityLabeling</t>
+  </si>
+  <si>
+    <t>EditAndBranching/ConsistentEntityLabeling</t>
+  </si>
+  <si>
+    <t>ErrorHandling/BotModelMismatch</t>
+  </si>
+  <si>
+    <t>Log/WhatsYourName</t>
+  </si>
+  <si>
+    <t>ErrorHandling/ActionUnavailable, ErrorHandling/MissingAction, ErrorHandling/TwoConsecutiveUserInputs, ErrorHandling/WaitNonWait</t>
   </si>
 </sst>
 </file>
@@ -1349,58 +1376,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BC12DD-D15D-4ACB-8324-39485D2A6A83}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>259</v>
+      <c r="E9" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:E24">
+    <sortCondition ref="E1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1411,8 +1541,8 @@
   <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A141" sqref="A141:XFD142"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,7 +1582,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -1466,16 +1596,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1483,16 +1613,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1500,16 +1630,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1517,16 +1647,16 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1534,16 +1664,16 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1551,16 +1681,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1568,16 +1698,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1585,16 +1715,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1602,13 +1732,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1616,13 +1746,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1630,13 +1760,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1644,13 +1774,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1658,13 +1788,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1672,13 +1802,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1695,7 +1825,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1709,10 +1839,10 @@
         <v>28</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1726,7 +1856,7 @@
         <v>28</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1740,7 +1870,7 @@
         <v>28</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1754,10 +1884,10 @@
         <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1765,13 +1895,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1779,13 +1909,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1793,13 +1923,13 @@
         <v>12</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1807,16 +1937,16 @@
         <v>12</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1824,16 +1954,16 @@
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1841,16 +1971,16 @@
         <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1858,13 +1988,13 @@
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1898,10 +2028,10 @@
         <v>21</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1915,7 +2045,7 @@
         <v>17</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1923,13 +2053,13 @@
         <v>12</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1937,13 +2067,13 @@
         <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1951,13 +2081,13 @@
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1965,13 +2095,13 @@
         <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1985,10 +2115,10 @@
         <v>30</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2002,10 +2132,10 @@
         <v>30</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2019,10 +2149,10 @@
         <v>30</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2036,10 +2166,10 @@
         <v>30</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2047,16 +2177,16 @@
         <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2064,16 +2194,16 @@
         <v>31</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2081,16 +2211,16 @@
         <v>31</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
         <v>30</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2107,7 +2237,7 @@
         <v>34</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2124,7 +2254,7 @@
         <v>35</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2141,7 +2271,7 @@
         <v>36</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2155,10 +2285,10 @@
         <v>30</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2172,10 +2302,10 @@
         <v>30</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2192,7 +2322,7 @@
         <v>53</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2209,7 +2339,7 @@
         <v>59</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2226,7 +2356,7 @@
         <v>61</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2243,7 +2373,7 @@
         <v>60</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2260,7 +2390,7 @@
         <v>54</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2277,7 +2407,7 @@
         <v>65</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2291,10 +2421,10 @@
         <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -2308,7 +2438,7 @@
         <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -2316,13 +2446,13 @@
         <v>48</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2339,7 +2469,7 @@
         <v>41</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2356,7 +2486,7 @@
         <v>55</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2373,7 +2503,7 @@
         <v>45</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2390,7 +2520,7 @@
         <v>42</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2407,7 +2537,7 @@
         <v>63</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2424,7 +2554,7 @@
         <v>47</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2441,7 +2571,7 @@
         <v>46</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2458,7 +2588,7 @@
         <v>56</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2475,7 +2605,7 @@
         <v>57</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2492,7 +2622,7 @@
         <v>43</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2509,7 +2639,7 @@
         <v>44</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2557,7 +2687,7 @@
         <v>66</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2571,10 +2701,10 @@
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2588,26 +2718,26 @@
         <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2624,7 +2754,7 @@
         <v>71</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>265</v>
+        <v>294</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2641,7 +2771,7 @@
         <v>72</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>265</v>
+        <v>294</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2658,7 +2788,7 @@
         <v>73</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>265</v>
+        <v>294</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2675,7 +2805,7 @@
         <v>74</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>265</v>
+        <v>294</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2692,7 +2822,7 @@
         <v>75</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>265</v>
+        <v>294</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2709,7 +2839,7 @@
         <v>76</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>77</v>
+        <v>288</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2723,10 +2853,10 @@
         <v>14</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2740,10 +2870,10 @@
         <v>14</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2757,10 +2887,10 @@
         <v>14</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2774,10 +2904,10 @@
         <v>14</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2791,10 +2921,10 @@
         <v>14</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2808,10 +2938,10 @@
         <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2825,10 +2955,10 @@
         <v>14</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,7 +2983,7 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2916,16 +3046,16 @@
         <v>48</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C109" t="s">
         <v>14</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2933,13 +3063,13 @@
         <v>48</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C110" t="s">
         <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2947,16 +3077,16 @@
         <v>48</v>
       </c>
       <c r="B111" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C111" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C111" t="s">
-        <v>14</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="E111" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2964,13 +3094,13 @@
         <v>48</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C112" t="s">
         <v>14</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2978,16 +3108,16 @@
         <v>48</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C113" t="s">
         <v>14</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2995,13 +3125,13 @@
         <v>48</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C114" t="s">
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3009,13 +3139,13 @@
         <v>48</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C115" t="s">
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -3023,13 +3153,13 @@
         <v>48</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C116" t="s">
         <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3037,13 +3167,13 @@
         <v>48</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C117" t="s">
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3051,16 +3181,16 @@
         <v>48</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C118" t="s">
         <v>14</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3068,16 +3198,16 @@
         <v>48</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C119" t="s">
         <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3085,16 +3215,16 @@
         <v>48</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C120" t="s">
         <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3102,13 +3232,13 @@
         <v>48</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C121" t="s">
         <v>14</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3116,13 +3246,13 @@
         <v>48</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C122" t="s">
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3136,10 +3266,10 @@
         <v>15</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3153,7 +3283,7 @@
         <v>15</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3167,7 +3297,7 @@
         <v>15</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3181,7 +3311,7 @@
         <v>15</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3195,7 +3325,7 @@
         <v>15</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3209,7 +3339,7 @@
         <v>15</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3223,7 +3353,7 @@
         <v>15</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3242,7 +3372,7 @@
         <v>3</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -3251,7 +3381,7 @@
         <v>24</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3259,13 +3389,13 @@
         <v>3</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3273,7 +3403,7 @@
         <v>3</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
@@ -3282,7 +3412,7 @@
         <v>67</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3290,7 +3420,7 @@
         <v>3</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
@@ -3415,111 +3545,111 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3527,38 +3657,38 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3566,21 +3696,21 @@
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3589,57 +3719,57 @@
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" t="s">
         <v>140</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3647,24 +3777,24 @@
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" t="s">
         <v>149</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3675,13 +3805,13 @@
         <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3689,10 +3819,10 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3700,13 +3830,13 @@
         <v>48</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3714,13 +3844,13 @@
         <v>48</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="C30" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3728,13 +3858,13 @@
         <v>48</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3742,10 +3872,10 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3753,13 +3883,13 @@
         <v>48</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3773,74 +3903,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" t="s">
         <v>164</v>
       </c>
-      <c r="B38" t="s">
-        <v>165</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B40" t="s">
+        <v>169</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B41" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B42" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B43" t="s">
+        <v>175</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3848,30 +3978,30 @@
     </row>
     <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" t="s">
         <v>178</v>
       </c>
-      <c r="B45" t="s">
-        <v>179</v>
-      </c>
       <c r="D45" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B47" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
Test Grid Updates and Fix for SaveAsIsVerifyInGrid (#1149)
Updates to the TestGrid.xlsx - For all covered test scenarios the test spec files are listed

SaveAsIsVerifyInGrid Fix - This fix is to deal with the rendering issues that come up when a Train Dialog is saved. While I am not happy with how convoluted this function and VerifyTrainingSummaryIsInGrid are becoming, right now I don't have a clear idea of the perfect fix. So I want to check it in and run with these changes for now, and see if any other rendering issues cause test failures while I think about how to write a better fix for this.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E824D44-1D5C-42E5-AE2A-E31EB89DC1E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D66D21-D67D-4693-9F1A-CA8D5200DBC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId2"/>
     <sheet name="List of Test Specs" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="295">
   <si>
     <t>Page</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Log Dialog - Chat Panel</t>
   </si>
   <si>
-    <t>Entities Grid</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -110,18 +107,9 @@
     <t>Saved to a file in JSON format</t>
   </si>
   <si>
-    <t>Setting is persisted, shows checked after save then edit</t>
-  </si>
-  <si>
-    <t>Checkbox is set in grid</t>
-  </si>
-  <si>
     <t>Entities accumulate values in training memory</t>
   </si>
   <si>
-    <t>Entities remove values in training memory</t>
-  </si>
-  <si>
     <t>All values show up as a list when displayed in training webchat</t>
   </si>
   <si>
@@ -134,9 +122,6 @@
     <t>Action Dialog</t>
   </si>
   <si>
-    <t>Entities Dialog</t>
-  </si>
-  <si>
     <t>Michael manually does this on a regular basis</t>
   </si>
   <si>
@@ -248,30 +233,12 @@
     <t>Selecting a user turn causes "Entity Detection" UI Elements to show up</t>
   </si>
   <si>
-    <t>CreateModels.TagAndFrog</t>
-  </si>
-  <si>
     <t>User can label one word of a user utterance as a single value for a single entity</t>
   </si>
   <si>
-    <t>User can label two words of a user utterance as two values for a single entity</t>
-  </si>
-  <si>
-    <t>Only verifies name</t>
-  </si>
-  <si>
-    <t>CreateModels All Test Cases</t>
-  </si>
-  <si>
     <t>A removed or replaced Entity shows in training memory as crossed out</t>
   </si>
   <si>
-    <t>Single-Value</t>
-  </si>
-  <si>
-    <t>All checkmarks are set or unset in grid after saving an entity</t>
-  </si>
-  <si>
     <t>All checkmarks are set or unset in grid based on entity that was used.</t>
   </si>
   <si>
@@ -299,30 +266,15 @@
     <t>Action is unavailable' error message appears on a Bot turn after a training is edited and the prior user turn is modified in a way that invalidates the Bot's response.</t>
   </si>
   <si>
-    <t>ErrorHandling - All Tests</t>
-  </si>
-  <si>
-    <t>ErrorHandling.ActionUnavailable</t>
-  </si>
-  <si>
     <t>Action does not exist' error message appears on a Bot turn after an Action used by a training has been deleted.</t>
   </si>
   <si>
     <t>Bot turn that used an Action that was deleted will be replaced with an error message giving the Id of the Action that was deleted.</t>
   </si>
   <si>
-    <t>ErrorHandling.MissingAction</t>
-  </si>
-  <si>
     <t>Two consecutive User Inputs' error message appears on a User turn after another user turn is inserted directly after that turn.</t>
   </si>
   <si>
-    <t>ErrorHandling.TwoConsecutiveUserInputs</t>
-  </si>
-  <si>
-    <t>ErrorHandling.WaitNonWait</t>
-  </si>
-  <si>
     <t>Action follows a Wait Action' error message appears on a Bot turn after inserting a new Bot turn directly after a Wait Action turn.</t>
   </si>
   <si>
@@ -338,9 +290,6 @@
     <t>EndSession</t>
   </si>
   <si>
-    <t>EndSession.EndSession</t>
-  </si>
-  <si>
     <t>An EndSession chat turn should only contain a delete button when selected.</t>
   </si>
   <si>
@@ -350,12 +299,6 @@
     <t>Inserting a Bot turn so that it is NOT the last turn should not automatically select an EndSession action based on past trainings.</t>
   </si>
   <si>
-    <t>Score Action for the last Bot turn that is already an EndSession should NOT disable all other EndSession Actions.</t>
-  </si>
-  <si>
-    <t>EndSession.AddEndSessionAction</t>
-  </si>
-  <si>
     <t>Chat input control for "Type your message" should not be visible when an EndSession Action has been used.</t>
   </si>
   <si>
@@ -371,18 +314,9 @@
     <t>Bot should respond to user utterance with expected response due to existing Train Dialogs</t>
   </si>
   <si>
-    <t>EndSession Action should show the Data defined in the Action as the final response to user utterance.</t>
-  </si>
-  <si>
-    <t>CreateModels.EndSession</t>
-  </si>
-  <si>
     <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn should not delete the description field. (Bug 2026)</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>Editing a Bot turn that is the last turn, and the user creates a new EndSession Action, it should automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 2014)</t>
   </si>
   <si>
@@ -405,12 +339,6 @@
   </si>
   <si>
     <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn and saving it should not result in two Train Dialogs. (Bug 1969)</t>
-  </si>
-  <si>
-    <t>Train.BookMeAFlight</t>
-  </si>
-  <si>
-    <t>User can label two or more words of a user utterance as a single value for a single entity</t>
   </si>
   <si>
     <t>Actions containing entites with "datetimeV2" resolver types resolve common expressions of dates, like "tomorrow" and "Sunday next week", to the correct calander dates.</t>
@@ -747,9 +675,6 @@
 4) Verify cannot click on to edit any other existing turn</t>
   </si>
   <si>
-    <t>Entity labeling from ConsistentEntityLabeling tests</t>
-  </si>
-  <si>
     <t>TODO new case for when something was not labeled and now it is</t>
   </si>
   <si>
@@ -792,9 +717,6 @@
     <t>CreateModels/EndSession, CreateModels/WaitVsNoWaitAction</t>
   </si>
   <si>
-    <t>CreateModels/EndSession.spec.js, CreateModels/EntityLabeling.spec.js, CreateModels/WaitVsNoWaitActions.spec.js, EndSession/EndSession.spec.js, ErrorHandling/ActionUnavailable.spec.js, ErrorHandling/MissingAction.spec.js, Train/ConsistentEntityLabeling.spec.js, Train/DisqualifyingEntities.spec.js, Train/ExpectedEntityLabeling.spec.js, Train/LearnedEntityLabeling.spec.js, Train/WaitVsNoWaitActions.spec.js</t>
-  </si>
-  <si>
     <t>Train with user and bot turns, save, training shows up in grid with all expected values</t>
   </si>
   <si>
@@ -819,18 +741,12 @@
     <t>Type user turns, wait for bot turns, save and log shows up in grid with all expected values</t>
   </si>
   <si>
-    <t>CreateModels/EndSession.spec.js, EditAndBranching/Branching.spec.js, EditAndBranching/VerifyEditTrainingControlsAndLabels.spec.js</t>
-  </si>
-  <si>
     <t>Log/WhatsYourName, Tools/LoopYourName</t>
   </si>
   <si>
     <t>Missing grid validation to be complete</t>
   </si>
   <si>
-    <t>EditAndBranching/Branching.spec.js, EditAndBranching/ConsistentEntityLabeling.spec.js, EditAndBranching/VerifyEditTrainingControlsAndLabels.spec.js, EndSession/EndSession.spec.js, ErrorHandling/ActionUnavailable.spec.js, ErrorHandling/BotModelMismatch.spec.js, ErrorHandling/MissingAction.spec.js, ErrorHandling/TwoConsecutiveUserInputs.spec.js, ErrorHandling/WaitNonWait.spec.js, Log/WhatsYourName.spec.js, Train/ConsistentEntityLabeling.spec.js, Train/DisqualifyingEntities.spec.js, Train/ExpectedEntityLabeling.spec.js, Train/LearnedEntityLabeling.spec.js, Train/WaitVsNoWaitActions.spec.js</t>
-  </si>
-  <si>
     <t>NO data fields are directly verified. They are indirectly verified by using the model to train and perform other scenarios which would fail if the expected fields were not present.</t>
   </si>
   <si>
@@ -904,6 +820,114 @@
   </si>
   <si>
     <t>How to use it…</t>
+  </si>
+  <si>
+    <t>CreateModels/EntityLabeling</t>
+  </si>
+  <si>
+    <t>CreateModels/EntityLabeling, ErrorHandling/ActionUnavailable, Train/DateTimeResolver, Train/LearnedEntityLabeling</t>
+  </si>
+  <si>
+    <t>User can label two words of a user utterance as two values for a single multi-valued entity</t>
+  </si>
+  <si>
+    <t>User can label a phrase (two or more consecutive words) of a user utterance as a single value for a single entity</t>
+  </si>
+  <si>
+    <t>Entity labeling scenarios from ConsistentEntityLabeling tests</t>
+  </si>
+  <si>
+    <t>EditAndBranching/Branching, EditAndBranching/ConsistentEntityLabeling, EditAndBranching/VerifyEditTrainingControlsAndLabels, EndSession/EndSession, ErrorHandling/ActionUnavailable, ErrorHandling/BotModelMismatch, ErrorHandling/MissingAction, ErrorHandling/TwoConsecutiveUserInputs, ErrorHandling/WaitNonWait, Log/WhatsYourName, Train/ConsistentEntityLabeling, Train/DisqualifyingEntities, Train/ExpectedEntityLabeling, Train/LearnedEntityLabeling, Train/WaitVsNoWaitActions</t>
+  </si>
+  <si>
+    <t>CreateModels/EndSession, CreateModels/EntityLabeling, CreateModels/WaitVsNoWaitActions, EndSession/EndSession, ErrorHandling/ActionUnavailable, ErrorHandling/MissingAction, Train/ConsistentEntityLabeling, Train/DisqualifyingEntities, Train/ExpectedEntityLabeling, Train/LearnedEntityLabeling, Train/WaitVsNoWaitActions</t>
+  </si>
+  <si>
+    <t>CreateModels/EndSession, EditAndBranching/Branching, EditAndBranching/VerifyEditTrainingControlsAndLabels</t>
+  </si>
+  <si>
+    <t>ErrorHandling/MissingAction</t>
+  </si>
+  <si>
+    <t>ErrorHandling/TwoConsecutiveUserInputs</t>
+  </si>
+  <si>
+    <t>ErrorHandling/WaitNonWait</t>
+  </si>
+  <si>
+    <t>TODO: There are more error messages to validate</t>
+  </si>
+  <si>
+    <t>Score Action for the last Bot turn that is already an EndSession should enable all EndSession Actions.</t>
+  </si>
+  <si>
+    <t>CreateModels/EndSession</t>
+  </si>
+  <si>
+    <t>User turn that causes Bot to respond with an EndSession Action should give no visible response to the user.</t>
+  </si>
+  <si>
+    <t>User turn that causes Bot to respond with an EndSession Action, followed by another set of user turns should result in two saved Log Dialogs.</t>
+  </si>
+  <si>
+    <t>Abandon button should discard Log Dialog session and not persist it, even when an EndSession is invoked by a user turn.</t>
+  </si>
+  <si>
+    <t>Edit existing Log Dialog, then delete should remove the log dialog from the list.</t>
+  </si>
+  <si>
+    <t>Abandon button should discard ALL Log Dialog sessions and not persist any of them when multiple Log Dialog sessions are created via invoking an EndSession action and then it is followed up by another round of multiple Log Dialogs sessions that are ultimately saved. (bug 2111)</t>
+  </si>
+  <si>
+    <t>Multi-Value, Memory Panel</t>
+  </si>
+  <si>
+    <t>Memory Panel</t>
+  </si>
+  <si>
+    <t>A removed Entity shows in training memory as crossed out</t>
+  </si>
+  <si>
+    <t>CreateModels/EntityLabeling, Train/DateTimeResolver, Train/DisqualifyingEntities, Train/ExpectedEntityLabeling, Train/LearnedEntityLabeling</t>
+  </si>
+  <si>
+    <t>Multi-Value, Negatable, Memory Panel</t>
+  </si>
+  <si>
+    <t>Single-Value, Negatable, Memory Panel</t>
+  </si>
+  <si>
+    <t>CreateModels/DateTimeResolver</t>
+  </si>
+  <si>
+    <t>CreateModels/DisqualifyingEntities</t>
+  </si>
+  <si>
+    <t>CreateModels/WaitVsNoWaitAction</t>
+  </si>
+  <si>
+    <t>CreateModels/WhatsYourName</t>
+  </si>
+  <si>
+    <t>ErrorHandling/ActionUnavailable</t>
+  </si>
+  <si>
+    <t>Train/ConsistentEntityLabeling</t>
+  </si>
+  <si>
+    <t>Train/ExpectedEntityLabeling</t>
+  </si>
+  <si>
+    <t>EditAndBranching/ConsistentEntityLabeling</t>
+  </si>
+  <si>
+    <t>ErrorHandling/BotModelMismatch</t>
+  </si>
+  <si>
+    <t>Log/WhatsYourName</t>
+  </si>
+  <si>
+    <t>ErrorHandling/ActionUnavailable, ErrorHandling/MissingAction, ErrorHandling/TwoConsecutiveUserInputs, ErrorHandling/WaitNonWait</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1065,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F154" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F154" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F148" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F148" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="3"/>
@@ -1352,58 +1376,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BC12DD-D15D-4ACB-8324-39485D2A6A83}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="E1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="E4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="E5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="E6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="E7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>286</v>
+        <v>258</v>
+      </c>
+      <c r="E9" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:E24">
+    <sortCondition ref="E1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1411,11 +1538,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,1888 +1574,1876 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>260</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
         <v>17</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C49" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E50" s="3" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" t="s">
-        <v>35</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="E51" s="3" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C52" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C53" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="E55" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C68" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="E68" s="3" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>73</v>
+        <v>261</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>125</v>
+        <v>262</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>124</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>234</v>
+        <v>263</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C88" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C89" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C90" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C92" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>88</v>
+        <v>294</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>89</v>
+        <v>288</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>92</v>
+        <v>267</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C95" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>92</v>
+        <v>267</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>94</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B97" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C97" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C97" t="s">
-        <v>15</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="E97" s="3" t="s">
-        <v>95</v>
+        <v>269</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C98" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>95</v>
+        <v>269</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>95</v>
+        <v>269</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C100" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>95</v>
+        <v>269</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C101" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C102" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C103" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C104" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C105" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C106" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C107" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C109" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>101</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C110" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>115</v>
+        <v>271</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C111" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>101</v>
+        <v>249</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C112" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>101</v>
+        <v>249</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>101</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C114" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C115" t="s">
-        <v>15</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C116" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C117" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C118" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>115</v>
+        <v>249</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C119" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>106</v>
+        <v>272</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C120" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>113</v>
+        <v>272</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B121" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D121" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C121" t="s">
-        <v>15</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C122" t="s">
+        <v>14</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>15</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>53</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C123" t="s">
+      <c r="B124" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>53</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="C124" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D124" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>15</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C125" t="s">
+        <v>15</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C126" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C127" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>110</v>
+        <v>277</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C128" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C129" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C130" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C131" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>3</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>4</v>
+        <v>278</v>
       </c>
       <c r="C134" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F134" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>3</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>4</v>
+        <v>282</v>
       </c>
       <c r="C135" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>3</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>4</v>
+        <v>283</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>3</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>4</v>
+        <v>279</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>3</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C138" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>3</v>
       </c>
@@ -3336,154 +3451,70 @@
         <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>3</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C140" t="s">
-        <v>10</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>3</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C141" t="s">
+        <v>10</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142" t="s">
         <v>11</v>
       </c>
-      <c r="D141" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D142" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>3</v>
       </c>
-      <c r="B143" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C143" t="s">
-        <v>33</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>3</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C144" t="s">
-        <v>12</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>3</v>
       </c>
-      <c r="B145" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C145" t="s">
-        <v>8</v>
-      </c>
-      <c r="D145" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>3</v>
       </c>
-      <c r="B146" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C146" t="s">
-        <v>8</v>
-      </c>
-      <c r="D146" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>3</v>
       </c>
-      <c r="B147" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C147" t="s">
-        <v>10</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>3</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C148" t="s">
-        <v>11</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>3</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3500,7 +3531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B719F-1470-4AFA-970E-2998AD817A19}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -3514,111 +3545,111 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3626,38 +3657,38 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,21 +3696,21 @@
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3688,57 +3719,57 @@
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3746,24 +3777,24 @@
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3771,94 +3802,94 @@
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="C31" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3872,74 +3903,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B38" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B40" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B42" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B43" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3947,30 +3978,30 @@
     </row>
     <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="B45" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="B46" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="B47" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: updated the read me sheet
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D66D21-D67D-4693-9F1A-CA8D5200DBC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A34DBC-BBDE-4C88-A4B8-41C971738865}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="292">
   <si>
     <t>Page</t>
   </si>
@@ -897,44 +897,67 @@
     <t>Single-Value, Negatable, Memory Panel</t>
   </si>
   <si>
-    <t>CreateModels/DateTimeResolver</t>
-  </si>
-  <si>
-    <t>CreateModels/DisqualifyingEntities</t>
-  </si>
-  <si>
-    <t>CreateModels/WaitVsNoWaitAction</t>
-  </si>
-  <si>
-    <t>CreateModels/WhatsYourName</t>
-  </si>
-  <si>
     <t>ErrorHandling/ActionUnavailable</t>
   </si>
   <si>
-    <t>Train/ConsistentEntityLabeling</t>
-  </si>
-  <si>
-    <t>Train/ExpectedEntityLabeling</t>
-  </si>
-  <si>
-    <t>EditAndBranching/ConsistentEntityLabeling</t>
-  </si>
-  <si>
-    <t>ErrorHandling/BotModelMismatch</t>
-  </si>
-  <si>
-    <t>Log/WhatsYourName</t>
-  </si>
-  <si>
     <t>ErrorHandling/ActionUnavailable, ErrorHandling/MissingAction, ErrorHandling/TwoConsecutiveUserInputs, ErrorHandling/WaitNonWait</t>
+  </si>
+  <si>
+    <r>
+      <t>Areas Features and Validations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – This sheet describes the areas and features being tested, along with the details of the scenario and the list of test spec files that cover them. This is the sheet I expect team members to use the most.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>List of Test Specs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – This sheet describes the test spec files and summarizes what it tests. It also references the old test names which right now helps me when I need to go back and figure out what test is doing what since I don’t remember the new names like I do the old ones…eventually I’ll probably eliminate this column as the need goes away.</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Name Column</t>
+  </si>
+  <si>
+    <t>An empty cell in the “Test Name” column indicates there is no test coverage for the scenario given. The names are listed to make them easy to copy to the clipboard and construct a command line to run just those test cases via Cypress. The “.spec.js” part of the file name was left out for brevity sake along with the path prefix that is common to all tests.</t>
+  </si>
+  <si>
+    <t>Column Filtering</t>
+  </si>
+  <si>
+    <t>By using the column filtering feature employed in this sheet you can focus in on a specific test spec file, or specific feature or area you are interested in. For example, if you want to know what scenarios and tests we have that deal with Entities, you could filter the “Feature” column by “entit” to limit the view to just tests dealing with Entities.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,13 +996,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1000,11 +1043,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1026,8 +1070,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1376,161 +1424,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BC12DD-D15D-4ACB-8324-39485D2A6A83}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="E1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>252</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C10" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>258</v>
-      </c>
-      <c r="E9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
-        <v>246</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:E24">
-    <sortCondition ref="E1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1541,8 +1514,8 @@
   <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,7 +2727,7 @@
         <v>71</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2771,7 +2744,7 @@
         <v>72</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2788,7 +2761,7 @@
         <v>73</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2805,7 +2778,7 @@
         <v>74</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2822,7 +2795,7 @@
         <v>75</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2839,7 +2812,7 @@
         <v>76</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: updated the read me sheet (#1153)
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D66D21-D67D-4693-9F1A-CA8D5200DBC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A34DBC-BBDE-4C88-A4B8-41C971738865}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="292">
   <si>
     <t>Page</t>
   </si>
@@ -897,44 +897,67 @@
     <t>Single-Value, Negatable, Memory Panel</t>
   </si>
   <si>
-    <t>CreateModels/DateTimeResolver</t>
-  </si>
-  <si>
-    <t>CreateModels/DisqualifyingEntities</t>
-  </si>
-  <si>
-    <t>CreateModels/WaitVsNoWaitAction</t>
-  </si>
-  <si>
-    <t>CreateModels/WhatsYourName</t>
-  </si>
-  <si>
     <t>ErrorHandling/ActionUnavailable</t>
   </si>
   <si>
-    <t>Train/ConsistentEntityLabeling</t>
-  </si>
-  <si>
-    <t>Train/ExpectedEntityLabeling</t>
-  </si>
-  <si>
-    <t>EditAndBranching/ConsistentEntityLabeling</t>
-  </si>
-  <si>
-    <t>ErrorHandling/BotModelMismatch</t>
-  </si>
-  <si>
-    <t>Log/WhatsYourName</t>
-  </si>
-  <si>
     <t>ErrorHandling/ActionUnavailable, ErrorHandling/MissingAction, ErrorHandling/TwoConsecutiveUserInputs, ErrorHandling/WaitNonWait</t>
+  </si>
+  <si>
+    <r>
+      <t>Areas Features and Validations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – This sheet describes the areas and features being tested, along with the details of the scenario and the list of test spec files that cover them. This is the sheet I expect team members to use the most.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>List of Test Specs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – This sheet describes the test spec files and summarizes what it tests. It also references the old test names which right now helps me when I need to go back and figure out what test is doing what since I don’t remember the new names like I do the old ones…eventually I’ll probably eliminate this column as the need goes away.</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Name Column</t>
+  </si>
+  <si>
+    <t>An empty cell in the “Test Name” column indicates there is no test coverage for the scenario given. The names are listed to make them easy to copy to the clipboard and construct a command line to run just those test cases via Cypress. The “.spec.js” part of the file name was left out for brevity sake along with the path prefix that is common to all tests.</t>
+  </si>
+  <si>
+    <t>Column Filtering</t>
+  </si>
+  <si>
+    <t>By using the column filtering feature employed in this sheet you can focus in on a specific test spec file, or specific feature or area you are interested in. For example, if you want to know what scenarios and tests we have that deal with Entities, you could filter the “Feature” column by “entit” to limit the view to just tests dealing with Entities.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,13 +996,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1000,11 +1043,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1026,8 +1070,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1376,161 +1424,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BC12DD-D15D-4ACB-8324-39485D2A6A83}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="E1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>252</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C10" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>258</v>
-      </c>
-      <c r="E9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
-        <v>246</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:E24">
-    <sortCondition ref="E1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1541,8 +1514,8 @@
   <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,7 +2727,7 @@
         <v>71</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2771,7 +2744,7 @@
         <v>72</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2788,7 +2761,7 @@
         <v>73</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2805,7 +2778,7 @@
         <v>74</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2822,7 +2795,7 @@
         <v>75</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2839,7 +2812,7 @@
         <v>76</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: updated the test grid spread sheet
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A34DBC-BBDE-4C88-A4B8-41C971738865}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA87D978-2D25-47E7-B7AA-06E164584A69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="304">
   <si>
     <t>Page</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>Bot should respond to user utterance with expected response due to existing Train Dialogs</t>
-  </si>
-  <si>
-    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn should not delete the description field. (Bug 2026)</t>
   </si>
   <si>
     <t>Editing a Bot turn that is the last turn, and the user creates a new EndSession Action, it should automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 2014)</t>
@@ -874,9 +871,6 @@
   </si>
   <si>
     <t>Edit existing Log Dialog, then delete should remove the log dialog from the list.</t>
-  </si>
-  <si>
-    <t>Abandon button should discard ALL Log Dialog sessions and not persist any of them when multiple Log Dialog sessions are created via invoking an EndSession action and then it is followed up by another round of multiple Log Dialogs sessions that are ultimately saved. (bug 2111)</t>
   </si>
   <si>
     <t>Multi-Value, Memory Panel</t>
@@ -952,12 +946,76 @@
   <si>
     <t>By using the column filtering feature employed in this sheet you can focus in on a specific test spec file, or specific feature or area you are interested in. For example, if you want to know what scenarios and tests we have that deal with Entities, you could filter the “Feature” column by “entit” to limit the view to just tests dealing with Entities.</t>
   </si>
+  <si>
+    <t>Log multiple dialogs (3) that each invoke an EndSession action - then abandon it - again log multiple log dialogs (3) that each invoke an EndSession action - then save it. Verify that log dialogs ONLY saved the ones we saved and abandoned the ones we had abandoned. (bug 2111)</t>
+  </si>
+  <si>
+    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn should not delete the description field and should not result in an extra TD. (Bug 2026)</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Abandoning a Train Dialog should cause model to forget the training that was in progress. (bug 2105)</t>
+  </si>
+  <si>
+    <t>Bot Response</t>
+  </si>
+  <si>
+    <r>
+      <t>Bot response should appear after Action selection (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AND SOME CONDITION THAT WE NEED MATT TO TELL US ABOUT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) (bug 2014)</t>
+    </r>
+  </si>
+  <si>
+    <t>Tree View</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Clicking on the 1st, last or any turn in Tree View should take you to the Train Dialog (bug 2097)</t>
+  </si>
+  <si>
+    <t>Click on a turn that comes after labeling an entity and it should show the Entity Detection and Memory panes. (bug 2096)</t>
+  </si>
+  <si>
+    <t>Merge Dialog</t>
+  </si>
+  <si>
+    <t>Save As Is</t>
+  </si>
+  <si>
+    <t>Merge Dialog Modal</t>
+  </si>
+  <si>
+    <t>"Save As Is" for a Train Dialog should update the Last Modified Time (bug 2092)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1007,6 +1065,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1113,8 +1178,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F148" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F148" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F149" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F149" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="3"/>
@@ -1439,68 +1504,68 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>288</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1511,16 +1576,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81.28515625" style="3" customWidth="1"/>
@@ -1555,7 +1620,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -1569,16 +1634,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1586,16 +1651,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1603,16 +1668,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1620,16 +1685,16 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1637,16 +1702,16 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1654,16 +1719,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1671,16 +1736,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1688,16 +1753,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,13 +1770,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1719,13 +1784,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1733,13 +1798,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,13 +1812,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1761,13 +1826,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1775,13 +1840,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1798,7 +1863,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1812,10 +1877,10 @@
         <v>28</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1829,7 +1894,7 @@
         <v>28</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1843,7 +1908,7 @@
         <v>28</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,10 +1922,10 @@
         <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,13 +1933,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1882,13 +1947,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1896,13 +1961,13 @@
         <v>12</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1910,16 +1975,16 @@
         <v>12</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1927,16 +1992,16 @@
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1944,16 +2009,16 @@
         <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1961,13 +2026,13 @@
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2001,10 +2066,10 @@
         <v>21</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2018,7 +2083,7 @@
         <v>17</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2026,13 +2091,13 @@
         <v>12</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,13 +2105,13 @@
         <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2054,13 +2119,13 @@
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2068,13 +2133,13 @@
         <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2091,7 +2156,7 @@
         <v>89</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2105,10 +2170,10 @@
         <v>30</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2122,10 +2187,10 @@
         <v>30</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2139,10 +2204,10 @@
         <v>30</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2150,16 +2215,16 @@
         <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2167,16 +2232,16 @@
         <v>31</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2184,16 +2249,16 @@
         <v>31</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" t="s">
         <v>30</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2210,7 +2275,7 @@
         <v>34</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2227,7 +2292,7 @@
         <v>35</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2244,7 +2309,7 @@
         <v>36</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2258,10 +2323,10 @@
         <v>30</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2278,7 +2343,7 @@
         <v>90</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2295,7 +2360,7 @@
         <v>53</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2312,7 +2377,7 @@
         <v>59</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2329,7 +2394,7 @@
         <v>61</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2346,7 +2411,7 @@
         <v>60</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2363,7 +2428,7 @@
         <v>54</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2380,7 +2445,7 @@
         <v>65</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2394,10 +2459,10 @@
         <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -2411,7 +2476,7 @@
         <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -2419,13 +2484,13 @@
         <v>48</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2442,7 +2507,7 @@
         <v>41</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2459,7 +2524,7 @@
         <v>55</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2476,7 +2541,7 @@
         <v>45</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2493,7 +2558,7 @@
         <v>42</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2510,7 +2575,7 @@
         <v>63</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2527,7 +2592,7 @@
         <v>47</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,7 +2609,7 @@
         <v>46</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2561,7 +2626,7 @@
         <v>56</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2578,7 +2643,7 @@
         <v>57</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2595,7 +2660,7 @@
         <v>43</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2612,7 +2677,7 @@
         <v>44</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2660,7 +2725,7 @@
         <v>66</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2674,10 +2739,10 @@
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2691,26 +2756,26 @@
         <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2727,7 +2792,7 @@
         <v>71</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2744,7 +2809,7 @@
         <v>72</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2761,7 +2826,7 @@
         <v>73</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2778,7 +2843,7 @@
         <v>74</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2795,7 +2860,7 @@
         <v>75</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2812,7 +2877,7 @@
         <v>76</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2829,7 +2894,7 @@
         <v>77</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2846,7 +2911,7 @@
         <v>78</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2863,7 +2928,7 @@
         <v>79</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2880,7 +2945,7 @@
         <v>81</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2897,7 +2962,7 @@
         <v>80</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2914,7 +2979,7 @@
         <v>82</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2931,7 +2996,7 @@
         <v>83</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2956,7 +3021,7 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3028,7 +3093,7 @@
         <v>86</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3042,7 +3107,7 @@
         <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3059,7 +3124,7 @@
         <v>85</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3073,7 +3138,7 @@
         <v>14</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3090,7 +3155,7 @@
         <v>87</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3104,7 +3169,7 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3118,7 +3183,7 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -3132,7 +3197,7 @@
         <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3146,7 +3211,7 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3163,7 +3228,7 @@
         <v>88</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3177,10 +3242,10 @@
         <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>93</v>
+        <v>291</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3194,10 +3259,10 @@
         <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3211,7 +3276,7 @@
         <v>14</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3225,41 +3290,10 @@
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>15</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C124" t="s">
-        <v>15</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>15</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C125" t="s">
-        <v>15</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>15</v>
       </c>
@@ -3270,10 +3304,13 @@
         <v>15</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>15</v>
       </c>
@@ -3284,7 +3321,7 @@
         <v>15</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>277</v>
+        <v>91</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3298,7 +3335,7 @@
         <v>15</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3312,10 +3349,10 @@
         <v>15</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -3326,7 +3363,7 @@
         <v>15</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3339,22 +3376,22 @@
       <c r="C131" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>3</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="C134" t="s">
-        <v>8</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>281</v>
+      <c r="D131" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>15</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C132" t="s">
+        <v>15</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3362,13 +3399,16 @@
         <v>3</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>280</v>
+        <v>24</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3376,30 +3416,30 @@
         <v>3</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E136" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>3</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3407,13 +3447,13 @@
         <v>3</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>4</v>
+        <v>277</v>
       </c>
       <c r="C138" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3424,24 +3464,24 @@
         <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>3</v>
       </c>
-      <c r="B141" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C141" t="s">
-        <v>10</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>26</v>
+      <c r="B140" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" t="s">
+        <v>11</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3452,7 +3492,7 @@
         <v>5</v>
       </c>
       <c r="C142" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>26</v>
@@ -3462,33 +3502,117 @@
       <c r="A143" t="s">
         <v>3</v>
       </c>
+      <c r="B143" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>3</v>
       </c>
-      <c r="B144" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>48</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C151" t="s">
+        <v>14</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>48</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C152" t="s">
+        <v>14</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>297</v>
+      </c>
+      <c r="B153" t="s">
+        <v>296</v>
+      </c>
+      <c r="C153" t="s">
+        <v>296</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>297</v>
+      </c>
+      <c r="B154" t="s">
+        <v>296</v>
+      </c>
+      <c r="C154" t="s">
+        <v>296</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>300</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C155" t="s">
+        <v>302</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -3518,111 +3642,111 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3630,38 +3754,38 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3675,7 +3799,7 @@
         <v>84</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3683,7 +3807,7 @@
         <v>84</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3692,57 +3816,57 @@
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" t="s">
         <v>139</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B22" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3750,24 +3874,24 @@
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24" t="s">
         <v>148</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3778,13 +3902,13 @@
         <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3792,10 +3916,10 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3803,13 +3927,13 @@
         <v>48</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3817,13 +3941,13 @@
         <v>48</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C30" t="s">
-        <v>153</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3831,13 +3955,13 @@
         <v>48</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3845,10 +3969,10 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3856,13 +3980,13 @@
         <v>48</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3876,74 +4000,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" t="s">
         <v>163</v>
       </c>
-      <c r="B38" t="s">
-        <v>164</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B39" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B40" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B41" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B43" t="s">
+        <v>174</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3951,30 +4075,30 @@
     </row>
     <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" t="s">
         <v>177</v>
       </c>
-      <c r="B45" t="s">
-        <v>178</v>
-      </c>
       <c r="D45" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: another hack to deal with inacurate traning status bug
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA87D978-2D25-47E7-B7AA-06E164584A69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A58D565-4CCB-4290-8A8E-202153735659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="309">
   <si>
     <t>Page</t>
   </si>
@@ -1009,6 +1009,21 @@
   </si>
   <si>
     <t>"Save As Is" for a Train Dialog should update the Last Modified Time (bug 2092)</t>
+  </si>
+  <si>
+    <t>Edit Dialog</t>
+  </si>
+  <si>
+    <t>Modify Entity label on a user turn, should not be able to select any user turns nor do anything thing that would cause the change to be lost (bug 2075)</t>
+  </si>
+  <si>
+    <t>Copy Model</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Copy a model and verify that modifications to a Train Dialog in the copy does not affect the original. See (bug 2065) for exact steps.</t>
   </si>
 </sst>
 </file>
@@ -1576,11 +1591,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F155"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A156" sqref="A156"/>
+      <selection pane="bottomLeft" activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,6 +3628,34 @@
       </c>
       <c r="D155" s="3" t="s">
         <v>303</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>48</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C156" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>12</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C157" t="s">
+        <v>307</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entity labeling fix (#1155)
* fix: update package-lock.json

* fix: updated the test grid spread sheet

* fix: another hack to deal with inacurate traning status bug
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A34DBC-BBDE-4C88-A4B8-41C971738865}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A58D565-4CCB-4290-8A8E-202153735659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="309">
   <si>
     <t>Page</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>Bot should respond to user utterance with expected response due to existing Train Dialogs</t>
-  </si>
-  <si>
-    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn should not delete the description field. (Bug 2026)</t>
   </si>
   <si>
     <t>Editing a Bot turn that is the last turn, and the user creates a new EndSession Action, it should automaticaly replace the existing Bot turn with that newly created EndSession Action. (Bug 2014)</t>
@@ -874,9 +871,6 @@
   </si>
   <si>
     <t>Edit existing Log Dialog, then delete should remove the log dialog from the list.</t>
-  </si>
-  <si>
-    <t>Abandon button should discard ALL Log Dialog sessions and not persist any of them when multiple Log Dialog sessions are created via invoking an EndSession action and then it is followed up by another round of multiple Log Dialogs sessions that are ultimately saved. (bug 2111)</t>
   </si>
   <si>
     <t>Multi-Value, Memory Panel</t>
@@ -952,12 +946,91 @@
   <si>
     <t>By using the column filtering feature employed in this sheet you can focus in on a specific test spec file, or specific feature or area you are interested in. For example, if you want to know what scenarios and tests we have that deal with Entities, you could filter the “Feature” column by “entit” to limit the view to just tests dealing with Entities.</t>
   </si>
+  <si>
+    <t>Log multiple dialogs (3) that each invoke an EndSession action - then abandon it - again log multiple log dialogs (3) that each invoke an EndSession action - then save it. Verify that log dialogs ONLY saved the ones we saved and abandoned the ones we had abandoned. (bug 2111)</t>
+  </si>
+  <si>
+    <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn should not delete the description field and should not result in an extra TD. (Bug 2026)</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Abandoning a Train Dialog should cause model to forget the training that was in progress. (bug 2105)</t>
+  </si>
+  <si>
+    <t>Bot Response</t>
+  </si>
+  <si>
+    <r>
+      <t>Bot response should appear after Action selection (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AND SOME CONDITION THAT WE NEED MATT TO TELL US ABOUT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) (bug 2014)</t>
+    </r>
+  </si>
+  <si>
+    <t>Tree View</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Clicking on the 1st, last or any turn in Tree View should take you to the Train Dialog (bug 2097)</t>
+  </si>
+  <si>
+    <t>Click on a turn that comes after labeling an entity and it should show the Entity Detection and Memory panes. (bug 2096)</t>
+  </si>
+  <si>
+    <t>Merge Dialog</t>
+  </si>
+  <si>
+    <t>Save As Is</t>
+  </si>
+  <si>
+    <t>Merge Dialog Modal</t>
+  </si>
+  <si>
+    <t>"Save As Is" for a Train Dialog should update the Last Modified Time (bug 2092)</t>
+  </si>
+  <si>
+    <t>Edit Dialog</t>
+  </si>
+  <si>
+    <t>Modify Entity label on a user turn, should not be able to select any user turns nor do anything thing that would cause the change to be lost (bug 2075)</t>
+  </si>
+  <si>
+    <t>Copy Model</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Copy a model and verify that modifications to a Train Dialog in the copy does not affect the original. See (bug 2065) for exact steps.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1007,6 +1080,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1113,8 +1193,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F148" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F148" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F149" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F149" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="3"/>
@@ -1439,68 +1519,68 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>288</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1511,16 +1591,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81.28515625" style="3" customWidth="1"/>
@@ -1555,7 +1635,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -1569,16 +1649,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1586,16 +1666,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1603,16 +1683,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1620,16 +1700,16 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1637,16 +1717,16 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1654,16 +1734,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1671,16 +1751,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1688,16 +1768,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,13 +1785,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1719,13 +1799,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1733,13 +1813,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,13 +1827,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1761,13 +1841,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1775,13 +1855,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1798,7 +1878,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1812,10 +1892,10 @@
         <v>28</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1829,7 +1909,7 @@
         <v>28</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1843,7 +1923,7 @@
         <v>28</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,10 +1937,10 @@
         <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,13 +1948,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1882,13 +1962,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1896,13 +1976,13 @@
         <v>12</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1910,16 +1990,16 @@
         <v>12</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1927,16 +2007,16 @@
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1944,16 +2024,16 @@
         <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1961,13 +2041,13 @@
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2001,10 +2081,10 @@
         <v>21</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2018,7 +2098,7 @@
         <v>17</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2026,13 +2106,13 @@
         <v>12</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,13 +2120,13 @@
         <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2054,13 +2134,13 @@
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2068,13 +2148,13 @@
         <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2091,7 +2171,7 @@
         <v>89</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2105,10 +2185,10 @@
         <v>30</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2122,10 +2202,10 @@
         <v>30</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2139,10 +2219,10 @@
         <v>30</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2150,16 +2230,16 @@
         <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2167,16 +2247,16 @@
         <v>31</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2184,16 +2264,16 @@
         <v>31</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" t="s">
         <v>30</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2210,7 +2290,7 @@
         <v>34</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2227,7 +2307,7 @@
         <v>35</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2244,7 +2324,7 @@
         <v>36</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2258,10 +2338,10 @@
         <v>30</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2278,7 +2358,7 @@
         <v>90</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2295,7 +2375,7 @@
         <v>53</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2312,7 +2392,7 @@
         <v>59</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2329,7 +2409,7 @@
         <v>61</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2346,7 +2426,7 @@
         <v>60</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2363,7 +2443,7 @@
         <v>54</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2380,7 +2460,7 @@
         <v>65</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2394,10 +2474,10 @@
         <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -2411,7 +2491,7 @@
         <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -2419,13 +2499,13 @@
         <v>48</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2442,7 +2522,7 @@
         <v>41</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2459,7 +2539,7 @@
         <v>55</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2476,7 +2556,7 @@
         <v>45</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2493,7 +2573,7 @@
         <v>42</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2510,7 +2590,7 @@
         <v>63</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2527,7 +2607,7 @@
         <v>47</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,7 +2624,7 @@
         <v>46</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2561,7 +2641,7 @@
         <v>56</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2578,7 +2658,7 @@
         <v>57</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2595,7 +2675,7 @@
         <v>43</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2612,7 +2692,7 @@
         <v>44</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2660,7 +2740,7 @@
         <v>66</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2674,10 +2754,10 @@
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2691,26 +2771,26 @@
         <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2727,7 +2807,7 @@
         <v>71</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2744,7 +2824,7 @@
         <v>72</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2761,7 +2841,7 @@
         <v>73</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2778,7 +2858,7 @@
         <v>74</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2795,7 +2875,7 @@
         <v>75</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2812,7 +2892,7 @@
         <v>76</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2829,7 +2909,7 @@
         <v>77</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2846,7 +2926,7 @@
         <v>78</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2863,7 +2943,7 @@
         <v>79</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2880,7 +2960,7 @@
         <v>81</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2897,7 +2977,7 @@
         <v>80</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2914,7 +2994,7 @@
         <v>82</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2931,7 +3011,7 @@
         <v>83</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2956,7 +3036,7 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3028,7 +3108,7 @@
         <v>86</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3042,7 +3122,7 @@
         <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3059,7 +3139,7 @@
         <v>85</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3073,7 +3153,7 @@
         <v>14</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3090,7 +3170,7 @@
         <v>87</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3104,7 +3184,7 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3118,7 +3198,7 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -3132,7 +3212,7 @@
         <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3146,7 +3226,7 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3163,7 +3243,7 @@
         <v>88</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3177,10 +3257,10 @@
         <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>93</v>
+        <v>291</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3194,10 +3274,10 @@
         <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3211,7 +3291,7 @@
         <v>14</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3225,41 +3305,10 @@
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>15</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C124" t="s">
-        <v>15</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>15</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C125" t="s">
-        <v>15</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>15</v>
       </c>
@@ -3270,10 +3319,13 @@
         <v>15</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>15</v>
       </c>
@@ -3284,7 +3336,7 @@
         <v>15</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>277</v>
+        <v>91</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3298,7 +3350,7 @@
         <v>15</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3312,10 +3364,10 @@
         <v>15</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -3326,7 +3378,7 @@
         <v>15</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3339,22 +3391,22 @@
       <c r="C131" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>3</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="C134" t="s">
-        <v>8</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>281</v>
+      <c r="D131" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>15</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C132" t="s">
+        <v>15</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3362,13 +3414,16 @@
         <v>3</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>280</v>
+        <v>24</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3376,30 +3431,30 @@
         <v>3</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E136" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>3</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3407,13 +3462,13 @@
         <v>3</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>4</v>
+        <v>277</v>
       </c>
       <c r="C138" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3424,24 +3479,24 @@
         <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>3</v>
       </c>
-      <c r="B141" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C141" t="s">
-        <v>10</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>26</v>
+      <c r="B140" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" t="s">
+        <v>11</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3452,7 +3507,7 @@
         <v>5</v>
       </c>
       <c r="C142" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>26</v>
@@ -3462,33 +3517,145 @@
       <c r="A143" t="s">
         <v>3</v>
       </c>
+      <c r="B143" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>3</v>
       </c>
-      <c r="B144" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>48</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C151" t="s">
+        <v>14</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>48</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C152" t="s">
+        <v>14</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>297</v>
+      </c>
+      <c r="B153" t="s">
+        <v>296</v>
+      </c>
+      <c r="C153" t="s">
+        <v>296</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>297</v>
+      </c>
+      <c r="B154" t="s">
+        <v>296</v>
+      </c>
+      <c r="C154" t="s">
+        <v>296</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>300</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C155" t="s">
+        <v>302</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>48</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C156" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>12</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C157" t="s">
+        <v>307</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3518,111 +3685,111 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3630,38 +3797,38 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3675,7 +3842,7 @@
         <v>84</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3683,7 +3850,7 @@
         <v>84</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3692,57 +3859,57 @@
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" t="s">
         <v>139</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B22" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3750,24 +3917,24 @@
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24" t="s">
         <v>148</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3778,13 +3945,13 @@
         <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3792,10 +3959,10 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3803,13 +3970,13 @@
         <v>48</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3817,13 +3984,13 @@
         <v>48</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C30" t="s">
-        <v>153</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3831,13 +3998,13 @@
         <v>48</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3845,10 +4012,10 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3856,13 +4023,13 @@
         <v>48</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3876,74 +4043,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" t="s">
         <v>163</v>
       </c>
-      <c r="B38" t="s">
-        <v>164</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B39" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B40" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B41" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B43" t="s">
+        <v>174</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3951,30 +4118,30 @@
     </row>
     <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" t="s">
         <v>177</v>
       </c>
-      <c r="B45" t="s">
-        <v>178</v>
-      </c>
       <c r="D45" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: all scenarios from test videos are in the grid
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DED358-125F-4A6E-AB27-A1DA68D05EE2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA4A435-C4E3-40A9-A85D-8E3831922249}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="370">
   <si>
     <t>Page</t>
   </si>
@@ -1175,6 +1175,18 @@
   </si>
   <si>
     <t>Verify that "Type your message" input box is present when editing a TD that ended with a Bot turn</t>
+  </si>
+  <si>
+    <t>Card Action</t>
+  </si>
+  <si>
+    <t>Verify that buttons clicked on a card causes a user turn to be appended to the end of the chat. Even if the card popped up many turns earlier in the chat.</t>
+  </si>
+  <si>
+    <t>see video "Prompts with buttons.mp4" for more info</t>
+  </si>
+  <si>
+    <t>see videos, "Render and Logic Errors.mp4, exception testing.mp4, API Call Cards.mp4" for more info</t>
   </si>
 </sst>
 </file>
@@ -1759,11 +1771,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F196"/>
+  <dimension ref="A1:F197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D80" sqref="D80"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4459,7 +4471,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>12</v>
       </c>
@@ -4476,7 +4488,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -4492,8 +4504,11 @@
       <c r="E179" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F179" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>48</v>
       </c>
@@ -4509,8 +4524,11 @@
       <c r="E180" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F180" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -4526,8 +4544,11 @@
       <c r="E181" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F181" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -4543,8 +4564,11 @@
       <c r="E182" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F182" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>48</v>
       </c>
@@ -4560,8 +4584,11 @@
       <c r="E183" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F183" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -4577,8 +4604,11 @@
       <c r="E184" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F184" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>48</v>
       </c>
@@ -4594,8 +4624,11 @@
       <c r="E185" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F185" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>48</v>
       </c>
@@ -4611,8 +4644,11 @@
       <c r="E186" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F186" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>48</v>
       </c>
@@ -4628,8 +4664,11 @@
       <c r="E187" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F187" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>48</v>
       </c>
@@ -4645,8 +4684,11 @@
       <c r="E188" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F188" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>48</v>
       </c>
@@ -4662,8 +4704,11 @@
       <c r="E189" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F189" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>48</v>
       </c>
@@ -4680,7 +4725,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>48</v>
       </c>
@@ -4697,7 +4742,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>48</v>
       </c>
@@ -4786,6 +4831,26 @@
       </c>
       <c r="F196" s="3" t="s">
         <v>353</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>48</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C197" t="s">
+        <v>14</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="F197" s="3" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: calling it good for now
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA4A435-C4E3-40A9-A85D-8E3831922249}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB35E872-1798-40A9-9CAC-C224A656EBEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="371">
   <si>
     <t>Page</t>
   </si>
@@ -330,9 +330,6 @@
   </si>
   <si>
     <t>The Description field should be empty on a new Train Dialog after adding a Description to a Train Dialog then Scoring an EndSession Bot response. (Bug 2031)</t>
-  </si>
-  <si>
-    <t>Exporting a model after saving and EndSession Train Dialog should not result in a duplicate Train Dialog in the model. (Bug 2032)</t>
   </si>
   <si>
     <t>Editing an existing Train Dialog and finishing it up with an EndSession chat turn and saving it should not result in two Train Dialogs. (Bug 1969)</t>
@@ -1187,6 +1184,12 @@
   </si>
   <si>
     <t>see videos, "Render and Logic Errors.mp4, exception testing.mp4, API Call Cards.mp4" for more info</t>
+  </si>
+  <si>
+    <t>Create a Train Dialog with two User turn in a row - validate the error - type in a new user input - validate the User turn with the error is not deleted (bug 2119)</t>
+  </si>
+  <si>
+    <t>Exporting a model after saving a Train Dialog with an EndSession in it should not result in a duplicate Train Dialog in the model. (Bug 2032)</t>
   </si>
 </sst>
 </file>
@@ -1370,8 +1373,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F219" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F219" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F220" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F220" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="3"/>
@@ -1696,42 +1699,42 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1739,28 +1742,28 @@
     </row>
     <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1771,11 +1774,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F197"/>
+  <dimension ref="A1:F198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E189" sqref="E189"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,7 +1818,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -1824,7 +1827,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1832,16 +1835,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1849,16 +1852,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1866,16 +1869,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1883,16 +1886,16 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1900,16 +1903,16 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,16 +1920,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1934,16 +1937,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1951,16 +1954,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1968,19 +1971,19 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1988,19 +1991,19 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2008,19 +2011,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2028,24 +2031,24 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E15" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2053,16 +2056,16 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2070,16 +2073,16 @@
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2087,16 +2090,16 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C18" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2104,16 +2107,16 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C19" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2121,16 +2124,16 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2138,16 +2141,16 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C21" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2164,7 +2167,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2178,10 +2181,10 @@
         <v>28</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2195,10 +2198,10 @@
         <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2212,10 +2215,10 @@
         <v>28</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2229,10 +2232,10 @@
         <v>28</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2240,16 +2243,16 @@
         <v>12</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2257,16 +2260,16 @@
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2274,16 +2277,16 @@
         <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -2291,16 +2294,16 @@
         <v>12</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C32" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2308,16 +2311,16 @@
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C33" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2325,19 +2328,19 @@
         <v>12</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2345,16 +2348,16 @@
         <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C35" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2371,7 +2374,7 @@
         <v>23</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>29</v>
@@ -2391,10 +2394,10 @@
         <v>21</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2411,7 +2414,7 @@
         <v>97</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2419,16 +2422,16 @@
         <v>12</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2436,16 +2439,16 @@
         <v>12</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C41" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2453,16 +2456,16 @@
         <v>12</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2470,16 +2473,16 @@
         <v>12</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2496,7 +2499,7 @@
         <v>89</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2510,10 +2513,10 @@
         <v>30</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2527,10 +2530,10 @@
         <v>30</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2544,10 +2547,10 @@
         <v>30</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2555,16 +2558,16 @@
         <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" t="s">
         <v>30</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2572,16 +2575,16 @@
         <v>31</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C51" t="s">
         <v>30</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2589,16 +2592,16 @@
         <v>31</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
       </c>
       <c r="D52" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2615,7 +2618,7 @@
         <v>34</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2632,7 +2635,7 @@
         <v>35</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2649,7 +2652,7 @@
         <v>36</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2663,10 +2666,10 @@
         <v>30</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2683,7 +2686,7 @@
         <v>90</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2697,10 +2700,10 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,10 +2717,10 @@
         <v>14</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2731,10 +2734,10 @@
         <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2748,10 +2751,10 @@
         <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2765,10 +2768,10 @@
         <v>14</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2782,10 +2785,10 @@
         <v>14</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2799,10 +2802,10 @@
         <v>14</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2816,10 +2819,10 @@
         <v>14</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2836,7 +2839,7 @@
         <v>53</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,7 +2856,7 @@
         <v>59</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2870,7 +2873,7 @@
         <v>61</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2887,7 +2890,7 @@
         <v>60</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2904,7 +2907,7 @@
         <v>54</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2921,7 +2924,7 @@
         <v>65</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2935,10 +2938,10 @@
         <v>14</v>
       </c>
       <c r="D74" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -2952,10 +2955,10 @@
         <v>14</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2969,10 +2972,10 @@
         <v>14</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2986,10 +2989,10 @@
         <v>14</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2997,16 +3000,16 @@
         <v>48</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C78" t="s">
         <v>14</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3014,16 +3017,16 @@
         <v>48</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C79" t="s">
         <v>14</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -3031,16 +3034,16 @@
         <v>48</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C81" t="s">
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3057,7 +3060,7 @@
         <v>41</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3074,7 +3077,7 @@
         <v>55</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3091,7 +3094,7 @@
         <v>45</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3108,7 +3111,7 @@
         <v>42</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3125,7 +3128,7 @@
         <v>63</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3142,7 +3145,7 @@
         <v>47</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3159,7 +3162,7 @@
         <v>46</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3176,7 +3179,7 @@
         <v>56</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3193,7 +3196,7 @@
         <v>57</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3210,7 +3213,7 @@
         <v>43</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3227,7 +3230,7 @@
         <v>44</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3244,7 +3247,7 @@
         <v>49</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>52</v>
@@ -3264,7 +3267,7 @@
         <v>50</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3281,7 +3284,7 @@
         <v>66</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3295,10 +3298,10 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3312,10 +3315,10 @@
         <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3329,10 +3332,10 @@
         <v>14</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3346,10 +3349,10 @@
         <v>14</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3363,10 +3366,10 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3380,10 +3383,10 @@
         <v>14</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3397,10 +3400,10 @@
         <v>14</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3414,10 +3417,10 @@
         <v>14</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3431,10 +3434,10 @@
         <v>14</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3448,10 +3451,10 @@
         <v>14</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3465,13 +3468,13 @@
         <v>14</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3485,13 +3488,13 @@
         <v>14</v>
       </c>
       <c r="D109" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F109" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3508,7 +3511,7 @@
         <v>71</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3525,7 +3528,7 @@
         <v>72</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3542,7 +3545,7 @@
         <v>73</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3559,7 +3562,7 @@
         <v>74</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3576,7 +3579,7 @@
         <v>75</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3593,7 +3596,7 @@
         <v>76</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3610,7 +3613,7 @@
         <v>77</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3627,7 +3630,7 @@
         <v>78</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3644,7 +3647,7 @@
         <v>79</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3661,7 +3664,7 @@
         <v>81</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3678,7 +3681,7 @@
         <v>80</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3695,7 +3698,7 @@
         <v>82</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3712,7 +3715,7 @@
         <v>83</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3726,10 +3729,10 @@
         <v>14</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3743,13 +3746,13 @@
         <v>14</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3757,19 +3760,19 @@
         <v>48</v>
       </c>
       <c r="B127" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C127" t="s">
+        <v>14</v>
+      </c>
+      <c r="D127" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="C127" t="s">
-        <v>14</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>336</v>
-      </c>
       <c r="E127" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3783,13 +3786,13 @@
         <v>14</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3803,13 +3806,13 @@
         <v>14</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3823,33 +3826,33 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F130" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="E130" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>48</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C132" t="s">
-        <v>14</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E132" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>48</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C131" t="s">
+        <v>14</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>48</v>
       </c>
@@ -3860,13 +3863,13 @@
         <v>14</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>267</v>
+        <v>86</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>48</v>
       </c>
@@ -3877,10 +3880,10 @@
         <v>14</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>85</v>
+        <v>266</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>246</v>
+        <v>303</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -3893,11 +3896,14 @@
       <c r="C135" t="s">
         <v>14</v>
       </c>
+      <c r="D135" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E135" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>48</v>
       </c>
@@ -3907,11 +3913,8 @@
       <c r="C136" t="s">
         <v>14</v>
       </c>
-      <c r="D136" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="E136" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3925,13 +3928,13 @@
         <v>14</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>48</v>
       </c>
@@ -3942,13 +3945,13 @@
         <v>14</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>48</v>
       </c>
@@ -3959,13 +3962,13 @@
         <v>14</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>48</v>
       </c>
@@ -3976,13 +3979,13 @@
         <v>14</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>48</v>
       </c>
@@ -3993,10 +3996,10 @@
         <v>14</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>246</v>
+        <v>303</v>
       </c>
     </row>
     <row r="142" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4010,10 +4013,10 @@
         <v>14</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>285</v>
+        <v>88</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4027,10 +4030,10 @@
         <v>14</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>100</v>
+        <v>284</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4047,7 +4050,7 @@
         <v>99</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>304</v>
+        <v>267</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4061,30 +4064,30 @@
         <v>14</v>
       </c>
       <c r="D145" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>48</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C146" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E145" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>15</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C149" t="s">
-        <v>15</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E146" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>15</v>
       </c>
@@ -4095,13 +4098,13 @@
         <v>15</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>15</v>
       </c>
@@ -4112,10 +4115,10 @@
         <v>15</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>271</v>
+        <v>91</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4129,10 +4132,10 @@
         <v>15</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4146,13 +4149,13 @@
         <v>15</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>15</v>
       </c>
@@ -4163,10 +4166,10 @@
         <v>15</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>342</v>
+        <v>269</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4180,47 +4183,47 @@
         <v>15</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F155" s="3" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>15</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C156" t="s">
         <v>15</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>284</v>
+        <v>342</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>3</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="C159" t="s">
-        <v>8</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>275</v>
+        <v>303</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>15</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C157" t="s">
+        <v>15</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4228,16 +4231,16 @@
         <v>3</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C160" t="s">
         <v>8</v>
       </c>
       <c r="D160" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E160" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="E160" s="3" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -4245,33 +4248,33 @@
         <v>3</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C161" t="s">
         <v>8</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>67</v>
+        <v>273</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>3</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C162" t="s">
         <v>8</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>304</v>
+        <v>242</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4279,16 +4282,16 @@
         <v>3</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>4</v>
+        <v>272</v>
       </c>
       <c r="C163" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4299,35 +4302,35 @@
         <v>4</v>
       </c>
       <c r="C164" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>3</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C165" t="s">
+        <v>11</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E165" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>3</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C166" t="s">
-        <v>10</v>
-      </c>
-      <c r="D166" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="E166" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4338,174 +4341,171 @@
         <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B168" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C168" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>3</v>
       </c>
-      <c r="B169" s="3" t="s">
+    </row>
+    <row r="170" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>3</v>
+      </c>
+      <c r="B170" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C170" t="s">
+        <v>306</v>
+      </c>
+      <c r="D170" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D169" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>48</v>
-      </c>
-      <c r="B171" s="3" t="s">
+      <c r="E170" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>48</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C172" t="s">
+        <v>14</v>
+      </c>
+      <c r="D172" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C171" t="s">
-        <v>14</v>
-      </c>
-      <c r="D171" s="3" t="s">
+      <c r="E172" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>48</v>
+      </c>
+      <c r="B173" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="E171" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>48</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C172" t="s">
-        <v>14</v>
-      </c>
-      <c r="D172" s="3" t="s">
+      <c r="C173" t="s">
+        <v>14</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E173" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>290</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C173" t="s">
-        <v>289</v>
-      </c>
-      <c r="D173" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E173" s="3" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>289</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C174" t="s">
+        <v>288</v>
+      </c>
+      <c r="D174" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B174" s="3" t="s">
+      <c r="E174" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>289</v>
       </c>
-      <c r="C174" t="s">
-        <v>289</v>
-      </c>
-      <c r="D174" s="3" t="s">
+      <c r="B175" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C175" t="s">
+        <v>288</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>292</v>
       </c>
-      <c r="E174" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="B176" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B175" s="3" t="s">
+      <c r="C176" t="s">
         <v>294</v>
       </c>
-      <c r="C175" t="s">
+      <c r="D176" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="D175" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="E175" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>48</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="C176" t="s">
-        <v>14</v>
-      </c>
-      <c r="D176" s="3" t="s">
-        <v>298</v>
-      </c>
       <c r="E176" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>48</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C177" t="s">
+        <v>14</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>12</v>
       </c>
-      <c r="B177" s="3" t="s">
+      <c r="B178" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C178" t="s">
         <v>299</v>
       </c>
-      <c r="C177" t="s">
+      <c r="D178" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="D177" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="E177" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>48</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C179" t="s">
-        <v>14</v>
-      </c>
-      <c r="D179" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="E179" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F179" s="3" t="s">
-        <v>369</v>
+      <c r="E178" s="3" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4513,19 +4513,19 @@
         <v>48</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C180" t="s">
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4533,19 +4533,19 @@
         <v>48</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C181" t="s">
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4553,19 +4553,19 @@
         <v>48</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C182" t="s">
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4573,19 +4573,19 @@
         <v>48</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C183" t="s">
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4593,7 +4593,7 @@
         <v>48</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C184" t="s">
         <v>14</v>
@@ -4602,10 +4602,10 @@
         <v>324</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4613,19 +4613,19 @@
         <v>48</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C185" t="s">
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4633,82 +4633,82 @@
         <v>48</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C186" t="s">
         <v>14</v>
       </c>
       <c r="D186" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>48</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C187" t="s">
+        <v>14</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>48</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C188" t="s">
+        <v>14</v>
+      </c>
+      <c r="D188" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="E186" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F186" s="3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>48</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C187" t="s">
-        <v>14</v>
-      </c>
-      <c r="D187" s="3" t="s">
+      <c r="E188" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>48</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C189" t="s">
+        <v>14</v>
+      </c>
+      <c r="D189" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E187" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F187" s="3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>48</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C188" t="s">
-        <v>14</v>
-      </c>
-      <c r="D188" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="E188" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F188" s="3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>48</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C189" t="s">
-        <v>14</v>
-      </c>
-      <c r="D189" s="3" t="s">
-        <v>326</v>
-      </c>
       <c r="E189" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>48</v>
       </c>
@@ -4719,10 +4719,13 @@
         <v>14</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4730,7 +4733,7 @@
         <v>48</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C191" t="s">
         <v>14</v>
@@ -4739,7 +4742,7 @@
         <v>348</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4747,33 +4750,33 @@
         <v>48</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C192" t="s">
         <v>14</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>48</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C193" t="s">
         <v>14</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E193" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4781,16 +4784,16 @@
         <v>48</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C194" t="s">
         <v>14</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4798,19 +4801,16 @@
         <v>48</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C195" t="s">
         <v>14</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E195" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F195" s="3" t="s">
-        <v>353</v>
+        <v>303</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4818,7 +4818,7 @@
         <v>48</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C196" t="s">
         <v>14</v>
@@ -4827,10 +4827,10 @@
         <v>351</v>
       </c>
       <c r="E196" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F196" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4838,19 +4838,39 @@
         <v>48</v>
       </c>
       <c r="B197" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C197" t="s">
+        <v>14</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F197" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>48</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C198" t="s">
+        <v>14</v>
+      </c>
+      <c r="D198" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="C197" t="s">
-        <v>14</v>
-      </c>
-      <c r="D197" s="3" t="s">
+      <c r="E198" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F198" s="3" t="s">
         <v>367</v>
-      </c>
-      <c r="E197" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F197" s="3" t="s">
-        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -4880,111 +4900,111 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
         <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="C7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4992,38 +5012,38 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5037,7 +5057,7 @@
         <v>84</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5045,7 +5065,7 @@
         <v>84</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -5054,57 +5074,57 @@
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
         <v>138</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5112,24 +5132,24 @@
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" t="s">
         <v>147</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5140,13 +5160,13 @@
         <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5154,10 +5174,10 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5165,13 +5185,13 @@
         <v>48</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -5179,13 +5199,13 @@
         <v>48</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="C30" t="s">
-        <v>152</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -5193,13 +5213,13 @@
         <v>48</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5207,10 +5227,10 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5218,13 +5238,13 @@
         <v>48</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5238,74 +5258,74 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" t="s">
         <v>162</v>
       </c>
-      <c r="B38" t="s">
-        <v>163</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B39" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B41" t="s">
+        <v>169</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B42" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B43" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -5313,30 +5333,30 @@
     </row>
     <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" t="s">
         <v>176</v>
       </c>
-      <c r="B45" t="s">
-        <v>177</v>
-      </c>
       <c r="D45" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D47" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: found more blank rows to delete
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB35E872-1798-40A9-9CAC-C224A656EBEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E83F43-4423-4F92-B161-7C293AB92A31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="367">
   <si>
     <t>Page</t>
   </si>
@@ -838,9 +838,6 @@
   </si>
   <si>
     <t>ErrorHandling/WaitNonWait</t>
-  </si>
-  <si>
-    <t>TODO: There are more error messages to validate</t>
   </si>
   <si>
     <t>Score Action for the last Bot turn that is already an EndSession should enable all EndSession Actions.</t>
@@ -938,9 +935,6 @@
     <t>Abandoning a Train Dialog should cause model to forget the training that was in progress. (bug 2105)</t>
   </si>
   <si>
-    <t>Bot Response</t>
-  </si>
-  <si>
     <t>Tree View</t>
   </si>
   <si>
@@ -978,12 +972,6 @@
   </si>
   <si>
     <t>Copy a model and verify that modifications to a Train Dialog in the copy does not affect the original. See (bug 2065) for exact steps.</t>
-  </si>
-  <si>
-    <t>(place holder for bug 2104 - can't easily create automated test for this one)</t>
-  </si>
-  <si>
-    <t>cannot automate</t>
   </si>
   <si>
     <t>todo</t>
@@ -1196,7 +1184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1250,15 +1238,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1268,11 +1249,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1294,13 +1270,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1329,14 +1304,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -1373,8 +1344,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F220" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F220" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F195" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F195" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="3"/>
@@ -1742,28 +1713,28 @@
     </row>
     <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -1774,11 +1745,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F198"/>
+  <dimension ref="A1:F173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D157" sqref="D157"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,7 +1798,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1977,13 +1948,13 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>215</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1997,13 +1968,13 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2017,13 +1988,13 @@
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2037,21 +2008,33 @@
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2062,13 +2045,13 @@
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2079,30 +2062,30 @@
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C18" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2113,13 +2096,13 @@
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -2130,30 +2113,47 @@
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>198</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>203</v>
+        <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -2164,13 +2164,13 @@
         <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>20</v>
+        <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2181,13 +2181,13 @@
         <v>28</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2198,166 +2198,206 @@
         <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>13</v>
+        <v>192</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>13</v>
+        <v>201</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>224</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>222</v>
+        <v>23</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>225</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>227</v>
+        <v>21</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>303</v>
+        <v>259</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>226</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>221</v>
+        <v>97</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2365,124 +2405,152 @@
         <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>23</v>
+        <v>183</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>21</v>
+        <v>186</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>22</v>
+        <v>185</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>97</v>
+        <v>187</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>180</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>182</v>
+        <v>89</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>181</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>183</v>
+        <v>235</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>184</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>186</v>
+        <v>236</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>303</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>185</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>303</v>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2490,33 +2558,33 @@
         <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>89</v>
+        <v>237</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>235</v>
+        <v>34</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2524,16 +2592,16 @@
         <v>31</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C48" t="s">
         <v>30</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>236</v>
+        <v>35</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2541,152 +2609,169 @@
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C49" t="s">
         <v>30</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>234</v>
+        <v>36</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>101</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
         <v>30</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="C51" t="s">
         <v>30</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>101</v>
+        <v>33</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>237</v>
+        <v>350</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>238</v>
+        <v>299</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>34</v>
+        <v>351</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C54" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>35</v>
+        <v>352</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>36</v>
+        <v>353</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>100</v>
+        <v>354</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>241</v>
+        <v>299</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C57" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>90</v>
+        <v>349</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>242</v>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2700,10 +2785,10 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2711,16 +2796,16 @@
         <v>48</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>355</v>
+        <v>53</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>303</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2728,16 +2813,16 @@
         <v>48</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>356</v>
+        <v>59</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>303</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2745,16 +2830,16 @@
         <v>48</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>357</v>
+        <v>61</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>303</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2762,16 +2847,16 @@
         <v>48</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>358</v>
+        <v>60</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>303</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2779,33 +2864,33 @@
         <v>48</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>353</v>
+        <v>54</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C65" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>359</v>
+        <v>65</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2813,16 +2898,33 @@
         <v>48</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C66" t="s">
         <v>14</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>360</v>
+        <v>244</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>303</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2836,10 +2938,10 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>53</v>
+        <v>357</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>243</v>
+        <v>299</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,129 +2955,129 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>59</v>
+        <v>358</v>
       </c>
       <c r="E69" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>48</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>48</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C70" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E70" s="3" t="s">
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C74" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>48</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C71" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>48</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C72" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>48</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C73" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>48</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C74" t="s">
-        <v>14</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>48</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C75" t="s">
         <v>14</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>206</v>
+        <v>45</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>48</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C76" t="s">
         <v>14</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>361</v>
+        <v>42</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>303</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2983,70 +3085,104 @@
         <v>48</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C77" t="s">
         <v>14</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>362</v>
+        <v>63</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>48</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>296</v>
+        <v>40</v>
       </c>
       <c r="C78" t="s">
         <v>14</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>363</v>
+        <v>47</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>48</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>296</v>
+        <v>40</v>
       </c>
       <c r="C79" t="s">
         <v>14</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>364</v>
+        <v>46</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>48</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>205</v>
+        <v>40</v>
       </c>
       <c r="C81" t="s">
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>207</v>
+        <v>57</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>48</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -3057,7 +3193,7 @@
         <v>14</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>243</v>
@@ -3074,13 +3210,16 @@
         <v>14</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -3091,10 +3230,10 @@
         <v>14</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>246</v>
+        <v>299</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3102,33 +3241,33 @@
         <v>48</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C86" t="s">
         <v>14</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>48</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C87" t="s">
         <v>14</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3136,141 +3275,155 @@
         <v>48</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C88" t="s">
         <v>14</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>47</v>
+        <v>258</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>48</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C89" t="s">
         <v>14</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>46</v>
+        <v>312</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>48</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C90" t="s">
         <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>56</v>
+        <v>305</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>48</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C91" t="s">
         <v>14</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>57</v>
+        <v>311</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C92" t="s">
         <v>14</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>43</v>
+        <v>306</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C93" t="s">
         <v>14</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>44</v>
+        <v>310</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>48</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C94" t="s">
         <v>14</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>49</v>
+        <v>307</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>48</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C95" t="s">
         <v>14</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>50</v>
+        <v>309</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>48</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C96" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -3281,10 +3434,13 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>66</v>
+        <v>340</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>256</v>
+        <v>299</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3298,27 +3454,30 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>257</v>
+        <v>341</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>48</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C99" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>258</v>
+        <v>71</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>238</v>
+        <v>277</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3326,16 +3485,16 @@
         <v>48</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C100" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>316</v>
+        <v>72</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3343,16 +3502,16 @@
         <v>48</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C101" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>309</v>
+        <v>73</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3360,16 +3519,16 @@
         <v>48</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C102" t="s">
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>315</v>
+        <v>74</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3377,104 +3536,101 @@
         <v>48</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C103" t="s">
         <v>14</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>310</v>
+        <v>75</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C104" t="s">
         <v>14</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>314</v>
+      <c r="D104" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C105" t="s">
         <v>14</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>311</v>
+      <c r="D105" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>48</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C106" t="s">
         <v>14</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>313</v>
+      <c r="D106" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>48</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C107" t="s">
         <v>14</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>312</v>
+      <c r="D107" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>48</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>344</v>
+      <c r="D108" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>346</v>
+        <v>264</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3482,22 +3638,36 @@
         <v>48</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C109" t="s">
         <v>14</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>345</v>
+      <c r="D109" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>48</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C110" t="s">
+        <v>14</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -3505,16 +3675,16 @@
         <v>70</v>
       </c>
       <c r="C111" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>48</v>
       </c>
@@ -3522,33 +3692,39 @@
         <v>70</v>
       </c>
       <c r="C112" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>72</v>
+        <v>329</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>48</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>70</v>
+        <v>330</v>
       </c>
       <c r="C113" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>73</v>
+        <v>331</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -3559,13 +3735,16 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>74</v>
+        <v>332</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>48</v>
       </c>
@@ -3576,10 +3755,13 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>75</v>
+        <v>333</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>278</v>
+        <v>299</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3592,11 +3774,14 @@
       <c r="C116" t="s">
         <v>14</v>
       </c>
-      <c r="D116" s="4" t="s">
-        <v>76</v>
+      <c r="D116" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>277</v>
+        <v>299</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3609,28 +3794,28 @@
       <c r="C117" t="s">
         <v>14</v>
       </c>
-      <c r="D117" s="4" t="s">
-        <v>77</v>
+      <c r="D117" s="3" t="s">
+        <v>365</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>48</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C118" t="s">
         <v>14</v>
       </c>
-      <c r="D118" s="4" t="s">
-        <v>78</v>
+      <c r="D118" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3638,50 +3823,47 @@
         <v>48</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C119" t="s">
         <v>14</v>
       </c>
-      <c r="D119" s="4" t="s">
-        <v>79</v>
+      <c r="D119" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>48</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C120" t="s">
         <v>14</v>
       </c>
-      <c r="D120" s="4" t="s">
-        <v>81</v>
+      <c r="D120" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>48</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C121" t="s">
         <v>14</v>
       </c>
-      <c r="D121" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="E121" s="3" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3689,16 +3871,16 @@
         <v>48</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C122" t="s">
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3706,53 +3888,67 @@
         <v>48</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C123" t="s">
         <v>14</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>48</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C124" t="s">
+        <v>14</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>48</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C125" t="s">
         <v>14</v>
       </c>
-      <c r="D125" s="14" t="s">
-        <v>265</v>
+      <c r="D125" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>48</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C126" t="s">
         <v>14</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>333</v>
+        <v>93</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F126" s="3" t="s">
-        <v>339</v>
+        <v>299</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3760,19 +3956,16 @@
         <v>48</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>334</v>
+        <v>84</v>
       </c>
       <c r="C127" t="s">
         <v>14</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>335</v>
+        <v>88</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F127" s="3" t="s">
-        <v>339</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3780,19 +3973,16 @@
         <v>48</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C128" t="s">
         <v>14</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>336</v>
+        <v>283</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F128" s="3" t="s">
-        <v>339</v>
+        <v>266</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3800,19 +3990,16 @@
         <v>48</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C129" t="s">
         <v>14</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>337</v>
+        <v>99</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F129" s="3" t="s">
-        <v>339</v>
+        <v>266</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3820,19 +4007,16 @@
         <v>48</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C130" t="s">
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>338</v>
+        <v>366</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>339</v>
+        <v>299</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3840,1037 +4024,775 @@
         <v>48</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C131" t="s">
         <v>14</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>369</v>
+        <v>98</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>15</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" t="s">
+        <v>15</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C133" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C134" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C135" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>85</v>
+        <v>267</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C136" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>268</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C137" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>87</v>
+        <v>337</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C138" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C139" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>94</v>
+        <v>282</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>84</v>
+        <v>270</v>
       </c>
       <c r="C140" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>303</v>
+        <v>273</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>84</v>
+        <v>274</v>
       </c>
       <c r="C141" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>93</v>
+        <v>272</v>
       </c>
       <c r="E141" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C142" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>3</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C143" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>3</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C144" t="s">
+        <v>10</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>3</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" t="s">
+        <v>11</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>3</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" t="s">
+        <v>10</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>3</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" t="s">
+        <v>11</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>3</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C148" t="s">
+        <v>302</v>
+      </c>
+      <c r="D148" s="3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>48</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C142" t="s">
-        <v>14</v>
-      </c>
-      <c r="D142" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E142" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>48</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C143" t="s">
-        <v>14</v>
-      </c>
-      <c r="D143" s="3" t="s">
+      <c r="E148" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>48</v>
+      </c>
+      <c r="B149" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="E143" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>48</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C144" t="s">
-        <v>14</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E144" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>48</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C145" t="s">
-        <v>14</v>
-      </c>
-      <c r="D145" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>48</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C146" t="s">
-        <v>14</v>
-      </c>
-      <c r="D146" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E146" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C149" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>15</v>
+        <v>287</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>15</v>
+        <v>286</v>
       </c>
       <c r="C150" t="s">
-        <v>15</v>
+        <v>286</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>92</v>
+        <v>288</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>15</v>
+        <v>287</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>15</v>
+        <v>286</v>
       </c>
       <c r="C151" t="s">
-        <v>15</v>
+        <v>286</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>91</v>
+        <v>289</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>15</v>
+        <v>290</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>15</v>
+        <v>291</v>
       </c>
       <c r="C152" t="s">
-        <v>15</v>
+        <v>292</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>15</v>
+        <v>294</v>
       </c>
       <c r="C153" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>15</v>
+        <v>296</v>
       </c>
       <c r="C154" t="s">
-        <v>15</v>
+        <v>297</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="C155" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="C156" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F156" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>48</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C157" t="s">
+        <v>14</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>48</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C158" t="s">
+        <v>14</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>48</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C159" t="s">
+        <v>14</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>48</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C160" t="s">
+        <v>14</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>48</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C161" t="s">
+        <v>14</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>48</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C162" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>48</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C163" t="s">
+        <v>14</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>48</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C164" t="s">
+        <v>14</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>48</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C165" t="s">
+        <v>14</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>48</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C166" t="s">
+        <v>14</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>48</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C167" t="s">
+        <v>14</v>
+      </c>
+      <c r="D167" s="3" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>15</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C157" t="s">
-        <v>15</v>
-      </c>
-      <c r="D157" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>3</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C160" t="s">
-        <v>8</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E160" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>3</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="C161" t="s">
-        <v>8</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>3</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C162" t="s">
-        <v>8</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>3</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="C163" t="s">
-        <v>8</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>3</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C164" t="s">
-        <v>10</v>
-      </c>
-      <c r="D164" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>3</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C165" t="s">
-        <v>11</v>
-      </c>
-      <c r="D165" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E166" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>3</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C167" t="s">
-        <v>10</v>
-      </c>
-      <c r="D167" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="E167" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>5</v>
+        <v>313</v>
       </c>
       <c r="C168" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>26</v>
+        <v>345</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C169" t="s">
+        <v>14</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>69</v>
+        <v>313</v>
       </c>
       <c r="C170" t="s">
-        <v>306</v>
+        <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>307</v>
+        <v>346</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>48</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C171" t="s">
+        <v>14</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>48</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>285</v>
+        <v>313</v>
       </c>
       <c r="C172" t="s">
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>286</v>
+        <v>346</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>48</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>287</v>
+        <v>361</v>
       </c>
       <c r="C173" t="s">
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>301</v>
+        <v>362</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>289</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C174" t="s">
-        <v>288</v>
-      </c>
-      <c r="D174" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="E174" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>289</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C175" t="s">
-        <v>288</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E175" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>292</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="C176" t="s">
-        <v>294</v>
-      </c>
-      <c r="D176" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="E176" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>48</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C177" t="s">
-        <v>14</v>
-      </c>
-      <c r="D177" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="E177" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>12</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C178" t="s">
-        <v>299</v>
-      </c>
-      <c r="D178" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="E178" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>48</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C180" t="s">
-        <v>14</v>
-      </c>
-      <c r="D180" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="E180" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F180" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>48</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C181" t="s">
-        <v>14</v>
-      </c>
-      <c r="D181" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="E181" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F181" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>48</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C182" t="s">
-        <v>14</v>
-      </c>
-      <c r="D182" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="E182" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F182" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>48</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C183" t="s">
-        <v>14</v>
-      </c>
-      <c r="D183" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="E183" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F183" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>48</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C184" t="s">
-        <v>14</v>
-      </c>
-      <c r="D184" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="E184" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F184" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>48</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C185" t="s">
-        <v>14</v>
-      </c>
-      <c r="D185" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="E185" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F185" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>48</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C186" t="s">
-        <v>14</v>
-      </c>
-      <c r="D186" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F186" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>48</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C187" t="s">
-        <v>14</v>
-      </c>
-      <c r="D187" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E187" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F187" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>48</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C188" t="s">
-        <v>14</v>
-      </c>
-      <c r="D188" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="E188" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F188" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>48</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C189" t="s">
-        <v>14</v>
-      </c>
-      <c r="D189" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E189" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F189" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>48</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C190" t="s">
-        <v>14</v>
-      </c>
-      <c r="D190" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="E190" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F190" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>48</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C191" t="s">
-        <v>14</v>
-      </c>
-      <c r="D191" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="E191" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>48</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C192" t="s">
-        <v>14</v>
-      </c>
-      <c r="D192" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="E192" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>48</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C193" t="s">
-        <v>14</v>
-      </c>
-      <c r="D193" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="E193" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>48</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C194" t="s">
-        <v>14</v>
-      </c>
-      <c r="D194" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E194" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>48</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C195" t="s">
-        <v>14</v>
-      </c>
-      <c r="D195" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E195" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>48</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C196" t="s">
-        <v>14</v>
-      </c>
-      <c r="D196" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E196" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F196" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>48</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C197" t="s">
-        <v>14</v>
-      </c>
-      <c r="D197" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E197" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F197" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>48</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="C198" t="s">
-        <v>14</v>
-      </c>
-      <c r="D198" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="E198" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F198" s="3" t="s">
-        <v>367</v>
+        <v>299</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Train API Callbacks Tests (#1162)
Train API Callbacks happy path tests. This is just a start. More to come.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865D136E-A3F4-4400-B5EC-3C70942A27F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF3033-446C-4E0E-A573-31293E11BFF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="381">
   <si>
     <t>Page</t>
   </si>
@@ -1211,6 +1211,15 @@
   </si>
   <si>
     <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - select any BOT turn - verify that all turns have no buttons.</t>
+  </si>
+  <si>
+    <t>CreateModels/ApiCallbacks</t>
+  </si>
+  <si>
+    <t>Bug 2132: TEST BLOCKER: Automation cannot trigger 2nd Entity picker in API Action arguments</t>
+  </si>
+  <si>
+    <t>train/ApiCallbacks</t>
   </si>
 </sst>
 </file>
@@ -1781,8 +1790,8 @@
   <dimension ref="A1:F183"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E174" sqref="E174:E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,7 +2195,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -2200,7 +2209,10 @@
         <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>299</v>
+        <v>378</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4830,7 +4842,7 @@
         <v>315</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>299</v>
+        <v>380</v>
       </c>
       <c r="F174" s="3" t="s">
         <v>364</v>
@@ -4850,7 +4862,7 @@
         <v>316</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>299</v>
+        <v>380</v>
       </c>
       <c r="F175" s="3" t="s">
         <v>364</v>

</xml_diff>

<commit_message>
fix: bug in verify in grid fixed
The code train.VerifyTrainingSummaryIsInGrid() had a bug in it that was discovered while writing new test cases. This was fixed.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF3033-446C-4E0E-A573-31293E11BFF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59E6318-E9EB-4AD9-AC2B-A582FC9A5039}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId2"/>
     <sheet name="List of Test Specs" sheetId="2" r:id="rId3"/>
+    <sheet name="Weekly Progress" sheetId="5" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="388">
   <si>
     <t>Page</t>
   </si>
@@ -1024,12 +1028,6 @@
     <t>API Callback, Error Handling</t>
   </si>
   <si>
-    <t>API callback containing no render function that takes no arguments - verify no errors</t>
-  </si>
-  <si>
-    <t>API callback containing no render function that does take arguments - verify no errors</t>
-  </si>
-  <si>
     <t>API callback whose logic function returns a value and contains no render function - verify error is produced</t>
   </si>
   <si>
@@ -1220,6 +1218,33 @@
   </si>
   <si>
     <t>train/ApiCallbacks</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>API callback with Logic function only, no arguments - verify renders using a card with "API Call:" in the card title and function name with open and close parenthesis that are empty inside.</t>
+  </si>
+  <si>
+    <t>API callback with Logic function only, 2 arguments - verify renders using a card with "API Call:" in the card title and function name with open and close parenthesis that contain the 2 argument values.</t>
+  </si>
+  <si>
+    <t>API callback with both Logic and Render functions, 7 arguments each - verify renders as text showing all 14 of the arguments passed to the two separate functions.</t>
+  </si>
+  <si>
+    <t>API callback with Render function only, taking 2 arguments for card title and inner text - verify renders using a card with given card title inner text.</t>
+  </si>
+  <si>
+    <t>Edit Train Dialog containing multiple API callbacks - verify that all turns with callbacks are rendered as expected.</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1342,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1346,13 +1371,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1385,18 +1414,1067 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Test Coverage</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Weekly Progress'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coverage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Weekly Progress'!$A$2:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Weekly Progress'!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0770-4BA9-91B5-03F3195BE4CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Weekly Progress'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Weekly Progress'!$A$2:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Weekly Progress'!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0770-4BA9-91B5-03F3195BE4CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="701744776"/>
+        <c:axId val="701742480"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="701744776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="701742480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="701742480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="701744776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51D8493D-3EAF-46B6-A90E-DA29FB8125F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="C1" t="str">
+            <v>Coverage</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Remaining</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>43602</v>
+          </cell>
+          <cell r="C2">
+            <v>79</v>
+          </cell>
+          <cell r="D2">
+            <v>104</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>43595</v>
+          </cell>
+          <cell r="C3">
+            <v>76</v>
+          </cell>
+          <cell r="D3">
+            <v>96</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F205" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F205" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F207" totalsRowShown="0" headerRowBorderDxfId="5" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F207" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
-    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{B0123158-48C7-47B5-8788-3102666127B5}" name="Page"/>
-    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
+    <tableColumn id="3" xr3:uid="{97683F47-20D1-4334-8379-20CB66181DC2}" name="Coverage"/>
+    <tableColumn id="4" xr3:uid="{0609BF2F-BE77-41CE-A44E-FF4395A9754B}" name="Remaining">
+      <calculatedColumnFormula>B2-C2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1703,49 +2781,49 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="67.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="80.5546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>254</v>
       </c>
@@ -1753,7 +2831,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>278</v>
       </c>
@@ -1764,7 +2842,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -1774,7 +2852,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>279</v>
       </c>
@@ -1787,26 +2865,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F183"/>
+  <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E174" sqref="E174:E175"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A174" sqref="A174:XFD175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="60.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1826,7 +2904,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1843,7 +2921,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1860,7 +2938,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1877,7 +2955,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1894,7 +2972,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1911,7 +2989,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1928,7 +3006,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1945,7 +3023,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1962,7 +3040,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1979,7 +3057,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1990,16 +3068,16 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>215</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2010,16 +3088,16 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2030,16 +3108,16 @@
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2050,16 +3128,16 @@
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2076,7 +3154,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2093,7 +3171,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2110,7 +3188,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2127,7 +3205,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2144,7 +3222,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -2161,7 +3239,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2178,7 +3256,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -2195,7 +3273,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -2209,13 +3287,13 @@
         <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2232,7 +3310,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2249,7 +3327,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -2266,7 +3344,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2283,7 +3361,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2300,7 +3378,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2317,7 +3395,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2334,7 +3412,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2354,7 +3432,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -2371,7 +3449,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -2391,7 +3469,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -2411,7 +3489,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -2428,7 +3506,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2445,7 +3523,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -2462,7 +3540,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2479,7 +3557,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -2496,7 +3574,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -2513,7 +3591,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -2530,7 +3608,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -2547,7 +3625,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -2564,7 +3642,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -2581,7 +3659,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -2598,7 +3676,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -2615,7 +3693,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -2632,7 +3710,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -2649,7 +3727,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -2666,7 +3744,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -2683,7 +3761,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -2700,7 +3778,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -2711,13 +3789,13 @@
         <v>14</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -2728,13 +3806,13 @@
         <v>14</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -2745,13 +3823,13 @@
         <v>14</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -2762,13 +3840,13 @@
         <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -2779,13 +3857,13 @@
         <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -2796,13 +3874,13 @@
         <v>14</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -2813,13 +3891,13 @@
         <v>14</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -2830,13 +3908,13 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -2853,7 +3931,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -2870,7 +3948,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -2887,7 +3965,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -2904,7 +3982,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -2921,7 +3999,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -2938,7 +4016,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -2955,7 +4033,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -2972,7 +4050,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -2983,13 +4061,13 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -3000,13 +4078,13 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -3017,13 +4095,13 @@
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -3034,13 +4112,13 @@
         <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -3057,7 +4135,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -3074,7 +4152,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -3091,7 +4169,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -3108,7 +4186,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -3125,7 +4203,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -3142,7 +4220,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -3159,7 +4237,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -3176,7 +4254,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -3193,7 +4271,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -3210,7 +4288,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -3227,7 +4305,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -3244,7 +4322,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -3264,7 +4342,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -3281,7 +4359,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -3298,7 +4376,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -3315,7 +4393,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -3332,7 +4410,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -3349,7 +4427,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -3366,7 +4444,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -3383,7 +4461,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -3400,7 +4478,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -3417,7 +4495,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -3434,7 +4512,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -3451,7 +4529,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -3468,7 +4546,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -3479,16 +4557,16 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="E97" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>48</v>
       </c>
@@ -3499,16 +4577,16 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -3525,7 +4603,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -3542,7 +4620,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -3559,7 +4637,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -3576,7 +4654,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -3593,7 +4671,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -3610,7 +4688,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -3627,7 +4705,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -3644,7 +4722,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -3661,7 +4739,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -3678,7 +4756,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -3695,7 +4773,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -3712,7 +4790,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -3729,7 +4807,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>48</v>
       </c>
@@ -3740,36 +4818,36 @@
         <v>14</v>
       </c>
       <c r="D112" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>48</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C113" t="s">
+        <v>14</v>
+      </c>
+      <c r="D113" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="E112" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>48</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="C113" t="s">
-        <v>14</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="E113" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -3780,16 +4858,16 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>48</v>
       </c>
@@ -3800,16 +4878,16 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F115" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E115" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -3820,16 +4898,16 @@
         <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -3840,13 +4918,13 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -3863,7 +4941,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -3880,7 +4958,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -3897,7 +4975,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>48</v>
       </c>
@@ -3911,7 +4989,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>48</v>
       </c>
@@ -3928,7 +5006,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>48</v>
       </c>
@@ -3945,7 +5023,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>48</v>
       </c>
@@ -3962,7 +5040,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -3979,7 +5057,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -3996,7 +5074,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -4013,7 +5091,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -4030,7 +5108,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -4047,7 +5125,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>48</v>
       </c>
@@ -4058,13 +5136,13 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>48</v>
       </c>
@@ -4081,7 +5159,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>15</v>
       </c>
@@ -4098,7 +5176,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>15</v>
       </c>
@@ -4115,7 +5193,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>15</v>
       </c>
@@ -4132,7 +5210,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>15</v>
       </c>
@@ -4149,7 +5227,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>15</v>
       </c>
@@ -4166,7 +5244,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -4177,13 +5255,13 @@
         <v>15</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>15</v>
       </c>
@@ -4194,16 +5272,16 @@
         <v>15</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>15</v>
       </c>
@@ -4220,7 +5298,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -4237,7 +5315,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -4254,7 +5332,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>3</v>
       </c>
@@ -4271,7 +5349,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>3</v>
       </c>
@@ -4288,7 +5366,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>3</v>
       </c>
@@ -4305,7 +5383,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>3</v>
       </c>
@@ -4322,7 +5400,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>3</v>
       </c>
@@ -4339,7 +5417,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>3</v>
       </c>
@@ -4356,7 +5434,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>3</v>
       </c>
@@ -4373,7 +5451,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>48</v>
       </c>
@@ -4390,7 +5468,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>287</v>
       </c>
@@ -4407,7 +5485,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>287</v>
       </c>
@@ -4424,7 +5502,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>290</v>
       </c>
@@ -4441,7 +5519,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>48</v>
       </c>
@@ -4458,7 +5536,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>12</v>
       </c>
@@ -4475,7 +5553,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>48</v>
       </c>
@@ -4486,16 +5564,16 @@
         <v>14</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>48</v>
       </c>
@@ -4506,13 +5584,13 @@
         <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>48</v>
       </c>
@@ -4523,13 +5601,13 @@
         <v>14</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>48</v>
       </c>
@@ -4540,13 +5618,13 @@
         <v>14</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>48</v>
       </c>
@@ -4557,13 +5635,13 @@
         <v>14</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>48</v>
       </c>
@@ -4574,13 +5652,13 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>48</v>
       </c>
@@ -4591,13 +5669,13 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>48</v>
       </c>
@@ -4608,13 +5686,13 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>48</v>
       </c>
@@ -4625,13 +5703,13 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>48</v>
       </c>
@@ -4642,13 +5720,13 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>48</v>
       </c>
@@ -4659,16 +5737,16 @@
         <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -4679,16 +5757,16 @@
         <v>14</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>48</v>
       </c>
@@ -4699,16 +5777,16 @@
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>48</v>
       </c>
@@ -4719,16 +5797,16 @@
         <v>14</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -4739,16 +5817,16 @@
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>48</v>
       </c>
@@ -4759,16 +5837,16 @@
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -4779,16 +5857,16 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -4799,16 +5877,16 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -4819,16 +5897,16 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>48</v>
       </c>
@@ -4839,16 +5917,13 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>315</v>
+        <v>342</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F174" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -4859,16 +5934,13 @@
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F175" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -4879,13 +5951,13 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>48</v>
       </c>
@@ -4896,13 +5968,13 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -4913,13 +5985,13 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -4930,13 +6002,16 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F179" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="E179" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>48</v>
       </c>
@@ -4947,13 +6022,16 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>346</v>
+        <v>383</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -4964,16 +6042,16 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>347</v>
+        <v>384</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>299</v>
+        <v>378</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -4984,33 +6062,73 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>346</v>
+        <v>385</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>299</v>
+        <v>378</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>48</v>
       </c>
       <c r="B183" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C183" t="s">
+        <v>14</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>48</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C184" t="s">
+        <v>14</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>48</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C185" t="s">
+        <v>14</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F185" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="C183" t="s">
-        <v>14</v>
-      </c>
-      <c r="D183" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="E183" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F183" s="3" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -5030,15 +6148,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="104.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="104.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>111</v>
       </c>
@@ -5052,7 +6170,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
@@ -5062,7 +6180,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
@@ -5074,7 +6192,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -5086,7 +6204,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -5097,7 +6215,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -5111,7 +6229,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -5125,7 +6243,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -5136,7 +6254,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -5147,10 +6265,10 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -5161,7 +6279,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -5175,7 +6293,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -5186,10 +6304,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -5200,7 +6318,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -5209,10 +6327,10 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -5223,7 +6341,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -5234,7 +6352,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -5245,7 +6363,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -5256,7 +6374,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>137</v>
       </c>
@@ -5267,10 +6385,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -5281,7 +6399,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -5292,10 +6410,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -5309,7 +6427,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -5320,7 +6438,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -5334,7 +6452,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -5348,7 +6466,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -5362,7 +6480,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -5373,7 +6491,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -5387,22 +6505,22 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -5413,7 +6531,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -5424,7 +6542,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>161</v>
       </c>
@@ -5435,7 +6553,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>161</v>
       </c>
@@ -5446,7 +6564,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -5457,7 +6575,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>161</v>
       </c>
@@ -5468,10 +6586,10 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>175</v>
       </c>
@@ -5482,7 +6600,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>175</v>
       </c>
@@ -5491,7 +6609,7 @@
       </c>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>175</v>
       </c>
@@ -5504,4 +6622,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>43602</v>
+      </c>
+      <c r="B2">
+        <v>183</v>
+      </c>
+      <c r="C2">
+        <v>79</v>
+      </c>
+      <c r="D2">
+        <f>B2-C2</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>43595</v>
+      </c>
+      <c r="B3">
+        <v>172</v>
+      </c>
+      <c r="C3">
+        <v>76</v>
+      </c>
+      <c r="D3">
+        <f>B3-C3</f>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: completed test spec and updated test grid
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4588BE-CD32-4A85-BE3B-797C221C533C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C5CC7C-8241-4B3A-B3D2-FE0237068F45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -18,9 +18,6 @@
     <sheet name="List of Test Specs" sheetId="2" r:id="rId3"/>
     <sheet name="Weekly Progress" sheetId="5" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="391">
   <si>
     <t>Page</t>
   </si>
@@ -1040,18 +1037,6 @@
     <t>API callback whose logic function throws an error - verify error is produced.</t>
   </si>
   <si>
-    <t>API callback whose EntityDetectionCallback function throws an error - verify error is produced.</t>
-  </si>
-  <si>
-    <t>API callback whose EntityDetectionCallback function throws an error - bot has not yet responded/user turn only - verify user turn is discarded after error popup is dismissed</t>
-  </si>
-  <si>
-    <t>API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that does have a Bot response - verify Bot response is replaced with error message</t>
-  </si>
-  <si>
-    <t>API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that does have a Bot response - user turn is then fixed to remove the offensive entity - verify Bot response error is dismissed and is returned to correct response</t>
-  </si>
-  <si>
     <t>Create pretrained Entity 1st of its type - verify warning message pops up</t>
   </si>
   <si>
@@ -1245,6 +1230,73 @@
   </si>
   <si>
     <t>Edit Train Dialog containing multiple API callbacks - verify that all turns with callbacks are rendered as expected.</t>
+  </si>
+  <si>
+    <t>ErrorHandling/ApiCallbacks</t>
+  </si>
+  <si>
+    <t>ErrorHandling/ApiCreateMultipleExceptions, ErrorHandling/ApiVerifyMultipleExceptions</t>
+  </si>
+  <si>
+    <t>API callback whose EntityDetectionCallback function throws an error on the 1st user turn of a new TD - verify entire new Train Dialog is discarded after error popup is dismissed</t>
+  </si>
+  <si>
+    <t>API callback whose EntityDetectionCallback function throws an error on a new user turn other than the 1st - verify the turn is discarded after error popup is dismissed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that has an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bot response - verify that Bot response and all subsequent Bot responses are replaced with error message</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that has a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEXT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bot response - verify that Bot response and all subsequent Bot responses are replaced with error message</t>
+    </r>
+  </si>
+  <si>
+    <t>API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that has a Bot response - user turn is then fixed to remove the offensive entity - verify Bot response error is dismissed and is returned to correct response</t>
   </si>
 </sst>
 </file>
@@ -2416,50 +2468,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="C1" t="str">
-            <v>Coverage</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>Remaining</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>43602</v>
-          </cell>
-          <cell r="C2">
-            <v>79</v>
-          </cell>
-          <cell r="D2">
-            <v>104</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>43595</v>
-          </cell>
-          <cell r="C3">
-            <v>76</v>
-          </cell>
-          <cell r="D3">
-            <v>96</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F207" totalsRowShown="0" headerRowBorderDxfId="5" headerRowCellStyle="Heading 1">
   <autoFilter ref="A1:F207" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
@@ -2793,49 +2801,49 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="80.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>254</v>
       </c>
@@ -2843,7 +2851,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>278</v>
       </c>
@@ -2854,7 +2862,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -2864,7 +2872,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>279</v>
       </c>
@@ -2880,23 +2888,23 @@
   <dimension ref="A1:F185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A174" sqref="A174:XFD175"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="60.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2916,7 +2924,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2933,7 +2941,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2950,7 +2958,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2967,7 +2975,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2984,7 +2992,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3001,7 +3009,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3018,7 +3026,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3035,7 +3043,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3052,7 +3060,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3069,7 +3077,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3080,16 +3088,16 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>215</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3100,16 +3108,16 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3120,16 +3128,16 @@
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3140,16 +3148,16 @@
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3166,7 +3174,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3183,7 +3191,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3200,7 +3208,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3217,7 +3225,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3234,7 +3242,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3251,7 +3259,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3268,7 +3276,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3285,7 +3293,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3299,13 +3307,13 @@
         <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3322,7 +3330,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3339,7 +3347,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -3356,7 +3364,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3373,7 +3381,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -3390,7 +3398,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -3407,7 +3415,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3424,7 +3432,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -3444,7 +3452,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -3461,7 +3469,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -3481,7 +3489,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -3501,7 +3509,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -3518,7 +3526,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -3535,7 +3543,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -3552,7 +3560,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -3569,7 +3577,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -3586,7 +3594,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -3603,7 +3611,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -3620,7 +3628,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -3637,7 +3645,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -3654,7 +3662,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -3671,7 +3679,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -3688,7 +3696,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -3705,7 +3713,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -3722,7 +3730,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -3739,7 +3747,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -3756,7 +3764,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -3773,7 +3781,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -3790,7 +3798,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -3801,13 +3809,13 @@
         <v>14</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -3818,13 +3826,13 @@
         <v>14</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -3835,13 +3843,13 @@
         <v>14</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -3852,13 +3860,13 @@
         <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -3869,13 +3877,13 @@
         <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -3886,13 +3894,13 @@
         <v>14</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -3903,13 +3911,13 @@
         <v>14</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -3920,13 +3928,13 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -3943,7 +3951,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -3960,7 +3968,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -3977,7 +3985,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -3994,7 +4002,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -4011,7 +4019,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -4028,7 +4036,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -4045,7 +4053,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -4062,7 +4070,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -4073,13 +4081,13 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -4090,13 +4098,13 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -4107,13 +4115,13 @@
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -4124,13 +4132,13 @@
         <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -4147,7 +4155,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -4164,7 +4172,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -4181,7 +4189,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -4198,7 +4206,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -4215,7 +4223,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -4232,7 +4240,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -4249,7 +4257,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -4266,7 +4274,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -4283,7 +4291,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -4300,7 +4308,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -4317,7 +4325,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -4334,7 +4342,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -4354,7 +4362,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -4371,7 +4379,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -4388,7 +4396,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -4405,7 +4413,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -4422,7 +4430,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -4439,7 +4447,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -4456,7 +4464,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -4473,7 +4481,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -4490,7 +4498,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -4507,7 +4515,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -4524,7 +4532,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -4541,7 +4549,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -4558,7 +4566,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -4569,16 +4577,16 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>48</v>
       </c>
@@ -4589,16 +4597,16 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -4615,7 +4623,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -4632,7 +4640,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -4649,7 +4657,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -4666,7 +4674,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -4683,7 +4691,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -4700,7 +4708,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -4717,7 +4725,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -4734,7 +4742,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -4751,7 +4759,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -4768,7 +4776,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -4785,7 +4793,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -4802,7 +4810,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -4819,7 +4827,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>48</v>
       </c>
@@ -4830,36 +4838,36 @@
         <v>14</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>48</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C113" t="s">
         <v>14</v>
       </c>
       <c r="D113" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F113" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="E113" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -4870,16 +4878,16 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>48</v>
       </c>
@@ -4890,16 +4898,16 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -4910,16 +4918,16 @@
         <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -4930,13 +4938,13 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -4953,7 +4961,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -4970,7 +4978,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -4987,7 +4995,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>48</v>
       </c>
@@ -5001,7 +5009,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>48</v>
       </c>
@@ -5018,7 +5026,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>48</v>
       </c>
@@ -5035,7 +5043,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>48</v>
       </c>
@@ -5052,7 +5060,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -5069,7 +5077,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -5086,7 +5094,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -5103,7 +5111,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -5120,7 +5128,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -5137,7 +5145,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>48</v>
       </c>
@@ -5148,13 +5156,13 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>48</v>
       </c>
@@ -5171,7 +5179,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>15</v>
       </c>
@@ -5188,7 +5196,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>15</v>
       </c>
@@ -5205,7 +5213,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>15</v>
       </c>
@@ -5222,7 +5230,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>15</v>
       </c>
@@ -5239,7 +5247,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>15</v>
       </c>
@@ -5256,7 +5264,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -5267,13 +5275,13 @@
         <v>15</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>15</v>
       </c>
@@ -5284,16 +5292,16 @@
         <v>15</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>15</v>
       </c>
@@ -5310,7 +5318,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -5327,7 +5335,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -5344,7 +5352,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>3</v>
       </c>
@@ -5361,7 +5369,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>3</v>
       </c>
@@ -5378,7 +5386,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>3</v>
       </c>
@@ -5395,7 +5403,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>3</v>
       </c>
@@ -5412,7 +5420,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>3</v>
       </c>
@@ -5429,7 +5437,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>3</v>
       </c>
@@ -5446,7 +5454,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>3</v>
       </c>
@@ -5463,7 +5471,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>48</v>
       </c>
@@ -5480,7 +5488,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>287</v>
       </c>
@@ -5497,7 +5505,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>287</v>
       </c>
@@ -5514,7 +5522,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>290</v>
       </c>
@@ -5531,7 +5539,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>48</v>
       </c>
@@ -5548,7 +5556,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>12</v>
       </c>
@@ -5565,7 +5573,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>48</v>
       </c>
@@ -5576,16 +5584,16 @@
         <v>14</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>48</v>
       </c>
@@ -5596,13 +5604,13 @@
         <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>48</v>
       </c>
@@ -5613,13 +5621,13 @@
         <v>14</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>48</v>
       </c>
@@ -5630,13 +5638,13 @@
         <v>14</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>48</v>
       </c>
@@ -5647,13 +5655,13 @@
         <v>14</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>48</v>
       </c>
@@ -5664,13 +5672,13 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>48</v>
       </c>
@@ -5681,13 +5689,13 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>48</v>
       </c>
@@ -5698,13 +5706,13 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>48</v>
       </c>
@@ -5715,13 +5723,13 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>48</v>
       </c>
@@ -5732,13 +5740,13 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>48</v>
       </c>
@@ -5752,13 +5760,13 @@
         <v>315</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>299</v>
+        <v>384</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -5772,13 +5780,13 @@
         <v>316</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>299</v>
+        <v>384</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>48</v>
       </c>
@@ -5792,13 +5800,13 @@
         <v>318</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>48</v>
       </c>
@@ -5812,13 +5820,13 @@
         <v>317</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -5829,16 +5837,16 @@
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>319</v>
+        <v>386</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>48</v>
       </c>
@@ -5849,16 +5857,16 @@
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>320</v>
+        <v>387</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -5869,16 +5877,16 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>321</v>
+        <v>388</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -5889,16 +5897,16 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>322</v>
+        <v>389</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -5909,16 +5917,16 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>319</v>
+        <v>390</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>48</v>
       </c>
@@ -5929,13 +5937,13 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -5946,13 +5954,13 @@
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -5963,13 +5971,13 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>48</v>
       </c>
@@ -5980,13 +5988,13 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -5997,13 +6005,13 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -6014,16 +6022,16 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>48</v>
       </c>
@@ -6034,16 +6042,16 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -6054,16 +6062,16 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -6074,16 +6082,16 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>48</v>
       </c>
@@ -6094,16 +6102,16 @@
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -6114,33 +6122,33 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>48</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C185" t="s">
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -6160,15 +6168,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="104.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="104.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>111</v>
       </c>
@@ -6182,7 +6190,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
@@ -6192,7 +6200,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
@@ -6204,7 +6212,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -6216,7 +6224,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -6227,7 +6235,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -6241,7 +6249,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -6255,7 +6263,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -6266,7 +6274,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -6277,10 +6285,10 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -6291,7 +6299,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -6305,7 +6313,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -6316,10 +6324,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -6330,7 +6338,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -6339,10 +6347,10 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -6353,7 +6361,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -6364,7 +6372,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -6375,7 +6383,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -6386,7 +6394,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>137</v>
       </c>
@@ -6397,10 +6405,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -6411,7 +6419,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -6422,10 +6430,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -6439,7 +6447,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -6450,7 +6458,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -6464,7 +6472,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -6478,7 +6486,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -6492,7 +6500,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -6503,7 +6511,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -6517,22 +6525,22 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -6543,7 +6551,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -6554,7 +6562,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>161</v>
       </c>
@@ -6565,7 +6573,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>161</v>
       </c>
@@ -6576,7 +6584,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -6587,7 +6595,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>161</v>
       </c>
@@ -6598,10 +6606,10 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>175</v>
       </c>
@@ -6612,7 +6620,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>175</v>
       </c>
@@ -6621,7 +6629,7 @@
       </c>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>175</v>
       </c>
@@ -6644,29 +6652,29 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>43609</v>
       </c>
@@ -6681,7 +6689,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>43602</v>
       </c>
@@ -6696,7 +6704,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>43595</v>
       </c>

</xml_diff>

<commit_message>
Api Multiple Exceptions Test Automation (#1166)
Added two new test suites:
...ErrorHandling/ApiCreateMultipleExceptions
...ErrorHandling/ApiVerifyMultipleExceptions
Fixed bugs found in existing helper functions while debugging the new tests.
Moved some verification code that was in ScorerModal.js into Train.js where it should have been in the first place.
Extended the Train/ApiCallback test case with some edit verifications.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF3033-446C-4E0E-A573-31293E11BFF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4588BE-CD32-4A85-BE3B-797C221C533C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -16,7 +16,11 @@
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId2"/>
     <sheet name="List of Test Specs" sheetId="2" r:id="rId3"/>
+    <sheet name="Weekly Progress" sheetId="5" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="388">
   <si>
     <t>Page</t>
   </si>
@@ -1024,12 +1028,6 @@
     <t>API Callback, Error Handling</t>
   </si>
   <si>
-    <t>API callback containing no render function that takes no arguments - verify no errors</t>
-  </si>
-  <si>
-    <t>API callback containing no render function that does take arguments - verify no errors</t>
-  </si>
-  <si>
     <t>API callback whose logic function returns a value and contains no render function - verify error is produced</t>
   </si>
   <si>
@@ -1220,6 +1218,33 @@
   </si>
   <si>
     <t>train/ApiCallbacks</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>API callback with Logic function only, no arguments - verify renders using a card with "API Call:" in the card title and function name with open and close parenthesis that are empty inside.</t>
+  </si>
+  <si>
+    <t>API callback with Logic function only, 2 arguments - verify renders using a card with "API Call:" in the card title and function name with open and close parenthesis that contain the 2 argument values.</t>
+  </si>
+  <si>
+    <t>API callback with both Logic and Render functions, 7 arguments each - verify renders as text showing all 14 of the arguments passed to the two separate functions.</t>
+  </si>
+  <si>
+    <t>API callback with Render function only, taking 2 arguments for card title and inner text - verify renders using a card with given card title inner text.</t>
+  </si>
+  <si>
+    <t>Edit Train Dialog containing multiple API callbacks - verify that all turns with callbacks are rendered as expected.</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1342,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1346,13 +1371,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1385,18 +1414,1079 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Test Coverage</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Weekly Progress'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coverage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Weekly Progress'!$A$2:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43609</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Weekly Progress'!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0770-4BA9-91B5-03F3195BE4CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Weekly Progress'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Weekly Progress'!$A$2:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43609</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Weekly Progress'!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0770-4BA9-91B5-03F3195BE4CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="701744776"/>
+        <c:axId val="701742480"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="701744776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="701742480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="701742480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="701744776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51D8493D-3EAF-46B6-A90E-DA29FB8125F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="C1" t="str">
+            <v>Coverage</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Remaining</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>43602</v>
+          </cell>
+          <cell r="C2">
+            <v>79</v>
+          </cell>
+          <cell r="D2">
+            <v>104</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>43595</v>
+          </cell>
+          <cell r="C3">
+            <v>76</v>
+          </cell>
+          <cell r="D3">
+            <v>96</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F205" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F205" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F207" totalsRowShown="0" headerRowBorderDxfId="5" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F207" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
-    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{B0123158-48C7-47B5-8788-3102666127B5}" name="Page"/>
-    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
+    <tableColumn id="3" xr3:uid="{97683F47-20D1-4334-8379-20CB66181DC2}" name="Coverage"/>
+    <tableColumn id="4" xr3:uid="{0609BF2F-BE77-41CE-A44E-FF4395A9754B}" name="Remaining">
+      <calculatedColumnFormula>B2-C2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1703,49 +2793,49 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="67.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="80.5546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>254</v>
       </c>
@@ -1753,7 +2843,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>278</v>
       </c>
@@ -1764,7 +2854,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -1774,7 +2864,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>279</v>
       </c>
@@ -1787,26 +2877,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F183"/>
+  <dimension ref="A1:F185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E174" sqref="E174:E175"/>
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A174" sqref="A174:XFD175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="60.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1826,7 +2916,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1843,7 +2933,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1860,7 +2950,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1877,7 +2967,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1894,7 +2984,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1911,7 +3001,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1928,7 +3018,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1945,7 +3035,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1962,7 +3052,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1979,7 +3069,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1990,16 +3080,16 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>215</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2010,16 +3100,16 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2030,16 +3120,16 @@
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2050,16 +3140,16 @@
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2076,7 +3166,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2093,7 +3183,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2110,7 +3200,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2127,7 +3217,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2144,7 +3234,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -2161,7 +3251,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2178,7 +3268,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -2195,7 +3285,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -2209,13 +3299,13 @@
         <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2232,7 +3322,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2249,7 +3339,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -2266,7 +3356,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2283,7 +3373,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2300,7 +3390,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2317,7 +3407,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2334,7 +3424,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2354,7 +3444,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -2371,7 +3461,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -2391,7 +3481,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -2411,7 +3501,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -2428,7 +3518,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2445,7 +3535,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -2462,7 +3552,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2479,7 +3569,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -2496,7 +3586,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -2513,7 +3603,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -2530,7 +3620,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -2547,7 +3637,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -2564,7 +3654,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -2581,7 +3671,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -2598,7 +3688,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -2615,7 +3705,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -2632,7 +3722,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -2649,7 +3739,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -2666,7 +3756,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -2683,7 +3773,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -2700,7 +3790,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -2711,13 +3801,13 @@
         <v>14</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -2728,13 +3818,13 @@
         <v>14</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -2745,13 +3835,13 @@
         <v>14</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -2762,13 +3852,13 @@
         <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -2779,13 +3869,13 @@
         <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -2796,13 +3886,13 @@
         <v>14</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -2813,13 +3903,13 @@
         <v>14</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -2830,13 +3920,13 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -2853,7 +3943,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -2870,7 +3960,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -2887,7 +3977,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -2904,7 +3994,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -2921,7 +4011,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -2938,7 +4028,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -2955,7 +4045,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -2972,7 +4062,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -2983,13 +4073,13 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -3000,13 +4090,13 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -3017,13 +4107,13 @@
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -3034,13 +4124,13 @@
         <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -3057,7 +4147,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -3074,7 +4164,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -3091,7 +4181,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -3108,7 +4198,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -3125,7 +4215,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -3142,7 +4232,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -3159,7 +4249,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -3176,7 +4266,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -3193,7 +4283,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -3210,7 +4300,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -3227,7 +4317,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -3244,7 +4334,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -3264,7 +4354,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -3281,7 +4371,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -3298,7 +4388,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -3315,7 +4405,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -3332,7 +4422,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -3349,7 +4439,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -3366,7 +4456,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -3383,7 +4473,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -3400,7 +4490,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -3417,7 +4507,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -3434,7 +4524,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -3451,7 +4541,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -3468,7 +4558,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -3479,16 +4569,16 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="E97" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>48</v>
       </c>
@@ -3499,16 +4589,16 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -3525,7 +4615,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -3542,7 +4632,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -3559,7 +4649,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -3576,7 +4666,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -3593,7 +4683,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -3610,7 +4700,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -3627,7 +4717,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -3644,7 +4734,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -3661,7 +4751,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -3678,7 +4768,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -3695,7 +4785,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -3712,7 +4802,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -3729,7 +4819,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>48</v>
       </c>
@@ -3740,36 +4830,36 @@
         <v>14</v>
       </c>
       <c r="D112" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>48</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C113" t="s">
+        <v>14</v>
+      </c>
+      <c r="D113" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="E112" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>48</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="C113" t="s">
-        <v>14</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="E113" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -3780,16 +4870,16 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>48</v>
       </c>
@@ -3800,16 +4890,16 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F115" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E115" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -3820,16 +4910,16 @@
         <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -3840,13 +4930,13 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -3863,7 +4953,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -3880,7 +4970,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -3897,7 +4987,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>48</v>
       </c>
@@ -3911,7 +5001,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>48</v>
       </c>
@@ -3928,7 +5018,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>48</v>
       </c>
@@ -3945,7 +5035,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>48</v>
       </c>
@@ -3962,7 +5052,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -3979,7 +5069,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -3996,7 +5086,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -4013,7 +5103,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -4030,7 +5120,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -4047,7 +5137,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>48</v>
       </c>
@@ -4058,13 +5148,13 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>48</v>
       </c>
@@ -4081,7 +5171,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>15</v>
       </c>
@@ -4098,7 +5188,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>15</v>
       </c>
@@ -4115,7 +5205,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>15</v>
       </c>
@@ -4132,7 +5222,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>15</v>
       </c>
@@ -4149,7 +5239,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>15</v>
       </c>
@@ -4166,7 +5256,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -4177,13 +5267,13 @@
         <v>15</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>15</v>
       </c>
@@ -4194,16 +5284,16 @@
         <v>15</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>15</v>
       </c>
@@ -4220,7 +5310,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -4237,7 +5327,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -4254,7 +5344,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>3</v>
       </c>
@@ -4271,7 +5361,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>3</v>
       </c>
@@ -4288,7 +5378,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>3</v>
       </c>
@@ -4305,7 +5395,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>3</v>
       </c>
@@ -4322,7 +5412,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>3</v>
       </c>
@@ -4339,7 +5429,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>3</v>
       </c>
@@ -4356,7 +5446,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>3</v>
       </c>
@@ -4373,7 +5463,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>48</v>
       </c>
@@ -4390,7 +5480,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>287</v>
       </c>
@@ -4407,7 +5497,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>287</v>
       </c>
@@ -4424,7 +5514,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>290</v>
       </c>
@@ -4441,7 +5531,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>48</v>
       </c>
@@ -4458,7 +5548,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>12</v>
       </c>
@@ -4475,7 +5565,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>48</v>
       </c>
@@ -4486,16 +5576,16 @@
         <v>14</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>48</v>
       </c>
@@ -4506,13 +5596,13 @@
         <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>48</v>
       </c>
@@ -4523,13 +5613,13 @@
         <v>14</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>48</v>
       </c>
@@ -4540,13 +5630,13 @@
         <v>14</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>48</v>
       </c>
@@ -4557,13 +5647,13 @@
         <v>14</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>48</v>
       </c>
@@ -4574,13 +5664,13 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>48</v>
       </c>
@@ -4591,13 +5681,13 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>48</v>
       </c>
@@ -4608,13 +5698,13 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>48</v>
       </c>
@@ -4625,13 +5715,13 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>48</v>
       </c>
@@ -4642,13 +5732,13 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>48</v>
       </c>
@@ -4659,16 +5749,16 @@
         <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -4679,16 +5769,16 @@
         <v>14</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>48</v>
       </c>
@@ -4699,16 +5789,16 @@
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>48</v>
       </c>
@@ -4719,16 +5809,16 @@
         <v>14</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -4739,16 +5829,16 @@
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>48</v>
       </c>
@@ -4759,16 +5849,16 @@
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -4779,16 +5869,16 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -4799,16 +5889,16 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -4819,16 +5909,16 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>48</v>
       </c>
@@ -4839,16 +5929,13 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>315</v>
+        <v>342</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F174" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -4859,16 +5946,13 @@
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F175" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -4879,13 +5963,13 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>48</v>
       </c>
@@ -4896,13 +5980,13 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -4913,13 +5997,13 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -4930,13 +6014,16 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F179" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="E179" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>48</v>
       </c>
@@ -4947,13 +6034,16 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>346</v>
+        <v>383</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -4964,16 +6054,16 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>347</v>
+        <v>384</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>299</v>
+        <v>378</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -4984,33 +6074,73 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>346</v>
+        <v>385</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>299</v>
+        <v>378</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>48</v>
       </c>
       <c r="B183" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C183" t="s">
+        <v>14</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>48</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C184" t="s">
+        <v>14</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>48</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C185" t="s">
+        <v>14</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F185" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="C183" t="s">
-        <v>14</v>
-      </c>
-      <c r="D183" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="E183" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F183" s="3" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -5030,15 +6160,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="104.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="104.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>111</v>
       </c>
@@ -5052,7 +6182,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
@@ -5062,7 +6192,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
@@ -5074,7 +6204,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -5086,7 +6216,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -5097,7 +6227,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -5111,7 +6241,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -5125,7 +6255,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -5136,7 +6266,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -5147,10 +6277,10 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -5161,7 +6291,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -5175,7 +6305,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -5186,10 +6316,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -5200,7 +6330,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -5209,10 +6339,10 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -5223,7 +6353,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -5234,7 +6364,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -5245,7 +6375,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -5256,7 +6386,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>137</v>
       </c>
@@ -5267,10 +6397,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -5281,7 +6411,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -5292,10 +6422,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -5309,7 +6439,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -5320,7 +6450,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -5334,7 +6464,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -5348,7 +6478,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -5362,7 +6492,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -5373,7 +6503,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -5387,22 +6517,22 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -5413,7 +6543,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -5424,7 +6554,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>161</v>
       </c>
@@ -5435,7 +6565,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>161</v>
       </c>
@@ -5446,7 +6576,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -5457,7 +6587,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>161</v>
       </c>
@@ -5468,10 +6598,10 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>175</v>
       </c>
@@ -5482,7 +6612,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>175</v>
       </c>
@@ -5491,7 +6621,7 @@
       </c>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>175</v>
       </c>
@@ -5504,4 +6634,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>43609</v>
+      </c>
+      <c r="B2">
+        <v>185</v>
+      </c>
+      <c r="C2">
+        <v>83</v>
+      </c>
+      <c r="D2">
+        <f>B2-C2</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>43602</v>
+      </c>
+      <c r="B3">
+        <v>183</v>
+      </c>
+      <c r="C3">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <f>B3-C3</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>43595</v>
+      </c>
+      <c r="B4">
+        <v>172</v>
+      </c>
+      <c r="C4">
+        <v>76</v>
+      </c>
+      <c r="D4">
+        <f>B4-C4</f>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Api Callback Error Handling (#1171)
- Expanded 3 test suites with additional scenarios.
- Renamed SelectAction function to SelectTextAction
- Expanded error reporting in a few cases to give more data
- Extended the timeout for CreateModel and ImportModel via the TypeModelName function
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4588BE-CD32-4A85-BE3B-797C221C533C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4E9262-5F77-4296-92D4-AB3638B8B0D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -18,9 +18,6 @@
     <sheet name="List of Test Specs" sheetId="2" r:id="rId3"/>
     <sheet name="Weekly Progress" sheetId="5" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="394">
   <si>
     <t>Page</t>
   </si>
@@ -1040,18 +1037,6 @@
     <t>API callback whose logic function throws an error - verify error is produced.</t>
   </si>
   <si>
-    <t>API callback whose EntityDetectionCallback function throws an error - verify error is produced.</t>
-  </si>
-  <si>
-    <t>API callback whose EntityDetectionCallback function throws an error - bot has not yet responded/user turn only - verify user turn is discarded after error popup is dismissed</t>
-  </si>
-  <si>
-    <t>API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that does have a Bot response - verify Bot response is replaced with error message</t>
-  </si>
-  <si>
-    <t>API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that does have a Bot response - user turn is then fixed to remove the offensive entity - verify Bot response error is dismissed and is returned to correct response</t>
-  </si>
-  <si>
     <t>Create pretrained Entity 1st of its type - verify warning message pops up</t>
   </si>
   <si>
@@ -1245,6 +1230,150 @@
   </si>
   <si>
     <t>Edit Train Dialog containing multiple API callbacks - verify that all turns with callbacks are rendered as expected.</t>
+  </si>
+  <si>
+    <t>ErrorHandling/ApiCallbacks</t>
+  </si>
+  <si>
+    <t>ErrorHandling/ApiCreateMultipleExceptions, ErrorHandling/ApiVerifyMultipleExceptions</t>
+  </si>
+  <si>
+    <t>API callback whose EntityDetectionCallback function throws an error on the 1st user turn of a new TD - verify entire new Train Dialog is discarded after error popup is dismissed</t>
+  </si>
+  <si>
+    <t>API callback whose EntityDetectionCallback function throws an error on a new user turn other than the 1st - verify the turn is discarded after error popup is dismissed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that has an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bot response - verify that Bot response and all subsequent Bot responses are replaced with error message</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that has a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEXT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bot response - verify that Bot response and all subsequent Bot responses are replaced with error message</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that has an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bot response - user turn is then fixed to remove the offensive entity - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>verify all Bot response errors are dismissed and is returned to correct response</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">API callback whose EntityDetectionCallback function throws an error - due to editing a user turn that has a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEXT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bot response - user turn is then fixed to remove the offensive entity - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>verify all Bot response errors are dismissed and is returned to correct response</t>
+    </r>
+  </si>
+  <si>
+    <t>ErrorHandling/ApiCreateMultipleExceptions</t>
+  </si>
+  <si>
+    <t>ErrorHandling/ApiVerifyMultipleExceptions</t>
   </si>
 </sst>
 </file>
@@ -1514,17 +1643,20 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$4</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>43616</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -1532,17 +1664,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$C$2:$C$4</c:f>
+              <c:f>'Weekly Progress'!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
@@ -1579,17 +1714,20 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$4</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>43616</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -1597,17 +1735,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$D$2:$D$4</c:f>
+              <c:f>'Weekly Progress'!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>104</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
@@ -2379,13 +2520,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2416,53 +2557,9 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="C1" t="str">
-            <v>Coverage</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>Remaining</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>43602</v>
-          </cell>
-          <cell r="C2">
-            <v>79</v>
-          </cell>
-          <cell r="D2">
-            <v>104</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>43595</v>
-          </cell>
-          <cell r="C3">
-            <v>76</v>
-          </cell>
-          <cell r="D3">
-            <v>96</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F207" totalsRowShown="0" headerRowBorderDxfId="5" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F207" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F208" totalsRowShown="0" headerRowBorderDxfId="5" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F208" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="4"/>
@@ -2476,8 +2573,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
@@ -2793,49 +2890,49 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="80.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>254</v>
       </c>
@@ -2843,7 +2940,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>278</v>
       </c>
@@ -2854,7 +2951,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -2864,7 +2961,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>279</v>
       </c>
@@ -2877,26 +2974,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F185"/>
+  <dimension ref="A1:F186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A174" sqref="A174:XFD175"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="60.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2916,7 +3013,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2933,7 +3030,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2950,7 +3047,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2967,7 +3064,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2984,7 +3081,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3001,7 +3098,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3018,7 +3115,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3035,7 +3132,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3052,7 +3149,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3069,7 +3166,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3080,16 +3177,16 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>215</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3100,16 +3197,16 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3120,16 +3217,16 @@
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3140,16 +3237,16 @@
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3166,7 +3263,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3183,7 +3280,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3200,7 +3297,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3217,7 +3314,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3234,7 +3331,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3251,7 +3348,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3268,7 +3365,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3285,7 +3382,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3299,13 +3396,13 @@
         <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3322,7 +3419,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3339,7 +3436,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -3356,7 +3453,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3373,7 +3470,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -3390,7 +3487,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -3407,7 +3504,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3424,7 +3521,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -3444,7 +3541,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -3461,7 +3558,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -3481,7 +3578,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -3501,7 +3598,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -3518,7 +3615,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -3535,7 +3632,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -3552,7 +3649,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -3569,7 +3666,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -3586,7 +3683,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -3603,7 +3700,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -3620,7 +3717,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -3637,7 +3734,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -3654,7 +3751,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -3671,7 +3768,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -3688,7 +3785,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -3705,7 +3802,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -3722,7 +3819,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -3739,7 +3836,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -3756,7 +3853,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -3773,7 +3870,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -3790,7 +3887,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -3801,13 +3898,13 @@
         <v>14</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -3818,13 +3915,13 @@
         <v>14</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -3835,13 +3932,13 @@
         <v>14</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -3852,13 +3949,13 @@
         <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -3869,13 +3966,13 @@
         <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -3886,13 +3983,13 @@
         <v>14</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -3903,13 +4000,13 @@
         <v>14</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -3920,13 +4017,13 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -3943,7 +4040,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -3960,7 +4057,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -3977,7 +4074,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -3994,7 +4091,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -4011,7 +4108,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -4028,7 +4125,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -4045,7 +4142,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -4062,7 +4159,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -4073,13 +4170,13 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -4090,13 +4187,13 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -4107,13 +4204,13 @@
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -4124,13 +4221,13 @@
         <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -4147,7 +4244,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -4164,7 +4261,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -4181,7 +4278,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -4198,7 +4295,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -4215,7 +4312,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -4232,7 +4329,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -4249,7 +4346,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -4266,7 +4363,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -4283,7 +4380,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -4300,7 +4397,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -4317,7 +4414,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -4334,7 +4431,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -4354,7 +4451,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -4371,7 +4468,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -4388,7 +4485,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -4405,7 +4502,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -4422,7 +4519,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -4439,7 +4536,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -4456,7 +4553,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -4473,7 +4570,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -4490,7 +4587,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -4507,7 +4604,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -4524,7 +4621,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -4541,7 +4638,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -4558,7 +4655,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -4569,16 +4666,16 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>48</v>
       </c>
@@ -4589,16 +4686,16 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -4615,7 +4712,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -4632,7 +4729,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -4649,7 +4746,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -4666,7 +4763,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -4683,7 +4780,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -4700,7 +4797,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -4717,7 +4814,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -4734,7 +4831,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -4751,7 +4848,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -4768,7 +4865,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -4785,7 +4882,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -4802,7 +4899,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -4819,7 +4916,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>48</v>
       </c>
@@ -4830,36 +4927,36 @@
         <v>14</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>48</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C113" t="s">
         <v>14</v>
       </c>
       <c r="D113" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F113" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="E113" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -4870,16 +4967,16 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>48</v>
       </c>
@@ -4890,16 +4987,16 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -4910,16 +5007,16 @@
         <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -4930,13 +5027,13 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -4953,7 +5050,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -4970,7 +5067,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -4987,7 +5084,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>48</v>
       </c>
@@ -5001,7 +5098,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>48</v>
       </c>
@@ -5018,7 +5115,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>48</v>
       </c>
@@ -5035,7 +5132,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>48</v>
       </c>
@@ -5052,7 +5149,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -5069,7 +5166,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -5086,7 +5183,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -5103,7 +5200,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -5120,7 +5217,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -5137,7 +5234,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>48</v>
       </c>
@@ -5148,13 +5245,13 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>48</v>
       </c>
@@ -5171,7 +5268,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>15</v>
       </c>
@@ -5188,7 +5285,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>15</v>
       </c>
@@ -5205,7 +5302,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>15</v>
       </c>
@@ -5222,7 +5319,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>15</v>
       </c>
@@ -5239,7 +5336,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>15</v>
       </c>
@@ -5256,7 +5353,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -5267,13 +5364,13 @@
         <v>15</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>15</v>
       </c>
@@ -5284,16 +5381,16 @@
         <v>15</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>15</v>
       </c>
@@ -5310,7 +5407,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -5327,7 +5424,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -5344,7 +5441,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>3</v>
       </c>
@@ -5361,7 +5458,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>3</v>
       </c>
@@ -5378,7 +5475,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>3</v>
       </c>
@@ -5395,7 +5492,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>3</v>
       </c>
@@ -5412,7 +5509,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>3</v>
       </c>
@@ -5429,7 +5526,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>3</v>
       </c>
@@ -5446,7 +5543,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>3</v>
       </c>
@@ -5463,7 +5560,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>48</v>
       </c>
@@ -5480,7 +5577,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>287</v>
       </c>
@@ -5497,7 +5594,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>287</v>
       </c>
@@ -5514,7 +5611,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>290</v>
       </c>
@@ -5531,7 +5628,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>48</v>
       </c>
@@ -5548,7 +5645,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>12</v>
       </c>
@@ -5565,7 +5662,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>48</v>
       </c>
@@ -5576,16 +5673,16 @@
         <v>14</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>48</v>
       </c>
@@ -5596,13 +5693,13 @@
         <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>48</v>
       </c>
@@ -5613,13 +5710,13 @@
         <v>14</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>48</v>
       </c>
@@ -5630,13 +5727,13 @@
         <v>14</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>48</v>
       </c>
@@ -5647,13 +5744,13 @@
         <v>14</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>48</v>
       </c>
@@ -5664,13 +5761,13 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>48</v>
       </c>
@@ -5681,13 +5778,13 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>48</v>
       </c>
@@ -5698,13 +5795,13 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>48</v>
       </c>
@@ -5715,13 +5812,13 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>48</v>
       </c>
@@ -5732,13 +5829,13 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>48</v>
       </c>
@@ -5752,13 +5849,13 @@
         <v>315</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>299</v>
+        <v>384</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -5772,13 +5869,13 @@
         <v>316</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>299</v>
+        <v>384</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>48</v>
       </c>
@@ -5792,13 +5889,13 @@
         <v>318</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>48</v>
       </c>
@@ -5812,13 +5909,13 @@
         <v>317</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>299</v>
+        <v>385</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -5829,16 +5926,16 @@
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>319</v>
+        <v>386</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>299</v>
+        <v>392</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>48</v>
       </c>
@@ -5849,16 +5946,16 @@
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>320</v>
+        <v>387</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>299</v>
+        <v>392</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -5869,16 +5966,16 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>321</v>
+        <v>388</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>299</v>
+        <v>393</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -5889,16 +5986,16 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>322</v>
+        <v>389</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>299</v>
+        <v>393</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -5909,33 +6006,36 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>319</v>
+        <v>390</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>299</v>
+        <v>393</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>48</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C174" t="s">
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>342</v>
+        <v>391</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>393</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -5946,13 +6046,13 @@
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -5963,13 +6063,13 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>48</v>
       </c>
@@ -5980,13 +6080,13 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -5997,13 +6097,13 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -6014,16 +6114,13 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="F179" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>48</v>
       </c>
@@ -6034,16 +6131,16 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>383</v>
+        <v>341</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>378</v>
+        <v>299</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -6054,16 +6151,16 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -6074,16 +6171,16 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>48</v>
       </c>
@@ -6094,16 +6191,16 @@
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -6114,33 +6211,53 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>48</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>359</v>
+        <v>313</v>
       </c>
       <c r="C185" t="s">
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>299</v>
+        <v>374</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>48</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C186" t="s">
+        <v>14</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -6160,15 +6277,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="104.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="104.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>111</v>
       </c>
@@ -6182,7 +6299,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
@@ -6192,7 +6309,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
@@ -6204,7 +6321,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -6216,7 +6333,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -6227,7 +6344,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -6241,7 +6358,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -6255,7 +6372,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -6266,7 +6383,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -6277,10 +6394,10 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -6291,7 +6408,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -6305,7 +6422,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -6316,10 +6433,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -6330,7 +6447,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -6339,10 +6456,10 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -6353,7 +6470,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -6364,7 +6481,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -6375,7 +6492,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -6386,7 +6503,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>137</v>
       </c>
@@ -6397,10 +6514,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -6411,7 +6528,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -6422,10 +6539,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -6439,7 +6556,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -6450,7 +6567,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -6464,7 +6581,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -6478,7 +6595,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -6492,7 +6609,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -6503,7 +6620,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -6517,22 +6634,22 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -6543,7 +6660,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -6554,7 +6671,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>161</v>
       </c>
@@ -6565,7 +6682,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>161</v>
       </c>
@@ -6576,7 +6693,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -6587,7 +6704,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>161</v>
       </c>
@@ -6598,10 +6715,10 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>175</v>
       </c>
@@ -6612,7 +6729,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>175</v>
       </c>
@@ -6621,7 +6738,7 @@
       </c>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>175</v>
       </c>
@@ -6638,76 +6755,91 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
+        <v>43616</v>
+      </c>
+      <c r="B2">
+        <v>186</v>
+      </c>
+      <c r="C2">
+        <f>SUM(B2,-D2)</f>
+        <v>93</v>
+      </c>
+      <c r="D2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
         <v>43609</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>185</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>83</v>
-      </c>
-      <c r="D2">
-        <f>B2-C2</f>
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
-        <v>43602</v>
-      </c>
-      <c r="B3">
-        <v>183</v>
-      </c>
-      <c r="C3">
-        <v>79</v>
       </c>
       <c r="D3">
         <f>B3-C3</f>
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>43595</v>
+        <v>43602</v>
       </c>
       <c r="B4">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C4">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D4">
         <f>B4-C4</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>43595</v>
+      </c>
+      <c r="B5">
+        <v>172</v>
+      </c>
+      <c r="C5">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <f>B5-C5</f>
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: working code - not done with test suite yet
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4E9262-5F77-4296-92D4-AB3638B8B0D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DB1C6C-C83F-455F-9A7C-29D00FDFF936}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId2"/>
-    <sheet name="List of Test Specs" sheetId="2" r:id="rId3"/>
-    <sheet name="Weekly Progress" sheetId="5" r:id="rId4"/>
+    <sheet name="Manual Validations" sheetId="6" r:id="rId3"/>
+    <sheet name="List of Test Specs" sheetId="2" r:id="rId4"/>
+    <sheet name="Weekly Progress" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="397">
   <si>
     <t>Page</t>
   </si>
@@ -1178,13 +1179,7 @@
     <t>Import model that was created for APIs that do not exist in the test API set - verify that the Train Dialogs pane shows a incident triangles for each TD that uses those APIs.</t>
   </si>
   <si>
-    <t xml:space="preserve">Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that the </t>
-  </si>
-  <si>
     <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that there is a generic warning message at bottom of window.</t>
-  </si>
-  <si>
-    <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that the API actions show error cards.</t>
   </si>
   <si>
     <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - select any BOT turn - verify that ALL of the Actions in the Scorer pane are diabled.</t>
@@ -1374,6 +1369,21 @@
   </si>
   <si>
     <t>ErrorHandling/ApiVerifyMultipleExceptions</t>
+  </si>
+  <si>
+    <t>ErrorHandling/BotModelMismatch</t>
+  </si>
+  <si>
+    <t>It does not do this, is it a bug?</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that the API actions show an error message</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - navigate to Log Dialogs pane - verify that New Log Dialog button is disabled</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - verify there are errors caused by using wrong Bot - restart the correct Bot - on Home Pane click "Retry" button - Verify the errors go away and the other UI features tested in the failing test validations are all activated and working again.</t>
   </si>
 </sst>
 </file>
@@ -1507,7 +1517,17 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -2558,25 +2578,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F208" totalsRowShown="0" headerRowBorderDxfId="5" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F208" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
   <autoFilter ref="A1:F208" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
-    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{B0123158-48C7-47B5-8788-3102666127B5}" name="Page"/>
-    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7660BDF-5A1B-49D9-81EE-59363A3E189C}" name="Table5" displayName="Table5" ref="A1:F8" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F8" xr:uid="{ABDE53FE-36A6-48A7-8159-AB5687FE6CE2}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{12C7EC41-7AEA-4B95-B723-8858111BAC3A}" name="Area"/>
+    <tableColumn id="2" xr3:uid="{73EA4828-CC64-4BF0-8855-4C4F6CCDB437}" name="Feature"/>
+    <tableColumn id="3" xr3:uid="{E7BCEF5E-D912-4BD3-937C-49CCFAC2FEF9}" name="Page"/>
+    <tableColumn id="4" xr3:uid="{0D3ED91E-5A11-465B-AB16-341017559B3A}" name="Test Validations"/>
+    <tableColumn id="5" xr3:uid="{9C68EA51-9734-488A-8389-4D971FE644FD}" name="Test Name"/>
+    <tableColumn id="6" xr3:uid="{32289615-F402-4BFE-9FCF-7E577EBEF08E}" name="Additional Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D5" totalsRowShown="0">
   <autoFilter ref="A1:D5" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
     <tableColumn id="3" xr3:uid="{97683F47-20D1-4334-8379-20CB66181DC2}" name="Coverage"/>
     <tableColumn id="4" xr3:uid="{0609BF2F-BE77-41CE-A44E-FF4395A9754B}" name="Remaining">
@@ -2977,17 +3012,17 @@
   <dimension ref="A1:F186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="82.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="70.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3396,10 +3431,10 @@
         <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -5676,7 +5711,7 @@
         <v>362</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>299</v>
+        <v>392</v>
       </c>
       <c r="F155" s="3" t="s">
         <v>361</v>
@@ -5696,7 +5731,7 @@
         <v>363</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>299</v>
+        <v>392</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5712,9 +5747,6 @@
       <c r="D157" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="E157" s="3" t="s">
-        <v>299</v>
-      </c>
     </row>
     <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
@@ -5730,7 +5762,7 @@
         <v>365</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>299</v>
+        <v>393</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5747,7 +5779,7 @@
         <v>366</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>299</v>
+        <v>392</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5761,13 +5793,13 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>367</v>
+        <v>394</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>48</v>
       </c>
@@ -5778,13 +5810,10 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>48</v>
       </c>
@@ -5795,10 +5824,7 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>299</v>
+        <v>368</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5812,10 +5838,7 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>299</v>
+        <v>369</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5829,10 +5852,7 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>299</v>
+        <v>395</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5849,7 +5869,7 @@
         <v>315</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F165" s="3" t="s">
         <v>358</v>
@@ -5869,7 +5889,7 @@
         <v>316</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F166" s="3" t="s">
         <v>358</v>
@@ -5889,7 +5909,7 @@
         <v>318</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F167" s="3" t="s">
         <v>358</v>
@@ -5909,7 +5929,7 @@
         <v>317</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F168" s="3" t="s">
         <v>358</v>
@@ -5926,10 +5946,10 @@
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F169" s="3" t="s">
         <v>358</v>
@@ -5946,10 +5966,10 @@
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F170" s="3" t="s">
         <v>358</v>
@@ -5966,10 +5986,10 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F171" s="3" t="s">
         <v>358</v>
@@ -5986,10 +6006,10 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F172" s="3" t="s">
         <v>358</v>
@@ -6006,10 +6026,10 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F173" s="3" t="s">
         <v>358</v>
@@ -6026,10 +6046,10 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E174" s="3" t="s">
         <v>391</v>
-      </c>
-      <c r="E174" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="F174" s="3" t="s">
         <v>358</v>
@@ -6151,10 +6171,10 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F181" s="3" t="s">
         <v>358</v>
@@ -6171,10 +6191,10 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F182" s="3" t="s">
         <v>358</v>
@@ -6191,10 +6211,10 @@
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F183" s="3" t="s">
         <v>358</v>
@@ -6211,10 +6231,10 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F184" s="3" t="s">
         <v>358</v>
@@ -6231,10 +6251,10 @@
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F185" s="3" t="s">
         <v>358</v>
@@ -6270,6 +6290,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85EFE73-8B28-4777-8911-7132E1D597B5}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="82.7109375" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B719F-1470-4AFA-970E-2998AD817A19}">
   <dimension ref="A1:D47"/>
   <sheetViews>
@@ -6753,7 +6836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -6771,16 +6854,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1" t="s">
         <v>375</v>
-      </c>
-      <c r="C1" t="s">
-        <v>376</v>
-      </c>
-      <c r="D1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: working code with more test scenarios to be added
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DB1C6C-C83F-455F-9A7C-29D00FDFF936}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CBE527-5E92-4C35-B5E8-DCF2A1A0DC0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="398">
   <si>
     <t>Page</t>
   </si>
@@ -1174,9 +1174,6 @@
   </si>
   <si>
     <t>Import model that was created for APIs that do not exist in the test API set - verify that opening an API Action shows error message under the API name.</t>
-  </si>
-  <si>
-    <t>Import model that was created for APIs that do not exist in the test API set - verify that the Train Dialogs pane shows a incident triangles for each TD that uses those APIs.</t>
   </si>
   <si>
     <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that there is a generic warning message at bottom of window.</t>
@@ -1374,16 +1371,22 @@
     <t>ErrorHandling/BotModelMismatch</t>
   </si>
   <si>
-    <t>It does not do this, is it a bug?</t>
-  </si>
-  <si>
     <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that the API actions show an error message</t>
   </si>
   <si>
-    <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - navigate to Log Dialogs pane - verify that New Log Dialog button is disabled</t>
-  </si>
-  <si>
     <t>Import model that was created for APIs that do not exist in the test API set - verify there are errors caused by using wrong Bot - restart the correct Bot - on Home Pane click "Retry" button - Verify the errors go away and the other UI features tested in the failing test validations are all activated and working again.</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - navigate to Log Dialogs pane - verify that New Log Dialog button is disabled</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - navigate to Train Dialogs pane - verify that New Train Dialog button is disabled</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - select any BOT turn - verify that the add action button is missing.</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - delete the action with the API that does not exist - verify that the model is now good and without errors - verify that new Train Dialogs can be created - verify that editing a TD has the usual controls enabled</t>
   </si>
 </sst>
 </file>
@@ -2578,8 +2581,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F208" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F208" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F210" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F210" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
@@ -3009,11 +3012,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F186"/>
+  <dimension ref="A1:F188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3431,10 +3434,10 @@
         <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>370</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -5711,7 +5714,7 @@
         <v>362</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F155" s="3" t="s">
         <v>361</v>
@@ -5731,7 +5734,7 @@
         <v>363</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5747,6 +5750,9 @@
       <c r="D157" s="3" t="s">
         <v>364</v>
       </c>
+      <c r="E157" s="3" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
@@ -5759,10 +5765,10 @@
         <v>14</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>365</v>
+        <v>395</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5776,10 +5782,10 @@
         <v>14</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5793,13 +5799,13 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>48</v>
       </c>
@@ -5810,7 +5816,10 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5824,7 +5833,10 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>368</v>
+        <v>396</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5838,7 +5850,10 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5852,7 +5867,7 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>395</v>
+        <v>367</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5866,16 +5881,10 @@
         <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -5886,13 +5895,7 @@
         <v>14</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="F166" s="3" t="s">
-        <v>358</v>
+        <v>397</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5906,10 +5909,10 @@
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F167" s="3" t="s">
         <v>358</v>
@@ -5926,10 +5929,10 @@
         <v>14</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F168" s="3" t="s">
         <v>358</v>
@@ -5946,10 +5949,10 @@
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>384</v>
+        <v>318</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="F169" s="3" t="s">
         <v>358</v>
@@ -5966,16 +5969,16 @@
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>385</v>
+        <v>317</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="F170" s="3" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -5986,16 +5989,16 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F171" s="3" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -6006,10 +6009,10 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F172" s="3" t="s">
         <v>358</v>
@@ -6026,10 +6029,10 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F173" s="3" t="s">
         <v>358</v>
@@ -6046,47 +6049,53 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F174" s="3" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>48</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C175" t="s">
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>338</v>
+        <v>387</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>48</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C176" t="s">
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>337</v>
+        <v>388</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>299</v>
+        <v>390</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6100,13 +6109,13 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -6117,13 +6126,13 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -6134,7 +6143,7 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>299</v>
@@ -6151,16 +6160,13 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="F180" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -6171,16 +6177,13 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>377</v>
+        <v>340</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="F181" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -6191,16 +6194,16 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>378</v>
+        <v>341</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>372</v>
+        <v>299</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>48</v>
       </c>
@@ -6211,16 +6214,16 @@
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F183" s="3" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -6231,10 +6234,10 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F184" s="3" t="s">
         <v>358</v>
@@ -6251,10 +6254,10 @@
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F185" s="3" t="s">
         <v>358</v>
@@ -6265,18 +6268,58 @@
         <v>48</v>
       </c>
       <c r="B186" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C186" t="s">
+        <v>14</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>48</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C187" t="s">
+        <v>14</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>48</v>
+      </c>
+      <c r="B188" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C186" t="s">
-        <v>14</v>
-      </c>
-      <c r="D186" s="3" t="s">
+      <c r="C188" t="s">
+        <v>14</v>
+      </c>
+      <c r="D188" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="E186" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F186" s="3" t="s">
+      <c r="E188" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F188" s="3" t="s">
         <v>357</v>
       </c>
     </row>
@@ -6338,7 +6381,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6854,16 +6897,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1" t="s">
         <v>373</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>374</v>
-      </c>
-      <c r="D1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: updated test grid
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CBE527-5E92-4C35-B5E8-DCF2A1A0DC0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6313310B-E12D-47B7-983E-9A92838639EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="398">
   <si>
     <t>Page</t>
   </si>
@@ -1666,20 +1666,23 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$5</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>43623</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -1687,20 +1690,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$C$2:$C$5</c:f>
+              <c:f>'Weekly Progress'!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
@@ -1737,20 +1743,23 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$5</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>43623</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -1758,20 +1767,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$D$2:$D$5</c:f>
+              <c:f>'Weekly Progress'!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>104</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
@@ -2543,13 +2555,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2611,8 +2623,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D5" totalsRowShown="0">
-  <autoFilter ref="A1:D5" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
@@ -3015,8 +3027,8 @@
   <dimension ref="A1:F188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E165" sqref="E165"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E164" sqref="E164:E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4523,7 +4535,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -4920,7 +4932,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -5869,6 +5881,9 @@
       <c r="D164" s="3" t="s">
         <v>367</v>
       </c>
+      <c r="E164" s="3" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
@@ -5883,6 +5898,9 @@
       <c r="D165" s="3" t="s">
         <v>394</v>
       </c>
+      <c r="E165" s="3" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="166" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
@@ -5896,6 +5914,9 @@
       </c>
       <c r="D166" s="3" t="s">
         <v>397</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6881,10 +6902,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6911,61 +6932,76 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
-        <v>43616</v>
+        <v>43623</v>
       </c>
       <c r="B2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C2">
         <f>SUM(B2,-D2)</f>
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D2">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>43609</v>
+        <v>43616</v>
       </c>
       <c r="B3">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C3">
-        <v>83</v>
+        <f>SUM(B3,-D3)</f>
+        <v>93</v>
       </c>
       <c r="D3">
-        <f>B3-C3</f>
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>43602</v>
+        <v>43609</v>
       </c>
       <c r="B4">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C4">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D4">
         <f>B4-C4</f>
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
-        <v>43595</v>
+        <v>43602</v>
       </c>
       <c r="B5">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C5">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D5">
         <f>B5-C5</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>43595</v>
+      </c>
+      <c r="B6">
+        <v>172</v>
+      </c>
+      <c r="C6">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <f>B6-C6</f>
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: updated test grid xlsx
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFE25C9-DE73-4748-9527-1B2BAEC2F2F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F028382-E287-4151-A2F8-4F8198EB7886}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -3027,8 +3027,8 @@
   <dimension ref="A1:F188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E164" sqref="E164:E165"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E165" sqref="E165:E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5916,7 +5916,7 @@
         <v>397</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Extending BotModelMismatch - Rename to BotMissingApi (#1178)
- Renamed the BotModelMismatch test suite to BotMissingApi
- Extended the suite by adding new test scenarios to it
- Renamed some functions which names started with "validate" to be consistent and start with "verify"
- Clarified the names of a few other functions
- Updated TestGrid to show new test coverage
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4E9262-5F77-4296-92D4-AB3638B8B0D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F028382-E287-4151-A2F8-4F8198EB7886}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
     <sheet name="Areas Features Validations" sheetId="1" r:id="rId2"/>
-    <sheet name="List of Test Specs" sheetId="2" r:id="rId3"/>
-    <sheet name="Weekly Progress" sheetId="5" r:id="rId4"/>
+    <sheet name="Manual Validations" sheetId="6" r:id="rId3"/>
+    <sheet name="List of Test Specs" sheetId="2" r:id="rId4"/>
+    <sheet name="Weekly Progress" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="398">
   <si>
     <t>Page</t>
   </si>
@@ -1175,16 +1176,7 @@
     <t>Import model that was created for APIs that do not exist in the test API set - verify that opening an API Action shows error message under the API name.</t>
   </si>
   <si>
-    <t>Import model that was created for APIs that do not exist in the test API set - verify that the Train Dialogs pane shows a incident triangles for each TD that uses those APIs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that the </t>
-  </si>
-  <si>
     <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that there is a generic warning message at bottom of window.</t>
-  </si>
-  <si>
-    <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that the API actions show error cards.</t>
   </si>
   <si>
     <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - select any BOT turn - verify that ALL of the Actions in the Scorer pane are diabled.</t>
@@ -1374,6 +1366,27 @@
   </si>
   <si>
     <t>ErrorHandling/ApiVerifyMultipleExceptions</t>
+  </si>
+  <si>
+    <t>ErrorHandling/BotModelMismatch</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - verify that the API actions show an error message</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - verify there are errors caused by using wrong Bot - restart the correct Bot - on Home Pane click "Retry" button - Verify the errors go away and the other UI features tested in the failing test validations are all activated and working again.</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - navigate to Log Dialogs pane - verify that New Log Dialog button is disabled</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - navigate to Train Dialogs pane - verify that New Train Dialog button is disabled</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - open a Train Dialog - select any BOT turn - verify that the add action button is missing.</t>
+  </si>
+  <si>
+    <t>Import model that was created for APIs that do not exist in the test API set - delete the action with the API that does not exist - verify that the model is now good and without errors - verify that new Train Dialogs can be created - verify that editing a TD has the usual controls enabled</t>
   </si>
 </sst>
 </file>
@@ -1507,9 +1520,19 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1643,20 +1666,23 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$5</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>43623</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -1664,20 +1690,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$C$2:$C$5</c:f>
+              <c:f>'Weekly Progress'!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
@@ -1714,20 +1743,23 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$5</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>43623</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -1735,20 +1767,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$D$2:$D$5</c:f>
+              <c:f>'Weekly Progress'!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>104</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
@@ -2520,13 +2555,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2558,23 +2593,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F208" totalsRowShown="0" headerRowBorderDxfId="5" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F208" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F210" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F210" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
-    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{B0123158-48C7-47B5-8788-3102666127B5}" name="Page"/>
-    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D5" totalsRowShown="0">
-  <autoFilter ref="A1:D5" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7660BDF-5A1B-49D9-81EE-59363A3E189C}" name="Table5" displayName="Table5" ref="A1:F8" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F8" xr:uid="{ABDE53FE-36A6-48A7-8159-AB5687FE6CE2}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{12C7EC41-7AEA-4B95-B723-8858111BAC3A}" name="Area"/>
+    <tableColumn id="2" xr3:uid="{73EA4828-CC64-4BF0-8855-4C4F6CCDB437}" name="Feature"/>
+    <tableColumn id="3" xr3:uid="{E7BCEF5E-D912-4BD3-937C-49CCFAC2FEF9}" name="Page"/>
+    <tableColumn id="4" xr3:uid="{0D3ED91E-5A11-465B-AB16-341017559B3A}" name="Test Validations"/>
+    <tableColumn id="5" xr3:uid="{9C68EA51-9734-488A-8389-4D971FE644FD}" name="Test Name"/>
+    <tableColumn id="6" xr3:uid="{32289615-F402-4BFE-9FCF-7E577EBEF08E}" name="Additional Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
@@ -2974,20 +3024,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F186"/>
+  <dimension ref="A1:F188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E165" sqref="E165:E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="82.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="70.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3396,10 +3446,10 @@
         <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4485,7 +4535,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -4882,7 +4932,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -5676,7 +5726,7 @@
         <v>362</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
       <c r="F155" s="3" t="s">
         <v>361</v>
@@ -5696,7 +5746,7 @@
         <v>363</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5713,7 +5763,7 @@
         <v>364</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5727,10 +5777,10 @@
         <v>14</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>365</v>
+        <v>395</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5744,10 +5794,10 @@
         <v>14</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5761,10 +5811,10 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>367</v>
+        <v>392</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5778,13 +5828,13 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>48</v>
       </c>
@@ -5795,10 +5845,10 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>369</v>
+        <v>396</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5812,10 +5862,10 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5829,10 +5879,10 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5846,16 +5896,13 @@
         <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>315</v>
+        <v>394</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -5866,13 +5913,10 @@
         <v>14</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>316</v>
+        <v>397</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="F166" s="3" t="s">
-        <v>358</v>
+        <v>391</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5886,10 +5930,10 @@
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F167" s="3" t="s">
         <v>358</v>
@@ -5906,10 +5950,10 @@
         <v>14</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F168" s="3" t="s">
         <v>358</v>
@@ -5926,10 +5970,10 @@
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>386</v>
+        <v>318</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="F169" s="3" t="s">
         <v>358</v>
@@ -5946,16 +5990,16 @@
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>387</v>
+        <v>317</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="F170" s="3" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -5966,16 +6010,16 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F171" s="3" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -5986,10 +6030,10 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="E172" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="F172" s="3" t="s">
         <v>358</v>
@@ -6006,10 +6050,10 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E173" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="E173" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="F173" s="3" t="s">
         <v>358</v>
@@ -6026,47 +6070,53 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F174" s="3" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>48</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C175" t="s">
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>338</v>
+        <v>387</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>48</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C176" t="s">
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>337</v>
+        <v>388</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>299</v>
+        <v>390</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6080,13 +6130,13 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -6097,13 +6147,13 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -6114,7 +6164,7 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>299</v>
@@ -6131,16 +6181,13 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="F180" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -6151,16 +6198,13 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>379</v>
+        <v>340</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="F181" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -6171,16 +6215,16 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>380</v>
+        <v>341</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>374</v>
+        <v>299</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>48</v>
       </c>
@@ -6191,16 +6235,16 @@
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F183" s="3" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -6211,10 +6255,10 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F184" s="3" t="s">
         <v>358</v>
@@ -6231,10 +6275,10 @@
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F185" s="3" t="s">
         <v>358</v>
@@ -6245,18 +6289,58 @@
         <v>48</v>
       </c>
       <c r="B186" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C186" t="s">
+        <v>14</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>48</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C187" t="s">
+        <v>14</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>48</v>
+      </c>
+      <c r="B188" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C186" t="s">
-        <v>14</v>
-      </c>
-      <c r="D186" s="3" t="s">
+      <c r="C188" t="s">
+        <v>14</v>
+      </c>
+      <c r="D188" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="E186" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F186" s="3" t="s">
+      <c r="E188" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F188" s="3" t="s">
         <v>357</v>
       </c>
     </row>
@@ -6270,6 +6354,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85EFE73-8B28-4777-8911-7132E1D597B5}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="82.7109375" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B719F-1470-4AFA-970E-2998AD817A19}">
   <dimension ref="A1:D47"/>
   <sheetViews>
@@ -6753,12 +6900,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6771,75 +6918,90 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
-        <v>43616</v>
+        <v>43623</v>
       </c>
       <c r="B2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C2">
         <f>SUM(B2,-D2)</f>
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D2">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>43609</v>
+        <v>43616</v>
       </c>
       <c r="B3">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C3">
-        <v>83</v>
+        <f>SUM(B3,-D3)</f>
+        <v>93</v>
       </c>
       <c r="D3">
-        <f>B3-C3</f>
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>43602</v>
+        <v>43609</v>
       </c>
       <c r="B4">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C4">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D4">
         <f>B4-C4</f>
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
-        <v>43595</v>
+        <v>43602</v>
       </c>
       <c r="B5">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C5">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D5">
         <f>B5-C5</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>43595</v>
+      </c>
+      <c r="B6">
+        <v>172</v>
+      </c>
+      <c r="C6">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <f>B6-C6</f>
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Api Memory Manipulation Test Suite (#1184)
Added a new test suite that uses APIs that manipulates Entity memory contents to verify the coupling of these various pieces all work together end-to-end. The basic pieces came from our Pizza Demo and the test scenario follows a simplified version of those demos.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F028382-E287-4151-A2F8-4F8198EB7886}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236D7686-6C0E-42A0-8E9A-2056DF249167}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="398">
   <si>
     <t>Page</t>
   </si>
@@ -1092,22 +1092,7 @@
     <t>Difference here is that it is detecting the conflict within 1 TD, no other TDs should exist.</t>
   </si>
   <si>
-    <t>API callback adds a value to an entity - verify it shows up in Entity Memory</t>
-  </si>
-  <si>
     <t>API callback returns a card with a message and a photo - verify it shows up in chat response</t>
-  </si>
-  <si>
-    <t>API callback adds a value to an entity - save - edit TD - verify it shows up in Entity Memory</t>
-  </si>
-  <si>
-    <t>API callback expects two Entities with numeric resolver types - renders the math it did on them - verify results</t>
-  </si>
-  <si>
-    <t>API callback expects two Entities with numeric resolver types - omit 1 number renders the math it did on them - verify results</t>
-  </si>
-  <si>
-    <t>see video "Edit with numbers.mp4" for more info</t>
   </si>
   <si>
     <t>Verify Wait and Type columns have correct values</t>
@@ -1387,6 +1372,21 @@
   </si>
   <si>
     <t>Import model that was created for APIs that do not exist in the test API set - delete the action with the API that does not exist - verify that the model is now good and without errors - verify that new Train Dialogs can be created - verify that editing a TD has the usual controls enabled</t>
+  </si>
+  <si>
+    <t>API callback sets a value in an entity - verify it shows up in Entity Memory</t>
+  </si>
+  <si>
+    <t>API callback deletes a value from an entity - verify it shows up in Entity Memory</t>
+  </si>
+  <si>
+    <t>API callback deletes an entity - verify it shows up in Entity Memory as having been deleted</t>
+  </si>
+  <si>
+    <t>API callback copies one entity into another - verify it shows up in Entity Memory</t>
+  </si>
+  <si>
+    <t>Train/ApiMemoryManipulation</t>
   </si>
 </sst>
 </file>
@@ -2593,8 +2593,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F210" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F210" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F209" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F209" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
@@ -3024,11 +3024,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F188"/>
+  <dimension ref="A1:F187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E165" sqref="E165:E166"/>
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E177" sqref="E177:E181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3446,10 +3446,10 @@
         <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3948,7 +3948,7 @@
         <v>14</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>299</v>
@@ -3965,7 +3965,7 @@
         <v>14</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>299</v>
@@ -3982,7 +3982,7 @@
         <v>14</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>299</v>
@@ -3999,7 +3999,7 @@
         <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>299</v>
@@ -4016,7 +4016,7 @@
         <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>299</v>
@@ -4033,7 +4033,7 @@
         <v>14</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>299</v>
@@ -4050,7 +4050,7 @@
         <v>14</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>262</v>
@@ -4067,7 +4067,7 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>299</v>
@@ -4220,7 +4220,7 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>299</v>
@@ -4237,7 +4237,7 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>299</v>
@@ -4254,7 +4254,7 @@
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>299</v>
@@ -4271,7 +4271,7 @@
         <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>299</v>
@@ -5077,7 +5077,7 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>299</v>
@@ -5295,7 +5295,7 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>299</v>
@@ -5723,13 +5723,13 @@
         <v>14</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5743,10 +5743,10 @@
         <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5760,10 +5760,10 @@
         <v>14</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5777,10 +5777,10 @@
         <v>14</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5794,10 +5794,10 @@
         <v>14</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5811,10 +5811,10 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5828,10 +5828,10 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5845,10 +5845,10 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5862,10 +5862,10 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5879,10 +5879,10 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5896,10 +5896,10 @@
         <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5913,10 +5913,10 @@
         <v>14</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5933,10 +5933,10 @@
         <v>315</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5953,10 +5953,10 @@
         <v>316</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5973,10 +5973,10 @@
         <v>318</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5993,10 +5993,10 @@
         <v>317</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6010,13 +6010,13 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6030,13 +6030,13 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E172" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="E172" s="3" t="s">
-        <v>389</v>
-      </c>
       <c r="F172" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6050,13 +6050,13 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E173" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="E173" s="3" t="s">
-        <v>390</v>
-      </c>
       <c r="F173" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6070,13 +6070,13 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6090,13 +6090,13 @@
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6110,13 +6110,13 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6130,10 +6130,10 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>299</v>
+        <v>397</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6147,10 +6147,10 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>337</v>
+        <v>393</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>299</v>
+        <v>397</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6164,13 +6164,13 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>339</v>
+        <v>394</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>48</v>
       </c>
@@ -6181,13 +6181,13 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>340</v>
+        <v>395</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -6198,13 +6198,13 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>340</v>
+        <v>396</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -6215,13 +6215,13 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>341</v>
+        <v>371</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>299</v>
+        <v>366</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6235,16 +6235,16 @@
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -6255,13 +6255,13 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6275,13 +6275,13 @@
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6295,13 +6295,13 @@
         <v>14</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6309,39 +6309,19 @@
         <v>48</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>313</v>
+        <v>350</v>
       </c>
       <c r="C187" t="s">
         <v>14</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>371</v>
+        <v>299</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>48</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="C188" t="s">
-        <v>14</v>
-      </c>
-      <c r="D188" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="E188" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F188" s="3" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -6402,7 +6382,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6918,16 +6898,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B1" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D1" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Api Photo Card (#1186)
- Added a scenario to Train/ApiCallbacks for photo cards.
- Fixed all "throws" in the test code so they use "new Error()" instead of just throwing a string.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236D7686-6C0E-42A0-8E9A-2056DF249167}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85D164A-A2AC-439F-A034-2AB965CA79B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1522,19 +1524,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1552,6 +1541,19 @@
           <color theme="4"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2593,22 +2595,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F209" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F209" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
   <autoFilter ref="A1:F209" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
-    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{B0123158-48C7-47B5-8788-3102666127B5}" name="Page"/>
-    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7660BDF-5A1B-49D9-81EE-59363A3E189C}" name="Table5" displayName="Table5" ref="A1:F8" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7660BDF-5A1B-49D9-81EE-59363A3E189C}" name="Table5" displayName="Table5" ref="A1:F8" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" headerRowCellStyle="Heading 1">
   <autoFilter ref="A1:F8" xr:uid="{ABDE53FE-36A6-48A7-8159-AB5687FE6CE2}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{12C7EC41-7AEA-4B95-B723-8858111BAC3A}" name="Area"/>
@@ -2626,7 +2628,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D6" totalsRowShown="0">
   <autoFilter ref="A1:D6" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
     <tableColumn id="3" xr3:uid="{97683F47-20D1-4334-8379-20CB66181DC2}" name="Coverage"/>
     <tableColumn id="4" xr3:uid="{0609BF2F-BE77-41CE-A44E-FF4395A9754B}" name="Remaining">
@@ -3027,8 +3029,8 @@
   <dimension ref="A1:F187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E177" sqref="E177:E181"/>
+      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A177" sqref="A177:XFD177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6130,7 +6132,7 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>337</v>
+        <v>393</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>397</v>
@@ -6147,7 +6149,7 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>397</v>
@@ -6164,7 +6166,7 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>397</v>
@@ -6181,7 +6183,7 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>397</v>
@@ -6198,10 +6200,10 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>396</v>
+        <v>337</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>397</v>
+        <v>366</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create Entity Tests (#1188)
- Split the CreateModels/AllEntityTypes into two tests
- Got rid of the FlipFlop code - expanded to cover all combinations
- Expanded the suite to cover creating Pretrained Entities followed by Custom with same Resolver type as well as doing it in the reverse order to ensure that the informational popup only comes up once per Resolver type.
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85D164A-A2AC-439F-A034-2AB965CA79B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215772F5-2A63-478C-B052-A00C2F8274AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -1524,6 +1524,19 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1541,19 +1554,6 @@
           <color theme="4"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1668,23 +1668,26 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$6</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>43630</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43623</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -1692,23 +1695,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$C$2:$C$6</c:f>
+              <c:f>'Weekly Progress'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
@@ -1745,23 +1751,26 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$6</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>43630</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43623</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -1769,23 +1778,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$D$2:$D$6</c:f>
+              <c:f>'Weekly Progress'!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>104</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
@@ -2557,13 +2569,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2595,22 +2607,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F209" totalsRowShown="0" headerRowBorderDxfId="4" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F209" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F209" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F209" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="todo"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
-    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{B0123158-48C7-47B5-8788-3102666127B5}" name="Page"/>
-    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{9E19D589-D83D-4717-9F5D-BD2AD9F935E9}" name="Test Validations" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{BC84EEBB-5D19-4499-B7FE-E62F4B6382CE}" name="Test Name" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{100F57C4-33FA-4044-AB33-66A70FCA33C1}" name="Additional Notes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7660BDF-5A1B-49D9-81EE-59363A3E189C}" name="Table5" displayName="Table5" ref="A1:F8" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E7660BDF-5A1B-49D9-81EE-59363A3E189C}" name="Table5" displayName="Table5" ref="A1:F8" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" headerRowCellStyle="Heading 1">
   <autoFilter ref="A1:F8" xr:uid="{ABDE53FE-36A6-48A7-8159-AB5687FE6CE2}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{12C7EC41-7AEA-4B95-B723-8858111BAC3A}" name="Area"/>
@@ -2625,10 +2643,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D6" totalsRowShown="0">
-  <autoFilter ref="A1:D6" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
     <tableColumn id="3" xr3:uid="{97683F47-20D1-4334-8379-20CB66181DC2}" name="Coverage"/>
     <tableColumn id="4" xr3:uid="{0609BF2F-BE77-41CE-A44E-FF4395A9754B}" name="Remaining">
@@ -3026,10 +3044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F187"/>
+  <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A177" sqref="A177:XFD177"/>
     </sheetView>
   </sheetViews>
@@ -3082,7 +3100,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3099,7 +3117,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3116,7 +3134,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3133,7 +3151,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3150,7 +3168,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3167,7 +3185,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3184,7 +3202,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3201,7 +3219,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3218,7 +3236,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3400,7 +3418,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3417,7 +3435,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3434,7 +3452,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3471,7 +3489,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3539,7 +3557,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -3556,7 +3574,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3630,7 +3648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -3735,7 +3753,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -3752,7 +3770,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -3769,7 +3787,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -3786,7 +3804,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -3803,7 +3821,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -3820,7 +3838,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -3837,7 +3855,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -3854,7 +3872,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -3871,7 +3889,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -3888,7 +3906,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -3905,7 +3923,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -3922,7 +3940,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -4041,7 +4059,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -4075,7 +4093,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -4092,7 +4110,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -4109,7 +4127,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -4126,7 +4144,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -4143,7 +4161,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -4160,7 +4178,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -4177,7 +4195,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -4296,7 +4314,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -4313,7 +4331,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -4330,7 +4348,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -4347,7 +4365,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -4364,7 +4382,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -4381,7 +4399,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -4398,7 +4416,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -4415,7 +4433,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -4432,7 +4450,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -4449,7 +4467,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -4466,7 +4484,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -4520,7 +4538,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -4537,7 +4555,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -4554,7 +4572,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -4571,7 +4589,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -4588,7 +4606,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -4605,7 +4623,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -4622,7 +4640,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -4747,7 +4765,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -4764,7 +4782,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -4781,7 +4799,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -4798,7 +4816,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -4815,7 +4833,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -4832,7 +4850,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -4849,7 +4867,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -4866,7 +4884,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -4883,7 +4901,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -4900,7 +4918,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -4917,7 +4935,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -4934,7 +4952,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -4951,7 +4969,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -5085,7 +5103,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -5119,7 +5137,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -5136,7 +5154,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>48</v>
       </c>
@@ -5150,7 +5168,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>48</v>
       </c>
@@ -5235,7 +5253,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -5252,7 +5270,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -5269,7 +5287,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -5320,7 +5338,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>15</v>
       </c>
@@ -5459,7 +5477,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -5493,7 +5511,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>3</v>
       </c>
@@ -5714,7 +5732,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>48</v>
       </c>
@@ -5734,7 +5752,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>48</v>
       </c>
@@ -5751,7 +5769,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>48</v>
       </c>
@@ -5768,7 +5786,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>48</v>
       </c>
@@ -5785,7 +5803,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>48</v>
       </c>
@@ -5802,7 +5820,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>48</v>
       </c>
@@ -5819,7 +5837,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>48</v>
       </c>
@@ -5836,7 +5854,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>48</v>
       </c>
@@ -5853,7 +5871,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>48</v>
       </c>
@@ -5870,7 +5888,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>48</v>
       </c>
@@ -5887,7 +5905,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>48</v>
       </c>
@@ -5904,7 +5922,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -5921,7 +5939,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>48</v>
       </c>
@@ -5941,7 +5959,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>48</v>
       </c>
@@ -5961,7 +5979,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -5981,7 +5999,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>48</v>
       </c>
@@ -6001,7 +6019,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -6021,7 +6039,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -6041,7 +6059,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -6061,7 +6079,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>48</v>
       </c>
@@ -6081,7 +6099,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -6101,7 +6119,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -6121,7 +6139,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>48</v>
       </c>
@@ -6138,7 +6156,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -6155,7 +6173,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -6172,7 +6190,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>48</v>
       </c>
@@ -6189,7 +6207,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -6206,7 +6224,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -6226,7 +6244,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>48</v>
       </c>
@@ -6246,7 +6264,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -6266,7 +6284,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>48</v>
       </c>
@@ -6286,7 +6304,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>48</v>
       </c>
@@ -6326,6 +6344,28 @@
         <v>352</v>
       </c>
     </row>
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6884,10 +6924,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6914,76 +6954,91 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
-        <v>43623</v>
+        <v>43630</v>
       </c>
       <c r="B2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2">
         <f>SUM(B2,-D2)</f>
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D2">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>43616</v>
+        <v>43623</v>
       </c>
       <c r="B3">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C3">
         <f>SUM(B3,-D3)</f>
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D3">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>43609</v>
+        <v>43616</v>
       </c>
       <c r="B4">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C4">
-        <v>83</v>
+        <f>SUM(B4,-D4)</f>
+        <v>93</v>
       </c>
       <c r="D4">
-        <f>B4-C4</f>
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
-        <v>43602</v>
+        <v>43609</v>
       </c>
       <c r="B5">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C5">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D5">
         <f>B5-C5</f>
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>43595</v>
+        <v>43602</v>
       </c>
       <c r="B6">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C6">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D6">
         <f>B6-C6</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>43595</v>
+      </c>
+      <c r="B7">
+        <v>172</v>
+      </c>
+      <c r="C7">
+        <v>76</v>
+      </c>
+      <c r="D7">
+        <f>B7-C7</f>
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: new bug in test code due to ui changes
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E2CAE6-27D5-498A-977C-86020C599179}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FF7886-4816-48C5-B3C1-9B1C197AECD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="410">
   <si>
     <t>Page</t>
   </si>
@@ -1419,6 +1419,12 @@
   </si>
   <si>
     <t>Verify that "Train Dialog" filter button navigates to Train Dialog pane and shows only the Train Dialogs in the list that use the selected Action.</t>
+  </si>
+  <si>
+    <t>Tools/EntityActionMissingUserTurn</t>
+  </si>
+  <si>
+    <t>Start with a model with 2 Train Dialogs that could be merged - Edit Train Dialog with a single turn involving 1 Entity label and a Bot Response that renders that Entity - Add a simple text User turn - Score a simple Text Action - Delete the User turn that was just added - Save TD as is. (Bug 2191)</t>
   </si>
 </sst>
 </file>
@@ -2655,8 +2661,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F215" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F215" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F216" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F216" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
@@ -3086,11 +3092,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F193"/>
+  <dimension ref="A1:F194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4376,7 +4382,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -4387,10 +4393,10 @@
         <v>14</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>342</v>
+        <v>409</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>295</v>
+        <v>408</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -4404,30 +4410,30 @@
         <v>14</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>48</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>290</v>
+        <v>58</v>
       </c>
       <c r="C76" t="s">
         <v>14</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -4438,47 +4444,47 @@
         <v>14</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>48</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>203</v>
+        <v>290</v>
       </c>
       <c r="C78" t="s">
         <v>14</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>205</v>
+        <v>345</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>48</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>40</v>
+        <v>203</v>
       </c>
       <c r="C79" t="s">
         <v>14</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>41</v>
+        <v>205</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -4489,7 +4495,7 @@
         <v>14</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>239</v>
@@ -4506,10 +4512,10 @@
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4523,13 +4529,13 @@
         <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -4540,13 +4546,13 @@
         <v>14</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -4557,13 +4563,13 @@
         <v>14</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -4574,7 +4580,7 @@
         <v>14</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>242</v>
@@ -4591,7 +4597,7 @@
         <v>14</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>242</v>
@@ -4608,10 +4614,10 @@
         <v>14</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -4625,13 +4631,13 @@
         <v>14</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -4642,7 +4648,7 @@
         <v>14</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>239</v>
@@ -4659,16 +4665,13 @@
         <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -4679,30 +4682,33 @@
         <v>14</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F91" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C92" t="s">
         <v>14</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -4713,13 +4719,13 @@
         <v>14</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>253</v>
+        <v>66</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -4730,13 +4736,13 @@
         <v>14</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -4747,10 +4753,10 @@
         <v>14</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>308</v>
+        <v>254</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>300</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4764,7 +4770,7 @@
         <v>14</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>300</v>
@@ -4781,7 +4787,7 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>300</v>
@@ -4798,7 +4804,7 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>300</v>
@@ -4815,10 +4821,10 @@
         <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4832,7 +4838,7 @@
         <v>14</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>295</v>
@@ -4849,7 +4855,7 @@
         <v>14</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>295</v>
@@ -4866,7 +4872,7 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>295</v>
@@ -4883,16 +4889,13 @@
         <v>14</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="F103" s="3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -4903,7 +4906,7 @@
         <v>14</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>295</v>
@@ -4912,21 +4915,24 @@
         <v>332</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C105" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>71</v>
+        <v>331</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>273</v>
+        <v>295</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4940,7 +4946,7 @@
         <v>12</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>273</v>
@@ -4957,7 +4963,7 @@
         <v>12</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>273</v>
@@ -4971,10 +4977,10 @@
         <v>70</v>
       </c>
       <c r="C108" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>273</v>
@@ -4991,13 +4997,13 @@
         <v>14</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -5007,11 +5013,11 @@
       <c r="C110" t="s">
         <v>14</v>
       </c>
-      <c r="D110" s="4" t="s">
-        <v>76</v>
+      <c r="D110" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5025,10 +5031,10 @@
         <v>14</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5042,7 +5048,7 @@
         <v>14</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>258</v>
@@ -5059,10 +5065,10 @@
         <v>14</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5076,10 +5082,10 @@
         <v>14</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5093,13 +5099,13 @@
         <v>14</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -5109,14 +5115,14 @@
       <c r="C116" t="s">
         <v>14</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>82</v>
+      <c r="D116" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -5127,13 +5133,13 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -5144,27 +5150,24 @@
         <v>14</v>
       </c>
       <c r="D118" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>48</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C119" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F118" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>48</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C119" t="s">
-        <v>14</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>321</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>295</v>
@@ -5178,13 +5181,13 @@
         <v>48</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>70</v>
+        <v>320</v>
       </c>
       <c r="C120" t="s">
         <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>295</v>
@@ -5204,7 +5207,7 @@
         <v>14</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>295</v>
@@ -5224,7 +5227,7 @@
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>295</v>
@@ -5244,30 +5247,33 @@
         <v>14</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F123" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>48</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C124" t="s">
         <v>14</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>86</v>
+        <v>350</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -5278,13 +5284,13 @@
         <v>14</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>261</v>
+        <v>86</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -5295,10 +5301,10 @@
         <v>14</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>85</v>
+        <v>261</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>241</v>
+        <v>295</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -5311,11 +5317,14 @@
       <c r="C127" t="s">
         <v>14</v>
       </c>
+      <c r="D127" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E127" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -5325,14 +5334,11 @@
       <c r="C128" t="s">
         <v>14</v>
       </c>
-      <c r="D128" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="E128" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -5343,13 +5349,13 @@
         <v>14</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>48</v>
       </c>
@@ -5360,13 +5366,13 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>48</v>
       </c>
@@ -5377,13 +5383,13 @@
         <v>14</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>48</v>
       </c>
@@ -5394,13 +5400,13 @@
         <v>14</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>48</v>
       </c>
@@ -5411,13 +5417,13 @@
         <v>14</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>48</v>
       </c>
@@ -5428,13 +5434,13 @@
         <v>14</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>279</v>
+        <v>88</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>48</v>
       </c>
@@ -5445,13 +5451,13 @@
         <v>14</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>99</v>
+        <v>279</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>48</v>
       </c>
@@ -5462,13 +5468,13 @@
         <v>14</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>351</v>
+        <v>99</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>48</v>
       </c>
@@ -5479,30 +5485,30 @@
         <v>14</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>98</v>
+        <v>351</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="C138" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>15</v>
       </c>
@@ -5513,13 +5519,13 @@
         <v>15</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>15</v>
       </c>
@@ -5530,13 +5536,13 @@
         <v>15</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>265</v>
+        <v>91</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>15</v>
       </c>
@@ -5547,13 +5553,13 @@
         <v>15</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>15</v>
       </c>
@@ -5564,13 +5570,13 @@
         <v>15</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>15</v>
       </c>
@@ -5581,13 +5587,13 @@
         <v>15</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>327</v>
+        <v>264</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>15</v>
       </c>
@@ -5598,118 +5604,118 @@
         <v>15</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="F144" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>15</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C145" t="s">
         <v>15</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>278</v>
+        <v>328</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F145" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>266</v>
+        <v>84</v>
       </c>
       <c r="C146" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>24</v>
+        <v>278</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>3</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C147" t="s">
         <v>8</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>268</v>
+        <v>24</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>3</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>67</v>
+        <v>268</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>3</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C149" t="s">
         <v>8</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>3</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>4</v>
+        <v>267</v>
       </c>
       <c r="C150" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>3</v>
       </c>
@@ -5717,7 +5723,7 @@
         <v>4</v>
       </c>
       <c r="C151" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>25</v>
@@ -5726,24 +5732,24 @@
         <v>295</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>3</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>3</v>
       </c>
@@ -5751,7 +5757,7 @@
         <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>26</v>
@@ -5760,58 +5766,58 @@
         <v>295</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>3</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>298</v>
+        <v>11</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>299</v>
+        <v>26</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>280</v>
+        <v>69</v>
       </c>
       <c r="C155" t="s">
-        <v>14</v>
+        <v>298</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>283</v>
+        <v>48</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C156" t="s">
-        <v>282</v>
+        <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>283</v>
       </c>
@@ -5822,58 +5828,58 @@
         <v>282</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C158" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>48</v>
+        <v>286</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C159" t="s">
-        <v>14</v>
+        <v>288</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C160" t="s">
-        <v>293</v>
+        <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>295</v>
@@ -5881,22 +5887,19 @@
     </row>
     <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="C161" t="s">
-        <v>14</v>
+        <v>293</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>353</v>
+        <v>294</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="F161" s="3" t="s">
-        <v>352</v>
+        <v>295</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5910,11 +5913,14 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>382</v>
       </c>
+      <c r="F162" s="3" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
@@ -5927,7 +5933,7 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>382</v>
@@ -5944,7 +5950,7 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>386</v>
+        <v>355</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>382</v>
@@ -5961,7 +5967,7 @@
         <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>356</v>
+        <v>386</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>382</v>
@@ -5978,7 +5984,7 @@
         <v>14</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>383</v>
+        <v>356</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>382</v>
@@ -5995,7 +6001,7 @@
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>357</v>
+        <v>383</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>382</v>
@@ -6012,7 +6018,7 @@
         <v>14</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>387</v>
+        <v>357</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>382</v>
@@ -6029,7 +6035,7 @@
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>359</v>
+        <v>387</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>382</v>
@@ -6046,7 +6052,7 @@
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>382</v>
@@ -6063,13 +6069,13 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>385</v>
+        <v>358</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -6080,13 +6086,13 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -6097,13 +6103,10 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>311</v>
+        <v>388</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="F173" s="3" t="s">
-        <v>349</v>
+        <v>382</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6117,7 +6120,7 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>372</v>
@@ -6137,10 +6140,10 @@
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F175" s="3" t="s">
         <v>349</v>
@@ -6157,7 +6160,7 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>373</v>
@@ -6177,10 +6180,10 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>374</v>
+        <v>313</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="F177" s="3" t="s">
         <v>349</v>
@@ -6197,7 +6200,7 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>380</v>
@@ -6206,7 +6209,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -6217,10 +6220,10 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F179" s="3" t="s">
         <v>349</v>
@@ -6237,7 +6240,7 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>381</v>
@@ -6257,7 +6260,7 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>381</v>
@@ -6277,7 +6280,7 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>381</v>
@@ -6286,21 +6289,24 @@
         <v>349</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>48</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C183" t="s">
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>393</v>
+        <v>381</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6314,7 +6320,7 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>393</v>
@@ -6331,7 +6337,7 @@
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>393</v>
@@ -6348,7 +6354,7 @@
         <v>14</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>393</v>
@@ -6365,13 +6371,13 @@
         <v>14</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>333</v>
+        <v>392</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>48</v>
       </c>
@@ -6382,14 +6388,11 @@
         <v>14</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>367</v>
+        <v>333</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="F188" s="3" t="s">
-        <v>349</v>
-      </c>
     </row>
     <row r="189" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
@@ -6402,7 +6405,7 @@
         <v>14</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>362</v>
@@ -6411,7 +6414,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>48</v>
       </c>
@@ -6422,7 +6425,7 @@
         <v>14</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>362</v>
@@ -6442,7 +6445,7 @@
         <v>14</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>362</v>
@@ -6462,7 +6465,7 @@
         <v>14</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>362</v>
@@ -6476,18 +6479,38 @@
         <v>48</v>
       </c>
       <c r="B193" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C193" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>48</v>
+      </c>
+      <c r="B194" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="C193" t="s">
-        <v>14</v>
-      </c>
-      <c r="D193" s="3" t="s">
+      <c r="C194" t="s">
+        <v>14</v>
+      </c>
+      <c r="D194" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="E193" s="3" t="s">
+      <c r="E194" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="F193" s="3" t="s">
+      <c r="F194" s="3" t="s">
         <v>348</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Entity Action Missing User Turn (#1207)
Adding a test case to produce Bug 2191: CRASH: Modifying Train Dialog to contain an error causes UI to throw an error
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D519725A-2F05-4AAB-ACE6-BF62FFB23ABE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14B01DC-968E-42E4-9ECB-678C276D7BB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="411">
   <si>
     <t>Page</t>
   </si>
@@ -1413,6 +1413,21 @@
   </si>
   <si>
     <t>Edit an existing Entity that is not used by any Actions and verify that both "Required For Actions" and the "Blocked Actions" tabs reveal no Actions in the grid.</t>
+  </si>
+  <si>
+    <t>Verify that you get a warning before deleting an Action that is used in a Train Dialog even if all the TDs using that action have errors (Bug 2188)</t>
+  </si>
+  <si>
+    <t>Verify that "Train Dialog" filter button navigates to Train Dialog pane and shows only the Train Dialogs in the list that use the selected Action.</t>
+  </si>
+  <si>
+    <t>Tools/EntityActionMissingUserTurn</t>
+  </si>
+  <si>
+    <t>Start with a model with 2 Train Dialogs that could be merged - Edit Train Dialog with a single turn involving 1 Entity label and a Bot Response that renders that Entity - Add a simple text User turn - Score a simple Text Action - Delete the User turn that was just added - Save TD as is. (Bug 2191)</t>
+  </si>
+  <si>
+    <t>Edit Turn, Error Handling</t>
   </si>
 </sst>
 </file>
@@ -2649,14 +2664,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F213" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F213" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="todo"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F216" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F216" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
@@ -3086,11 +3095,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F213"/>
+  <dimension ref="A1:F194"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3125,7 +3134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3142,7 +3151,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3159,7 +3168,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3176,7 +3185,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3193,7 +3202,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3210,7 +3219,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3227,7 +3236,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3244,7 +3253,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3261,7 +3270,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3278,7 +3287,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3298,7 +3307,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3318,7 +3327,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3338,7 +3347,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3358,7 +3367,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3378,7 +3387,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3395,7 +3404,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3412,7 +3421,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3429,7 +3438,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3446,7 +3455,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3463,7 +3472,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3480,7 +3489,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3497,7 +3506,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3514,7 +3523,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3531,7 +3540,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="75.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3548,7 +3557,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="75.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -3565,7 +3574,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3585,7 +3594,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -3602,7 +3611,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -3664,64 +3673,61 @@
         <v>28</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>202</v>
+        <v>406</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>218</v>
+        <v>407</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3729,56 +3735,53 @@
         <v>12</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>16</v>
+        <v>221</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>23</v>
+        <v>223</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>295</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>18</v>
+        <v>222</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>21</v>
+        <v>217</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>226</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3786,33 +3789,39 @@
         <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>180</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>182</v>
+        <v>21</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>295</v>
+        <v>255</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3820,13 +3829,13 @@
         <v>12</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>181</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>183</v>
+        <v>97</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>295</v>
@@ -3837,87 +3846,87 @@
         <v>12</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>38</v>
+        <v>184</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>89</v>
+        <v>186</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>39</v>
+        <v>185</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>232</v>
+        <v>89</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -3928,47 +3937,47 @@
         <v>30</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
         <v>30</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>102</v>
+        <v>232</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>31</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
         <v>30</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>103</v>
+        <v>230</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -3979,64 +3988,64 @@
         <v>30</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>233</v>
+        <v>102</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="C51" t="s">
         <v>30</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>31</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>31</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C53" t="s">
         <v>30</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -4047,61 +4056,61 @@
         <v>30</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>31</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
         <v>30</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>335</v>
+        <v>100</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>295</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>336</v>
+        <v>90</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>295</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -4115,7 +4124,7 @@
         <v>14</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>295</v>
@@ -4132,7 +4141,7 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>295</v>
@@ -4149,7 +4158,7 @@
         <v>14</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>295</v>
@@ -4166,13 +4175,13 @@
         <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -4183,10 +4192,10 @@
         <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>258</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -4200,47 +4209,47 @@
         <v>14</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>48</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>53</v>
+        <v>340</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C65" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>59</v>
+        <v>341</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -4251,13 +4260,13 @@
         <v>14</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -4268,13 +4277,13 @@
         <v>14</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -4285,13 +4294,13 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -4302,13 +4311,13 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -4319,13 +4328,13 @@
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>240</v>
+        <v>54</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -4336,10 +4345,10 @@
         <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>204</v>
+        <v>65</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>295</v>
+        <v>227</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4353,13 +4362,13 @@
         <v>14</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>342</v>
+        <v>240</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -4370,115 +4379,115 @@
         <v>14</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>343</v>
+        <v>204</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>48</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>290</v>
+        <v>410</v>
       </c>
       <c r="C74" t="s">
         <v>14</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>344</v>
+        <v>409</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>48</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>290</v>
+        <v>58</v>
       </c>
       <c r="C75" t="s">
         <v>14</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>48</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>203</v>
+        <v>58</v>
       </c>
       <c r="C76" t="s">
         <v>14</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>205</v>
+        <v>343</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>48</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
       <c r="C77" t="s">
         <v>14</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>41</v>
+        <v>344</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>48</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
       <c r="C78" t="s">
         <v>14</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>55</v>
+        <v>345</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>48</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>40</v>
+        <v>203</v>
       </c>
       <c r="C79" t="s">
         <v>14</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>45</v>
+        <v>205</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -4489,13 +4498,13 @@
         <v>14</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -4506,13 +4515,13 @@
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -4523,13 +4532,13 @@
         <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -4540,13 +4549,13 @@
         <v>14</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -4557,13 +4566,13 @@
         <v>14</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -4574,13 +4583,13 @@
         <v>14</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -4591,13 +4600,13 @@
         <v>14</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -4608,13 +4617,13 @@
         <v>14</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -4625,13 +4634,10 @@
         <v>14</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>52</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -4645,64 +4651,67 @@
         <v>14</v>
       </c>
       <c r="D89" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>48</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C90" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>48</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C91" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>48</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C92" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E92" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>48</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C90" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>48</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C91" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>48</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C92" t="s">
-        <v>14</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -4713,13 +4722,13 @@
         <v>14</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>308</v>
+        <v>66</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -4730,13 +4739,13 @@
         <v>14</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -4747,13 +4756,13 @@
         <v>14</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>307</v>
+        <v>254</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -4764,7 +4773,7 @@
         <v>14</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>300</v>
@@ -4781,10 +4790,10 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4798,10 +4807,10 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4815,10 +4824,10 @@
         <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4832,7 +4841,7 @@
         <v>14</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>295</v>
@@ -4849,16 +4858,13 @@
         <v>14</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="F101" s="3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -4869,67 +4875,70 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="F102" s="3" t="s">
+    </row>
+    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>48</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>48</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C104" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F104" s="3" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>48</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C103" t="s">
-        <v>12</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>48</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C104" t="s">
-        <v>12</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C105" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>73</v>
+        <v>331</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -4937,16 +4946,16 @@
         <v>70</v>
       </c>
       <c r="C106" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -4954,16 +4963,16 @@
         <v>70</v>
       </c>
       <c r="C107" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -4971,16 +4980,16 @@
         <v>70</v>
       </c>
       <c r="C108" t="s">
-        <v>14</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>76</v>
+        <v>12</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -4990,14 +4999,14 @@
       <c r="C109" t="s">
         <v>14</v>
       </c>
-      <c r="D109" s="4" t="s">
-        <v>77</v>
+      <c r="D109" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -5007,14 +5016,14 @@
       <c r="C110" t="s">
         <v>14</v>
       </c>
-      <c r="D110" s="4" t="s">
-        <v>78</v>
+      <c r="D110" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -5025,13 +5034,13 @@
         <v>14</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>48</v>
       </c>
@@ -5042,13 +5051,13 @@
         <v>14</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>48</v>
       </c>
@@ -5059,13 +5068,13 @@
         <v>14</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -5075,14 +5084,14 @@
       <c r="C114" t="s">
         <v>14</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>82</v>
+      <c r="D114" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>48</v>
       </c>
@@ -5092,14 +5101,14 @@
       <c r="C115" t="s">
         <v>14</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>83</v>
+      <c r="D115" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -5109,34 +5118,28 @@
       <c r="C116" t="s">
         <v>14</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>319</v>
+      <c r="D116" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F116" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>48</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>320</v>
+        <v>70</v>
       </c>
       <c r="C117" t="s">
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>321</v>
+        <v>82</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F117" s="3" t="s">
-        <v>325</v>
+        <v>260</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5150,16 +5153,13 @@
         <v>14</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>322</v>
+        <v>83</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F118" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>295</v>
@@ -5184,13 +5184,13 @@
         <v>48</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>70</v>
+        <v>320</v>
       </c>
       <c r="C120" t="s">
         <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>295</v>
@@ -5210,27 +5210,33 @@
         <v>14</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>350</v>
+        <v>322</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F121" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>48</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C122" t="s">
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>86</v>
+        <v>323</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>241</v>
+        <v>295</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5238,36 +5244,39 @@
         <v>48</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C123" t="s">
         <v>14</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>261</v>
+        <v>324</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F123" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>48</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C124" t="s">
         <v>14</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>85</v>
+        <v>350</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -5277,11 +5286,14 @@
       <c r="C125" t="s">
         <v>14</v>
       </c>
+      <c r="D125" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="E125" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -5292,13 +5304,13 @@
         <v>14</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>87</v>
+        <v>261</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -5309,13 +5321,13 @@
         <v>14</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -5325,14 +5337,11 @@
       <c r="C128" t="s">
         <v>14</v>
       </c>
-      <c r="D128" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="E128" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -5343,13 +5352,13 @@
         <v>14</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>48</v>
       </c>
@@ -5360,13 +5369,13 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>48</v>
       </c>
@@ -5377,13 +5386,13 @@
         <v>14</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>48</v>
       </c>
@@ -5394,13 +5403,13 @@
         <v>14</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>279</v>
+        <v>95</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>48</v>
       </c>
@@ -5411,13 +5420,13 @@
         <v>14</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>48</v>
       </c>
@@ -5428,13 +5437,13 @@
         <v>14</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>351</v>
+        <v>88</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>48</v>
       </c>
@@ -5445,64 +5454,64 @@
         <v>14</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>98</v>
+        <v>279</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="C136" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="C137" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>91</v>
+        <v>351</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="C138" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>265</v>
+        <v>98</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>15</v>
       </c>
@@ -5513,13 +5522,13 @@
         <v>15</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>263</v>
+        <v>92</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>15</v>
       </c>
@@ -5530,13 +5539,13 @@
         <v>15</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>264</v>
+        <v>91</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>15</v>
       </c>
@@ -5547,13 +5556,13 @@
         <v>15</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>327</v>
+        <v>265</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>15</v>
       </c>
@@ -5564,132 +5573,132 @@
         <v>15</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>328</v>
+        <v>263</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="F142" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>15</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C143" t="s">
         <v>15</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>266</v>
+        <v>15</v>
       </c>
       <c r="C144" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>24</v>
+        <v>327</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>270</v>
+        <v>15</v>
       </c>
       <c r="C145" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>268</v>
+        <v>328</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F145" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>271</v>
+        <v>84</v>
       </c>
       <c r="C146" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>67</v>
+        <v>278</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>3</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C147" t="s">
         <v>8</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>3</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>4</v>
+        <v>270</v>
       </c>
       <c r="C148" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>25</v>
+        <v>268</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>3</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>4</v>
+        <v>271</v>
       </c>
       <c r="C149" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>295</v>
+        <v>238</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -5697,13 +5706,13 @@
         <v>3</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>5</v>
+        <v>267</v>
       </c>
       <c r="C150" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>295</v>
@@ -5714,64 +5723,64 @@
         <v>3</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C151" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>3</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>298</v>
+        <v>11</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>299</v>
+        <v>25</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>280</v>
+        <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>281</v>
+        <v>26</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>283</v>
+        <v>3</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>282</v>
+        <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>282</v>
+        <v>11</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>284</v>
+        <v>26</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>295</v>
@@ -5779,33 +5788,33 @@
     </row>
     <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>283</v>
+        <v>3</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>282</v>
+        <v>69</v>
       </c>
       <c r="C155" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>286</v>
+        <v>48</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C156" t="s">
-        <v>288</v>
+        <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>295</v>
@@ -5813,16 +5822,16 @@
     </row>
     <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>48</v>
+        <v>283</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C157" t="s">
-        <v>14</v>
+        <v>282</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>295</v>
@@ -5830,76 +5839,73 @@
     </row>
     <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>12</v>
+        <v>283</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="C158" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>48</v>
+        <v>286</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="C159" t="s">
-        <v>14</v>
+        <v>288</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>353</v>
+        <v>289</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="F159" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>48</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="C160" t="s">
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>354</v>
+        <v>291</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="C161" t="s">
-        <v>14</v>
+        <v>293</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>355</v>
+        <v>294</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>48</v>
       </c>
@@ -5910,13 +5916,16 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F162" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>48</v>
       </c>
@@ -5927,13 +5936,13 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>48</v>
       </c>
@@ -5944,13 +5953,13 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>383</v>
+        <v>355</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>48</v>
       </c>
@@ -5961,13 +5970,13 @@
         <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>357</v>
+        <v>386</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>48</v>
       </c>
@@ -5978,13 +5987,13 @@
         <v>14</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>387</v>
+        <v>356</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>48</v>
       </c>
@@ -5995,13 +6004,13 @@
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>359</v>
+        <v>383</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>48</v>
       </c>
@@ -6012,13 +6021,13 @@
         <v>14</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -6029,13 +6038,13 @@
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>48</v>
       </c>
@@ -6046,13 +6055,13 @@
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>388</v>
+        <v>359</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -6063,16 +6072,13 @@
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>311</v>
+        <v>358</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="F171" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -6083,16 +6089,13 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>312</v>
+        <v>385</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="F172" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -6103,16 +6106,13 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>314</v>
+        <v>388</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="F173" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>48</v>
       </c>
@@ -6123,16 +6123,16 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F174" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -6143,16 +6143,16 @@
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>374</v>
+        <v>312</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="F175" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -6163,16 +6163,16 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>375</v>
+        <v>314</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="F176" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>48</v>
       </c>
@@ -6183,16 +6183,16 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>376</v>
+        <v>313</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="F177" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -6203,16 +6203,16 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F178" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -6223,16 +6223,16 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F179" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>48</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>381</v>
@@ -6252,58 +6252,67 @@
         <v>349</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>48</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C181" t="s">
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>48</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C182" t="s">
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+      <c r="F182" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>48</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C183" t="s">
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -6314,13 +6323,13 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>48</v>
       </c>
@@ -6331,13 +6340,13 @@
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>333</v>
+        <v>390</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>48</v>
       </c>
@@ -6348,16 +6357,13 @@
         <v>14</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>367</v>
+        <v>391</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="F186" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>48</v>
       </c>
@@ -6368,16 +6374,13 @@
         <v>14</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>368</v>
+        <v>392</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="F187" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>48</v>
       </c>
@@ -6388,16 +6391,13 @@
         <v>14</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>369</v>
+        <v>333</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="F188" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>48</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>14</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>362</v>
@@ -6417,7 +6417,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>48</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>14</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>362</v>
@@ -6442,43 +6442,81 @@
         <v>48</v>
       </c>
       <c r="B191" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C191" t="s">
+        <v>14</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>48</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C192" t="s">
+        <v>14</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F192" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>48</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C193" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>48</v>
+      </c>
+      <c r="B194" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="C191" t="s">
-        <v>14</v>
-      </c>
-      <c r="D191" s="3" t="s">
+      <c r="C194" t="s">
+        <v>14</v>
+      </c>
+      <c r="D194" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="E191" s="3" t="s">
+      <c r="E194" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="F191" s="3" t="s">
+      <c r="F194" s="3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="210" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="211" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="212" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="213" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7040,7 +7078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: started adding more test scenarios
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FF7886-4816-48C5-B3C1-9B1C197AECD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1F31ED-2D56-487A-B643-FEB2530D065C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="412">
   <si>
     <t>Page</t>
   </si>
@@ -616,9 +616,6 @@
   </si>
   <si>
     <t>Edit Action</t>
-  </si>
-  <si>
-    <t>Edit an existing Action and verify that the "Action Type" field is disabled</t>
   </si>
   <si>
     <t>Edit Entity</t>
@@ -1397,9 +1394,6 @@
     <t>Verify that you can delete an Entity that is not used by an Action nor a Train Dialog by simply confirming that you want to delete it without other warnings poping up.</t>
   </si>
   <si>
-    <t>EntitiesActions/EditAndDeleteEntities</t>
-  </si>
-  <si>
     <t>Filter on Entity</t>
   </si>
   <si>
@@ -1425,6 +1419,18 @@
   </si>
   <si>
     <t>Start with a model with 2 Train Dialogs that could be merged - Edit Train Dialog with a single turn involving 1 Entity label and a Bot Response that renders that Entity - Add a simple text User turn - Score a simple Text Action - Delete the User turn that was just added - Save TD as is. (Bug 2191)</t>
+  </si>
+  <si>
+    <t>EntitiesActions/EntitiesEditAndDelete</t>
+  </si>
+  <si>
+    <t>Verify that you can cancel deleting an Action when propmpted to confirm the delete.</t>
+  </si>
+  <si>
+    <t>EntitiesActions/ActionEditAndDelete</t>
+  </si>
+  <si>
+    <t>Edit an Action - Verify that the Action Type field is disabled</t>
   </si>
 </sst>
 </file>
@@ -2661,8 +2667,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F216" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F216" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F217" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F217" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
@@ -3017,42 +3023,42 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -3060,28 +3066,28 @@
     </row>
     <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3092,11 +3098,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F194"/>
+  <dimension ref="A1:F195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3145,7 +3151,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,7 +3168,7 @@
         <v>107</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3179,7 +3185,7 @@
         <v>104</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3196,7 +3202,7 @@
         <v>105</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3213,7 +3219,7 @@
         <v>106</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3227,10 +3233,10 @@
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3247,7 +3253,7 @@
         <v>108</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3264,7 +3270,7 @@
         <v>109</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3278,10 +3284,10 @@
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3295,13 +3301,13 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3315,13 +3321,13 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3335,13 +3341,13 @@
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3355,13 +3361,13 @@
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3375,13 +3381,13 @@
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3389,16 +3395,16 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3406,16 +3412,16 @@
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3423,16 +3429,16 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3440,16 +3446,16 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C19" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3457,16 +3463,16 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3474,16 +3480,16 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C21" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3491,16 +3497,16 @@
         <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3508,16 +3514,16 @@
         <v>12</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3525,16 +3531,16 @@
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -3551,7 +3557,7 @@
         <v>20</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -3568,7 +3574,7 @@
         <v>188</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3585,10 +3591,10 @@
         <v>189</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>360</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3605,7 +3611,7 @@
         <v>190</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3622,7 +3628,7 @@
         <v>191</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3636,44 +3642,44 @@
         <v>28</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>193</v>
+        <v>411</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>201</v>
+        <v>405</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>406</v>
+        <v>200</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>295</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3681,67 +3687,67 @@
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C33" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>202</v>
+        <v>404</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C34" t="s">
         <v>28</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3749,19 +3755,16 @@
         <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3769,73 +3772,76 @@
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>16</v>
+        <v>221</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>23</v>
+        <v>216</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>255</v>
+        <v>294</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>295</v>
+        <v>254</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3843,16 +3849,16 @@
         <v>12</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>180</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>182</v>
+        <v>97</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3860,16 +3866,16 @@
         <v>12</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3877,50 +3883,50 @@
         <v>12</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>38</v>
+        <v>185</v>
       </c>
       <c r="C46" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>89</v>
+        <v>187</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>227</v>
+        <v>294</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3928,16 +3934,16 @@
         <v>31</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>231</v>
+        <v>89</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3951,10 +3957,10 @@
         <v>30</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3968,10 +3974,10 @@
         <v>30</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3979,16 +3985,16 @@
         <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
         <v>30</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>102</v>
+        <v>229</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4002,10 +4008,10 @@
         <v>30</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4019,44 +4025,44 @@
         <v>30</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>233</v>
+        <v>103</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>31</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
         <v>30</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>34</v>
+        <v>232</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>31</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C54" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4070,13 +4076,13 @@
         <v>30</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -4087,44 +4093,44 @@
         <v>30</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>31</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C57" t="s">
         <v>30</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>335</v>
+        <v>90</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>295</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -4138,10 +4144,10 @@
         <v>14</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -4155,10 +4161,10 @@
         <v>14</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -4172,10 +4178,10 @@
         <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -4189,10 +4195,10 @@
         <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -4206,10 +4212,10 @@
         <v>14</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -4223,10 +4229,10 @@
         <v>14</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>258</v>
+        <v>294</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -4240,10 +4246,10 @@
         <v>14</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>295</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -4251,16 +4257,16 @@
         <v>48</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C66" t="s">
         <v>14</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>53</v>
+        <v>340</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>239</v>
+        <v>294</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -4274,10 +4280,10 @@
         <v>14</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -4291,10 +4297,10 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -4308,10 +4314,10 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -4325,13 +4331,13 @@
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -4342,13 +4348,13 @@
         <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -4359,13 +4365,13 @@
         <v>14</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>240</v>
+        <v>65</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -4376,13 +4382,13 @@
         <v>14</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>204</v>
+        <v>239</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -4393,13 +4399,13 @@
         <v>14</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>409</v>
+        <v>203</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -4410,10 +4416,10 @@
         <v>14</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>342</v>
+        <v>407</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>295</v>
+        <v>406</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -4427,81 +4433,81 @@
         <v>14</v>
       </c>
       <c r="D76" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>48</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="E76" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>48</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C77" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="3" t="s">
+      <c r="E78" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>48</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C79" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="E77" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>48</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C78" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>48</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C79" t="s">
-        <v>14</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="E79" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>48</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>40</v>
+        <v>202</v>
       </c>
       <c r="C80" t="s">
         <v>14</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>41</v>
+        <v>204</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -4512,10 +4518,10 @@
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4529,10 +4535,10 @@
         <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4546,13 +4552,13 @@
         <v>14</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -4563,13 +4569,13 @@
         <v>14</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -4580,13 +4586,13 @@
         <v>14</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -4597,10 +4603,10 @@
         <v>14</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -4614,10 +4620,10 @@
         <v>14</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -4631,10 +4637,10 @@
         <v>14</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -4648,13 +4654,13 @@
         <v>14</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -4665,10 +4671,10 @@
         <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4682,16 +4688,13 @@
         <v>14</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -4702,30 +4705,33 @@
         <v>14</v>
       </c>
       <c r="D92" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>48</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E92" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>48</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C93" t="s">
-        <v>14</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="E93" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -4736,13 +4742,13 @@
         <v>14</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>253</v>
+        <v>66</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -4753,13 +4759,13 @@
         <v>14</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -4770,10 +4776,10 @@
         <v>14</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>300</v>
+        <v>233</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4787,10 +4793,10 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4804,10 +4810,10 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4821,10 +4827,10 @@
         <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4838,10 +4844,10 @@
         <v>14</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4855,10 +4861,10 @@
         <v>14</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4872,10 +4878,10 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4892,7 +4898,7 @@
         <v>304</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4906,16 +4912,13 @@
         <v>14</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -4926,30 +4929,33 @@
         <v>14</v>
       </c>
       <c r="D105" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F105" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="E105" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>48</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C106" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>71</v>
+        <v>330</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>273</v>
+        <v>294</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4963,10 +4969,10 @@
         <v>12</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4980,10 +4986,10 @@
         <v>12</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4994,13 +5000,13 @@
         <v>70</v>
       </c>
       <c r="C109" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -5014,13 +5020,13 @@
         <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -5030,8 +5036,8 @@
       <c r="C111" t="s">
         <v>14</v>
       </c>
-      <c r="D111" s="4" t="s">
-        <v>76</v>
+      <c r="D111" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>272</v>
@@ -5048,10 +5054,10 @@
         <v>14</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5065,10 +5071,10 @@
         <v>14</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5082,10 +5088,10 @@
         <v>14</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5099,10 +5105,10 @@
         <v>14</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5116,13 +5122,13 @@
         <v>14</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -5132,14 +5138,14 @@
       <c r="C117" t="s">
         <v>14</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>82</v>
+      <c r="D117" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -5150,13 +5156,13 @@
         <v>14</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -5167,33 +5173,30 @@
         <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>319</v>
+        <v>83</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>48</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>320</v>
+        <v>70</v>
       </c>
       <c r="C120" t="s">
         <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5201,19 +5204,19 @@
         <v>48</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>70</v>
+        <v>319</v>
       </c>
       <c r="C121" t="s">
         <v>14</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5227,13 +5230,13 @@
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5247,13 +5250,13 @@
         <v>14</v>
       </c>
       <c r="D123" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F123" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F123" s="3" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5267,30 +5270,33 @@
         <v>14</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>48</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C125" t="s">
         <v>14</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>86</v>
+        <v>349</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -5301,13 +5307,13 @@
         <v>14</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>261</v>
+        <v>86</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -5318,10 +5324,10 @@
         <v>14</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>85</v>
+        <v>260</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>241</v>
+        <v>294</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -5334,11 +5340,14 @@
       <c r="C128" t="s">
         <v>14</v>
       </c>
+      <c r="D128" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E128" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -5348,11 +5357,8 @@
       <c r="C129" t="s">
         <v>14</v>
       </c>
-      <c r="D129" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="E129" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5366,13 +5372,13 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>48</v>
       </c>
@@ -5383,13 +5389,13 @@
         <v>14</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>48</v>
       </c>
@@ -5400,13 +5406,13 @@
         <v>14</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>48</v>
       </c>
@@ -5417,13 +5423,13 @@
         <v>14</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>48</v>
       </c>
@@ -5434,10 +5440,10 @@
         <v>14</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>241</v>
+        <v>294</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5451,10 +5457,10 @@
         <v>14</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>279</v>
+        <v>88</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5468,10 +5474,10 @@
         <v>14</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>99</v>
+        <v>278</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5485,10 +5491,10 @@
         <v>14</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>351</v>
+        <v>99</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>295</v>
+        <v>261</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5502,30 +5508,30 @@
         <v>14</v>
       </c>
       <c r="D138" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>48</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C139" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E138" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>15</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C139" t="s">
-        <v>15</v>
-      </c>
-      <c r="D139" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="E139" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>15</v>
       </c>
@@ -5536,13 +5542,13 @@
         <v>15</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>15</v>
       </c>
@@ -5553,10 +5559,10 @@
         <v>15</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>265</v>
+        <v>91</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5570,10 +5576,10 @@
         <v>15</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5587,13 +5593,13 @@
         <v>15</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>15</v>
       </c>
@@ -5604,10 +5610,10 @@
         <v>15</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>327</v>
+        <v>263</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -5621,47 +5627,47 @@
         <v>15</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F145" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>15</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C146" t="s">
         <v>15</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>278</v>
+        <v>327</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>266</v>
+        <v>84</v>
       </c>
       <c r="C147" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>24</v>
+        <v>277</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>269</v>
+        <v>294</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -5669,16 +5675,16 @@
         <v>3</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
       </c>
       <c r="D148" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E148" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -5686,33 +5692,33 @@
         <v>3</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C149" t="s">
         <v>8</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>67</v>
+        <v>267</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>3</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C150" t="s">
         <v>8</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>295</v>
+        <v>237</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -5720,16 +5726,16 @@
         <v>3</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>4</v>
+        <v>266</v>
       </c>
       <c r="C151" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -5740,13 +5746,13 @@
         <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -5754,16 +5760,16 @@
         <v>3</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C153" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -5774,152 +5780,149 @@
         <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>3</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="C155" t="s">
-        <v>298</v>
+        <v>11</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>299</v>
+        <v>26</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>280</v>
+        <v>69</v>
       </c>
       <c r="C156" t="s">
-        <v>14</v>
+        <v>297</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>283</v>
+        <v>48</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C157" t="s">
-        <v>282</v>
+        <v>14</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>282</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C158" t="s">
+        <v>281</v>
+      </c>
+      <c r="D158" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B158" s="3" t="s">
+      <c r="E158" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>282</v>
       </c>
-      <c r="C158" t="s">
-        <v>282</v>
-      </c>
-      <c r="D158" s="3" t="s">
+      <c r="B159" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C159" t="s">
+        <v>281</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>285</v>
       </c>
-      <c r="E158" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="B160" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B159" s="3" t="s">
+      <c r="C160" t="s">
         <v>287</v>
       </c>
-      <c r="C159" t="s">
+      <c r="D160" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D159" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>48</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C160" t="s">
-        <v>14</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>291</v>
-      </c>
       <c r="E160" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C161" t="s">
-        <v>293</v>
+        <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E161" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="C162" t="s">
-        <v>14</v>
+        <v>292</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>353</v>
+        <v>293</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="F162" s="3" t="s">
-        <v>352</v>
+        <v>294</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5927,16 +5930,19 @@
         <v>48</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C163" t="s">
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5944,16 +5950,16 @@
         <v>48</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C164" t="s">
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5961,16 +5967,16 @@
         <v>48</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C165" t="s">
         <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>386</v>
+        <v>354</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5978,16 +5984,16 @@
         <v>48</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C166" t="s">
         <v>14</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>356</v>
+        <v>385</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5995,16 +6001,16 @@
         <v>48</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C167" t="s">
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>383</v>
+        <v>355</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6012,16 +6018,16 @@
         <v>48</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C168" t="s">
         <v>14</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6029,16 +6035,16 @@
         <v>48</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C169" t="s">
         <v>14</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>387</v>
+        <v>356</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6046,16 +6052,16 @@
         <v>48</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C170" t="s">
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>359</v>
+        <v>386</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6063,7 +6069,7 @@
         <v>48</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C171" t="s">
         <v>14</v>
@@ -6072,7 +6078,7 @@
         <v>358</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6080,53 +6086,50 @@
         <v>48</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C172" t="s">
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>385</v>
+        <v>357</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>48</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C173" t="s">
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>48</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C174" t="s">
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>311</v>
+        <v>387</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="F174" s="3" t="s">
-        <v>349</v>
+        <v>381</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6134,19 +6137,19 @@
         <v>48</v>
       </c>
       <c r="B175" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C175" t="s">
+        <v>14</v>
+      </c>
+      <c r="D175" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="C175" t="s">
-        <v>14</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>312</v>
-      </c>
       <c r="E175" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6154,19 +6157,19 @@
         <v>48</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C176" t="s">
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6174,7 +6177,7 @@
         <v>48</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C177" t="s">
         <v>14</v>
@@ -6183,10 +6186,10 @@
         <v>313</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6194,19 +6197,19 @@
         <v>48</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C178" t="s">
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>374</v>
+        <v>312</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6214,39 +6217,39 @@
         <v>48</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C179" t="s">
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>48</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C180" t="s">
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="181" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6254,19 +6257,19 @@
         <v>48</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C181" t="s">
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6274,19 +6277,19 @@
         <v>48</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C182" t="s">
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6294,22 +6297,22 @@
         <v>48</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C183" t="s">
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -6320,10 +6323,13 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>393</v>
+        <v>380</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6331,16 +6337,16 @@
         <v>48</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C185" t="s">
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6348,16 +6354,16 @@
         <v>48</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C186" t="s">
         <v>14</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6365,16 +6371,16 @@
         <v>48</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C187" t="s">
         <v>14</v>
       </c>
       <c r="D187" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E187" s="3" t="s">
         <v>392</v>
-      </c>
-      <c r="E187" s="3" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6382,36 +6388,33 @@
         <v>48</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C188" t="s">
         <v>14</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>333</v>
+        <v>391</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>48</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C189" t="s">
         <v>14</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>367</v>
+        <v>332</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="F189" s="3" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6419,39 +6422,39 @@
         <v>48</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C190" t="s">
         <v>14</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>48</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C191" t="s">
         <v>14</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F191" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6459,19 +6462,19 @@
         <v>48</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C192" t="s">
         <v>14</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6479,19 +6482,19 @@
         <v>48</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C193" t="s">
         <v>14</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E193" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6499,19 +6502,39 @@
         <v>48</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="C194" t="s">
         <v>14</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>347</v>
+        <v>370</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>295</v>
+        <v>361</v>
       </c>
       <c r="F194" s="3" t="s">
         <v>348</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>48</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C195" t="s">
+        <v>14</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F195" s="3" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -6567,13 +6590,13 @@
         <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6611,7 +6634,7 @@
         <v>112</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>113</v>
@@ -6667,7 +6690,7 @@
         <v>114</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
         <v>121</v>
@@ -6731,7 +6754,7 @@
         <v>130</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
         <v>121</v>
@@ -6770,7 +6793,7 @@
         <v>84</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -6854,7 +6877,7 @@
         <v>128</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -6918,7 +6941,7 @@
         <v>48</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C31" t="s">
         <v>121</v>
@@ -6949,7 +6972,7 @@
         <v>128</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -7089,16 +7112,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1" t="s">
         <v>363</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>364</v>
-      </c>
-      <c r="D1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: off to a good start
</commit_message>
<xml_diff>
--- a/cypress/TestGrid.xlsx
+++ b/cypress/TestGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1912C0-7DC7-4843-8F1B-487552AFBC31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5C1668-9AA4-4818-9073-999170F6D2EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="413">
   <si>
     <t>Page</t>
   </si>
@@ -2683,7 +2683,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F218" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F218" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+  <autoFilter ref="A1:F218" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Edit Log Dialog, Save"/>
+        <filter val="Log Dialog"/>
+        <filter val="New Log Dialog, Save"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
@@ -3113,11 +3121,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F196"/>
+  <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,7 +3160,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="60.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3169,7 +3177,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3186,7 +3194,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3203,7 +3211,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3220,7 +3228,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3237,7 +3245,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3254,7 +3262,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3271,7 +3279,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3288,7 +3296,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3305,7 +3313,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3325,7 +3333,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3345,7 +3353,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3365,7 +3373,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3385,7 +3393,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3405,7 +3413,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3422,7 +3430,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3439,7 +3447,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3456,7 +3464,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3473,7 +3481,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3490,7 +3498,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3507,7 +3515,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3524,7 +3532,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3541,7 +3549,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3558,7 +3566,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="75.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3575,7 +3583,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="75.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -3592,7 +3600,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3612,7 +3620,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -3626,10 +3634,13 @@
         <v>190</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -3646,7 +3657,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3663,7 +3674,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -3680,7 +3691,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -3697,7 +3708,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -3714,7 +3725,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -3731,7 +3742,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -3748,7 +3759,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -3765,7 +3776,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="90.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -3782,7 +3793,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="30.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -3799,7 +3810,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -3836,7 +3847,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -3856,7 +3867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -3876,7 +3887,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -3893,7 +3904,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -3910,7 +3921,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -3927,7 +3938,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -3944,7 +3955,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -3961,7 +3972,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -3978,7 +3989,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -3995,7 +4006,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -4012,7 +4023,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -4029,7 +4040,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -4046,7 +4057,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -4063,7 +4074,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -4080,7 +4091,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -4097,7 +4108,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -4114,7 +4125,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -4131,7 +4142,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>31</v>
       </c>
@@ -4148,7 +4159,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -4165,7 +4176,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -4182,7 +4193,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -4199,7 +4210,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -4216,7 +4227,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -4233,7 +4244,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -4250,7 +4261,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -4267,7 +4278,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -4284,7 +4295,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -4301,7 +4312,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -4318,7 +4329,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -4335,7 +4346,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -4352,7 +4363,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -4369,7 +4380,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -4386,7 +4397,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -4403,7 +4414,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -4420,7 +4431,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -4437,7 +4448,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -4454,7 +4465,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -4471,7 +4482,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -4488,7 +4499,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -4505,7 +4516,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -4522,7 +4533,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -4539,7 +4550,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -4556,7 +4567,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -4573,7 +4584,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -4590,7 +4601,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -4607,7 +4618,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -4624,7 +4635,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -4641,7 +4652,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -4658,7 +4669,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -4675,7 +4686,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -4692,7 +4703,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -4709,7 +4720,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -4726,7 +4737,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -4746,7 +4757,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -4763,7 +4774,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -4780,7 +4791,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -4797,7 +4808,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -4814,7 +4825,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>48</v>
       </c>
@@ -4831,7 +4842,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -4848,7 +4859,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -4865,7 +4876,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -4882,7 +4893,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -4899,7 +4910,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -4916,7 +4927,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -4933,7 +4944,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -4950,7 +4961,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -4970,7 +4981,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -4990,7 +5001,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -5007,7 +5018,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -5024,7 +5035,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="45" x14ac